<commit_message>
Added 45nm test case data and references
</commit_message>
<xml_diff>
--- a/data/processor_wla_validation.xlsx
+++ b/data/processor_wla_validation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Merom 65nm Data" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="22nm - Ivy Bridge EP10" sheetId="4" r:id="rId4"/>
     <sheet name="32nm Sandy Bridge (standard)" sheetId="6" r:id="rId5"/>
     <sheet name="22nm Ivy Bridge (standard)" sheetId="5" r:id="rId6"/>
+    <sheet name="45nm Penryn" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="43">
   <si>
     <t>w (px)</t>
   </si>
@@ -130,6 +131,24 @@
   </si>
   <si>
     <t>Pitch</t>
+  </si>
+  <si>
+    <t>Thickness (nm)</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>width_frac</t>
+  </si>
+  <si>
+    <t>TDP (W)</t>
+  </si>
+  <si>
+    <t>FSB (MT/s)</t>
+  </si>
+  <si>
+    <t>Vdd (V)</t>
   </si>
 </sst>
 </file>
@@ -173,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -185,6 +204,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -412,11 +434,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="50016256"/>
-        <c:axId val="50018176"/>
+        <c:axId val="53681152"/>
+        <c:axId val="53683328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="50016256"/>
+        <c:axId val="53681152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -440,19 +462,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50018176"/>
+        <c:crossAx val="53683328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50018176"/>
+        <c:axId val="53683328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -482,14 +503,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50016256"/>
+        <c:crossAx val="53681152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1187,7 +1207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
@@ -2817,7 +2837,7 @@
   <dimension ref="A2:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="A2" sqref="A2:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3041,4 +3061,370 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5">
+        <v>385</v>
+      </c>
+      <c r="C2" s="5">
+        <v>237</v>
+      </c>
+      <c r="D2" s="5">
+        <f>B2*C2</f>
+        <v>91245</v>
+      </c>
+      <c r="E2" s="5">
+        <f>D2*E4/D4</f>
+        <v>21.676765097690943</v>
+      </c>
+      <c r="F2" s="6">
+        <f>F4*E2/E4</f>
+        <v>83060501.776198953</v>
+      </c>
+      <c r="G2" s="6">
+        <f>E2/F2*1000000</f>
+        <v>0.26097560975609752</v>
+      </c>
+      <c r="H2" s="5">
+        <f>SQRT(G2)</f>
+        <v>0.51085771967945981</v>
+      </c>
+      <c r="I2" s="5">
+        <f>2*H2</f>
+        <v>1.0217154393589196</v>
+      </c>
+      <c r="K2" s="7">
+        <v>35</v>
+      </c>
+      <c r="L2">
+        <v>1066</v>
+      </c>
+      <c r="M2">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7">
+        <v>800</v>
+      </c>
+      <c r="C4" s="7">
+        <v>563</v>
+      </c>
+      <c r="D4" s="7">
+        <f>B4*C4</f>
+        <v>450400</v>
+      </c>
+      <c r="E4" s="5">
+        <v>107</v>
+      </c>
+      <c r="F4" s="6">
+        <v>410000000</v>
+      </c>
+      <c r="G4" s="6">
+        <f>E4/F4*1000000</f>
+        <v>0.26097560975609757</v>
+      </c>
+      <c r="H4" s="5">
+        <f>SQRT(G4)</f>
+        <v>0.51085771967945981</v>
+      </c>
+      <c r="I4" s="5">
+        <f>2*H4</f>
+        <v>1.0217154393589196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>160</v>
+      </c>
+      <c r="C8" s="5">
+        <v>144</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E8">
+        <f>C8/D8</f>
+        <v>80</v>
+      </c>
+      <c r="F8">
+        <f>E8/B8</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>160</v>
+      </c>
+      <c r="C9" s="5">
+        <v>144</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ref="E9:E16" si="0">C9/D9</f>
+        <v>80</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9:F16" si="1">E9/B9</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>160</v>
+      </c>
+      <c r="C10" s="5">
+        <v>144</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>250</v>
+      </c>
+      <c r="C11" s="5">
+        <v>216</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>280</v>
+      </c>
+      <c r="C12" s="5">
+        <v>252</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>360</v>
+      </c>
+      <c r="C13" s="5">
+        <v>324</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>560</v>
+      </c>
+      <c r="C14" s="5">
+        <v>504</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>810</v>
+      </c>
+      <c r="C15" s="5">
+        <v>720</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0.49382716049382713</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>30500</v>
+      </c>
+      <c r="C16" s="5">
+        <v>7000</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>17500</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0.57377049180327866</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding test_codesign_system_22nm_match and cpu_wiring_comparison
test_codesign_system_22nm_match file has all the conditions which mach
the 22nm single core ivy bridge test case the best

cpu_wiring_comparison compares the various fits to real data
</commit_message>
<xml_diff>
--- a/data/processor_wla_validation.xlsx
+++ b/data/processor_wla_validation.xlsx
@@ -4,23 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Merom 65nm Data" sheetId="1" r:id="rId1"/>
     <sheet name="Merom2" sheetId="2" r:id="rId2"/>
     <sheet name="Sandy Bridge EP-4 32nm Data" sheetId="3" r:id="rId3"/>
     <sheet name="22nm - Ivy Bridge EP10" sheetId="4" r:id="rId4"/>
-    <sheet name="32nm Sandy Bridge (standard)" sheetId="6" r:id="rId5"/>
-    <sheet name="22nm Ivy Bridge (standard)" sheetId="5" r:id="rId6"/>
-    <sheet name="45nm Penryn" sheetId="7" r:id="rId7"/>
+    <sheet name="45nm Penryn" sheetId="7" r:id="rId5"/>
+    <sheet name="32nm Sandy Bridge (standard)" sheetId="6" r:id="rId6"/>
+    <sheet name="22nm Ivy Bridge (standard)" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="44">
   <si>
     <t>w (px)</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>Vdd (V)</t>
+  </si>
+  <si>
+    <t>fmax (GHz)</t>
   </si>
 </sst>
 </file>
@@ -2450,6 +2453,378 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5">
+        <v>385</v>
+      </c>
+      <c r="C2" s="5">
+        <v>237</v>
+      </c>
+      <c r="D2" s="5">
+        <f>B2*C2</f>
+        <v>91245</v>
+      </c>
+      <c r="E2" s="5">
+        <f>D2*E4/D4</f>
+        <v>21.676765097690943</v>
+      </c>
+      <c r="F2" s="6">
+        <f>F4*E2/E4</f>
+        <v>83060501.776198953</v>
+      </c>
+      <c r="G2" s="6">
+        <f>E2/F2*1000000</f>
+        <v>0.26097560975609752</v>
+      </c>
+      <c r="H2" s="5">
+        <f>SQRT(G2)</f>
+        <v>0.51085771967945981</v>
+      </c>
+      <c r="I2" s="5">
+        <f>2*H2</f>
+        <v>1.0217154393589196</v>
+      </c>
+      <c r="K2" s="7">
+        <v>35</v>
+      </c>
+      <c r="L2">
+        <v>1066</v>
+      </c>
+      <c r="M2">
+        <v>1.2</v>
+      </c>
+      <c r="N2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7">
+        <v>800</v>
+      </c>
+      <c r="C4" s="7">
+        <v>563</v>
+      </c>
+      <c r="D4" s="7">
+        <f>B4*C4</f>
+        <v>450400</v>
+      </c>
+      <c r="E4" s="5">
+        <v>107</v>
+      </c>
+      <c r="F4" s="6">
+        <v>410000000</v>
+      </c>
+      <c r="G4" s="6">
+        <f>E4/F4*1000000</f>
+        <v>0.26097560975609757</v>
+      </c>
+      <c r="H4" s="5">
+        <f>SQRT(G4)</f>
+        <v>0.51085771967945981</v>
+      </c>
+      <c r="I4" s="5">
+        <f>2*H4</f>
+        <v>1.0217154393589196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>160</v>
+      </c>
+      <c r="C8" s="5">
+        <v>144</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E8">
+        <f>C8/D8</f>
+        <v>80</v>
+      </c>
+      <c r="F8">
+        <f>E8/B8</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>160</v>
+      </c>
+      <c r="C9" s="5">
+        <v>144</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ref="E9:E16" si="0">C9/D9</f>
+        <v>80</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9:F16" si="1">E9/B9</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>160</v>
+      </c>
+      <c r="C10" s="5">
+        <v>144</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>250</v>
+      </c>
+      <c r="C11" s="5">
+        <v>216</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>280</v>
+      </c>
+      <c r="C12" s="5">
+        <v>252</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>360</v>
+      </c>
+      <c r="C13" s="5">
+        <v>324</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>560</v>
+      </c>
+      <c r="C14" s="5">
+        <v>504</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>810</v>
+      </c>
+      <c r="C15" s="5">
+        <v>720</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0.49382716049382713</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>30500</v>
+      </c>
+      <c r="C16" s="5">
+        <v>7000</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>17500</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0.57377049180327866</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2832,7 +3207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I17"/>
   <sheetViews>
@@ -3061,370 +3436,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5">
-        <v>385</v>
-      </c>
-      <c r="C2" s="5">
-        <v>237</v>
-      </c>
-      <c r="D2" s="5">
-        <f>B2*C2</f>
-        <v>91245</v>
-      </c>
-      <c r="E2" s="5">
-        <f>D2*E4/D4</f>
-        <v>21.676765097690943</v>
-      </c>
-      <c r="F2" s="6">
-        <f>F4*E2/E4</f>
-        <v>83060501.776198953</v>
-      </c>
-      <c r="G2" s="6">
-        <f>E2/F2*1000000</f>
-        <v>0.26097560975609752</v>
-      </c>
-      <c r="H2" s="5">
-        <f>SQRT(G2)</f>
-        <v>0.51085771967945981</v>
-      </c>
-      <c r="I2" s="5">
-        <f>2*H2</f>
-        <v>1.0217154393589196</v>
-      </c>
-      <c r="K2" s="7">
-        <v>35</v>
-      </c>
-      <c r="L2">
-        <v>1066</v>
-      </c>
-      <c r="M2">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="7">
-        <v>800</v>
-      </c>
-      <c r="C4" s="7">
-        <v>563</v>
-      </c>
-      <c r="D4" s="7">
-        <f>B4*C4</f>
-        <v>450400</v>
-      </c>
-      <c r="E4" s="5">
-        <v>107</v>
-      </c>
-      <c r="F4" s="6">
-        <v>410000000</v>
-      </c>
-      <c r="G4" s="6">
-        <f>E4/F4*1000000</f>
-        <v>0.26097560975609757</v>
-      </c>
-      <c r="H4" s="5">
-        <f>SQRT(G4)</f>
-        <v>0.51085771967945981</v>
-      </c>
-      <c r="I4" s="5">
-        <f>2*H4</f>
-        <v>1.0217154393589196</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>160</v>
-      </c>
-      <c r="C8" s="5">
-        <v>144</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E8">
-        <f>C8/D8</f>
-        <v>80</v>
-      </c>
-      <c r="F8">
-        <f>E8/B8</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>160</v>
-      </c>
-      <c r="C9" s="5">
-        <v>144</v>
-      </c>
-      <c r="D9" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E9">
-        <f t="shared" ref="E9:E16" si="0">C9/D9</f>
-        <v>80</v>
-      </c>
-      <c r="F9">
-        <f t="shared" ref="F9:F16" si="1">E9/B9</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>160</v>
-      </c>
-      <c r="C10" s="5">
-        <v>144</v>
-      </c>
-      <c r="D10" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>4</v>
-      </c>
-      <c r="B11">
-        <v>250</v>
-      </c>
-      <c r="C11" s="5">
-        <v>216</v>
-      </c>
-      <c r="D11" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="1"/>
-        <v>0.48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>5</v>
-      </c>
-      <c r="B12">
-        <v>280</v>
-      </c>
-      <c r="C12" s="5">
-        <v>252</v>
-      </c>
-      <c r="D12" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>140</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>6</v>
-      </c>
-      <c r="B13">
-        <v>360</v>
-      </c>
-      <c r="C13" s="5">
-        <v>324</v>
-      </c>
-      <c r="D13" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>180</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>7</v>
-      </c>
-      <c r="B14">
-        <v>560</v>
-      </c>
-      <c r="C14" s="5">
-        <v>504</v>
-      </c>
-      <c r="D14" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>280</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>8</v>
-      </c>
-      <c r="B15">
-        <v>810</v>
-      </c>
-      <c r="C15" s="5">
-        <v>720</v>
-      </c>
-      <c r="D15" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="1"/>
-        <v>0.49382716049382713</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>9</v>
-      </c>
-      <c r="B16">
-        <v>30500</v>
-      </c>
-      <c r="C16" s="5">
-        <v>7000</v>
-      </c>
-      <c r="D16" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>17500</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="1"/>
-        <v>0.57377049180327866</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
more power and wiring comparison updates
</commit_message>
<xml_diff>
--- a/data/processor_wla_validation.xlsx
+++ b/data/processor_wla_validation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="15120" windowHeight="7995" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Merom 65nm Data" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="45nm Penryn" sheetId="7" r:id="rId5"/>
     <sheet name="32nm Sandy Bridge (standard)" sheetId="6" r:id="rId6"/>
     <sheet name="22nm Ivy Bridge (standard)" sheetId="5" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="46">
   <si>
     <t>w (px)</t>
   </si>
@@ -152,6 +153,12 @@
   </si>
   <si>
     <t>fmax (GHz)</t>
+  </si>
+  <si>
+    <t>Node</t>
+  </si>
+  <si>
+    <t>Core Power</t>
   </si>
 </sst>
 </file>
@@ -437,11 +444,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="53681152"/>
-        <c:axId val="53683328"/>
+        <c:axId val="86349312"/>
+        <c:axId val="66159744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53681152"/>
+        <c:axId val="86349312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -471,12 +478,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53683328"/>
+        <c:crossAx val="66159744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53683328"/>
+        <c:axId val="66159744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -512,7 +519,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53681152"/>
+        <c:crossAx val="86349312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2455,7 +2462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
@@ -2827,7 +2834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -3212,7 +3219,7 @@
   <dimension ref="A2:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I17"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3436,4 +3443,54 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>65</v>
+      </c>
+      <c r="B2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added best fit scripts for merom and penryn test cases
</commit_message>
<xml_diff>
--- a/data/processor_wla_validation.xlsx
+++ b/data/processor_wla_validation.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="15120" windowHeight="7995" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="15120" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Merom 65nm Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Merom2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sandy Bridge EP-4 32nm Data" sheetId="3" r:id="rId3"/>
-    <sheet name="22nm - Ivy Bridge EP10" sheetId="4" r:id="rId4"/>
-    <sheet name="45nm Penryn" sheetId="7" r:id="rId5"/>
-    <sheet name="32nm Sandy Bridge (standard)" sheetId="6" r:id="rId6"/>
+    <sheet name="65nm Merom" sheetId="2" r:id="rId2"/>
+    <sheet name="45nm Penryn" sheetId="7" r:id="rId3"/>
+    <sheet name="Sandy Bridge EP-4 32nm Data" sheetId="3" r:id="rId4"/>
+    <sheet name="32nm Sandy Bridge (standard)" sheetId="6" r:id="rId5"/>
+    <sheet name="22nm - Ivy Bridge EP10" sheetId="4" r:id="rId6"/>
     <sheet name="22nm Ivy Bridge (standard)" sheetId="5" r:id="rId7"/>
     <sheet name="Sheet1" sheetId="8" r:id="rId8"/>
   </sheets>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="46">
   <si>
     <t>w (px)</t>
   </si>
@@ -444,11 +444,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="86349312"/>
-        <c:axId val="66159744"/>
+        <c:axId val="136654208"/>
+        <c:axId val="136660480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86349312"/>
+        <c:axId val="136654208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -472,18 +472,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66159744"/>
+        <c:crossAx val="136660480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66159744"/>
+        <c:axId val="136660480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -513,13 +514,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86349312"/>
+        <c:crossAx val="136654208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1215,10 +1217,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P21"/>
+  <dimension ref="A2:P33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1681,6 +1683,207 @@
         <v>0.52984767393989296</v>
       </c>
     </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>210</v>
+      </c>
+      <c r="C25" s="5">
+        <v>170</v>
+      </c>
+      <c r="D25" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="E25">
+        <f>C25/D25</f>
+        <v>106.25</v>
+      </c>
+      <c r="F25">
+        <f>E25/B25</f>
+        <v>0.50595238095238093</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>210</v>
+      </c>
+      <c r="C26" s="5">
+        <v>190</v>
+      </c>
+      <c r="D26" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ref="E26:E33" si="3">C26/D26</f>
+        <v>105.55555555555556</v>
+      </c>
+      <c r="F26">
+        <f t="shared" ref="F26:F33" si="4">E26/B26</f>
+        <v>0.50264550264550267</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>220</v>
+      </c>
+      <c r="C27" s="5">
+        <v>200</v>
+      </c>
+      <c r="D27" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="3"/>
+        <v>111.11111111111111</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="4"/>
+        <v>0.50505050505050508</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>280</v>
+      </c>
+      <c r="C28" s="5">
+        <v>250</v>
+      </c>
+      <c r="D28" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="3"/>
+        <v>138.88888888888889</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="4"/>
+        <v>0.49603174603174605</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>330</v>
+      </c>
+      <c r="C29" s="5">
+        <v>300</v>
+      </c>
+      <c r="D29" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="3"/>
+        <v>166.66666666666666</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="4"/>
+        <v>0.50505050505050497</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>480</v>
+      </c>
+      <c r="C30" s="5">
+        <v>430</v>
+      </c>
+      <c r="D30" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="3"/>
+        <v>238.88888888888889</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="4"/>
+        <v>0.49768518518518517</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <v>720</v>
+      </c>
+      <c r="C31" s="5">
+        <v>650</v>
+      </c>
+      <c r="D31" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="3"/>
+        <v>361.11111111111109</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="4"/>
+        <v>0.50154320987654322</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <v>1080</v>
+      </c>
+      <c r="C32" s="5">
+        <v>975</v>
+      </c>
+      <c r="D32" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="3"/>
+        <v>541.66666666666663</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="4"/>
+        <v>0.50154320987654322</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1688,6 +1891,378 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5">
+        <v>385</v>
+      </c>
+      <c r="C2" s="5">
+        <v>237</v>
+      </c>
+      <c r="D2" s="5">
+        <f>B2*C2</f>
+        <v>91245</v>
+      </c>
+      <c r="E2" s="5">
+        <f>D2*E4/D4</f>
+        <v>21.676765097690943</v>
+      </c>
+      <c r="F2" s="6">
+        <f>F4*E2/E4</f>
+        <v>83060501.776198953</v>
+      </c>
+      <c r="G2" s="6">
+        <f>E2/F2*1000000</f>
+        <v>0.26097560975609752</v>
+      </c>
+      <c r="H2" s="5">
+        <f>SQRT(G2)</f>
+        <v>0.51085771967945981</v>
+      </c>
+      <c r="I2" s="5">
+        <f>2*H2</f>
+        <v>1.0217154393589196</v>
+      </c>
+      <c r="K2" s="7">
+        <v>35</v>
+      </c>
+      <c r="L2">
+        <v>1066</v>
+      </c>
+      <c r="M2">
+        <v>1.2</v>
+      </c>
+      <c r="N2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7">
+        <v>800</v>
+      </c>
+      <c r="C4" s="7">
+        <v>563</v>
+      </c>
+      <c r="D4" s="7">
+        <f>B4*C4</f>
+        <v>450400</v>
+      </c>
+      <c r="E4" s="5">
+        <v>107</v>
+      </c>
+      <c r="F4" s="6">
+        <v>410000000</v>
+      </c>
+      <c r="G4" s="6">
+        <f>E4/F4*1000000</f>
+        <v>0.26097560975609757</v>
+      </c>
+      <c r="H4" s="5">
+        <f>SQRT(G4)</f>
+        <v>0.51085771967945981</v>
+      </c>
+      <c r="I4" s="5">
+        <f>2*H4</f>
+        <v>1.0217154393589196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>160</v>
+      </c>
+      <c r="C8" s="5">
+        <v>144</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E8">
+        <f>C8/D8</f>
+        <v>80</v>
+      </c>
+      <c r="F8">
+        <f>E8/B8</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>160</v>
+      </c>
+      <c r="C9" s="5">
+        <v>144</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ref="E9:E16" si="0">C9/D9</f>
+        <v>80</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9:F16" si="1">E9/B9</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>160</v>
+      </c>
+      <c r="C10" s="5">
+        <v>144</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>250</v>
+      </c>
+      <c r="C11" s="5">
+        <v>216</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>280</v>
+      </c>
+      <c r="C12" s="5">
+        <v>252</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>360</v>
+      </c>
+      <c r="C13" s="5">
+        <v>324</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>560</v>
+      </c>
+      <c r="C14" s="5">
+        <v>504</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>810</v>
+      </c>
+      <c r="C15" s="5">
+        <v>720</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0.49382716049382713</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>30500</v>
+      </c>
+      <c r="C16" s="5">
+        <v>7000</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>17500</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0.57377049180327866</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O24"/>
   <sheetViews>
@@ -2228,7 +2803,391 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>169</v>
+      </c>
+      <c r="C2">
+        <v>287</v>
+      </c>
+      <c r="D2">
+        <f>B2*C2</f>
+        <v>48503</v>
+      </c>
+      <c r="E2">
+        <f>D2/$D$4*$E$4</f>
+        <v>18.546941608010311</v>
+      </c>
+      <c r="F2" s="2">
+        <f>E2/$E$4*$F$4</f>
+        <v>85436143.055417866</v>
+      </c>
+      <c r="G2" s="2">
+        <f>E2/F2*1000000</f>
+        <v>0.21708542713567841</v>
+      </c>
+      <c r="H2">
+        <f>SQRT(G2)</f>
+        <v>0.46592427188941166</v>
+      </c>
+      <c r="I2">
+        <f>2*H2</f>
+        <v>0.93184854377882331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>228</v>
+      </c>
+      <c r="C3">
+        <v>325</v>
+      </c>
+      <c r="D3">
+        <f>B3*C3</f>
+        <v>74100</v>
+      </c>
+      <c r="F3">
+        <f>B8</f>
+        <v>1006632960</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G4" si="0">E3/F3*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H4" si="1">SQRT(G3)</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I4" si="2">2*H3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1078</v>
+      </c>
+      <c r="C4" s="1">
+        <v>524</v>
+      </c>
+      <c r="D4">
+        <f>B4*C4</f>
+        <v>564872</v>
+      </c>
+      <c r="E4">
+        <v>216</v>
+      </c>
+      <c r="F4" s="2">
+        <v>995000000</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
+        <v>0.21708542713567841</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>0.46592427188941166</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>0.93184854377882331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2270000000</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <f>E7*POWER(2,20)*8</f>
+        <v>167772160</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <f>G7*F7</f>
+        <v>1006632960</v>
+      </c>
+      <c r="I7">
+        <f>E3/H7*1000000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <f>H7</f>
+        <v>1006632960</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2">
+        <f>B7-B8</f>
+        <v>1263367040</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="D14">
+        <v>0.1125</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1</v>
+      </c>
+      <c r="G14" s="5">
+        <v>112.5</v>
+      </c>
+      <c r="H14">
+        <v>112.5</v>
+      </c>
+      <c r="I14">
+        <v>112.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="3">
+        <v>0.1993</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="5">
+        <v>2</v>
+      </c>
+      <c r="G15" s="5">
+        <v>112.5</v>
+      </c>
+      <c r="H15">
+        <v>112.5</v>
+      </c>
+      <c r="I15">
+        <v>112.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="D16">
+        <v>0.42</v>
+      </c>
+      <c r="F16" s="5">
+        <v>3</v>
+      </c>
+      <c r="G16" s="5">
+        <v>112.5</v>
+      </c>
+      <c r="H16">
+        <v>199.3</v>
+      </c>
+      <c r="I16">
+        <v>131.49469999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>0.71819999999999995</v>
+      </c>
+      <c r="F17" s="5">
+        <v>4</v>
+      </c>
+      <c r="G17" s="5">
+        <v>168.8</v>
+      </c>
+      <c r="H17">
+        <v>199.3</v>
+      </c>
+      <c r="I17">
+        <v>247.32849999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F18" s="5">
+        <v>5</v>
+      </c>
+      <c r="G18" s="5">
+        <v>225</v>
+      </c>
+      <c r="H18">
+        <v>420</v>
+      </c>
+      <c r="I18">
+        <v>374.14409999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F19" s="5">
+        <v>6</v>
+      </c>
+      <c r="G19" s="5">
+        <v>337.6</v>
+      </c>
+      <c r="H19">
+        <v>420</v>
+      </c>
+      <c r="I19">
+        <v>540.39850000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F20" s="5">
+        <v>7</v>
+      </c>
+      <c r="G20" s="5">
+        <v>450.1</v>
+      </c>
+      <c r="H20">
+        <v>718.2</v>
+      </c>
+      <c r="I20">
+        <v>718.20759999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F21" s="5">
+        <v>8</v>
+      </c>
+      <c r="G21" s="5">
+        <v>566.5</v>
+      </c>
+      <c r="H21">
+        <v>718.2</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F22" s="5">
+        <v>9</v>
+      </c>
+      <c r="G22" s="5">
+        <v>19400</v>
+      </c>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F23" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="6">
+        <v>145900</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I18"/>
   <sheetViews>
@@ -2455,762 +3414,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5">
-        <v>385</v>
-      </c>
-      <c r="C2" s="5">
-        <v>237</v>
-      </c>
-      <c r="D2" s="5">
-        <f>B2*C2</f>
-        <v>91245</v>
-      </c>
-      <c r="E2" s="5">
-        <f>D2*E4/D4</f>
-        <v>21.676765097690943</v>
-      </c>
-      <c r="F2" s="6">
-        <f>F4*E2/E4</f>
-        <v>83060501.776198953</v>
-      </c>
-      <c r="G2" s="6">
-        <f>E2/F2*1000000</f>
-        <v>0.26097560975609752</v>
-      </c>
-      <c r="H2" s="5">
-        <f>SQRT(G2)</f>
-        <v>0.51085771967945981</v>
-      </c>
-      <c r="I2" s="5">
-        <f>2*H2</f>
-        <v>1.0217154393589196</v>
-      </c>
-      <c r="K2" s="7">
-        <v>35</v>
-      </c>
-      <c r="L2">
-        <v>1066</v>
-      </c>
-      <c r="M2">
-        <v>1.2</v>
-      </c>
-      <c r="N2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="7">
-        <v>800</v>
-      </c>
-      <c r="C4" s="7">
-        <v>563</v>
-      </c>
-      <c r="D4" s="7">
-        <f>B4*C4</f>
-        <v>450400</v>
-      </c>
-      <c r="E4" s="5">
-        <v>107</v>
-      </c>
-      <c r="F4" s="6">
-        <v>410000000</v>
-      </c>
-      <c r="G4" s="6">
-        <f>E4/F4*1000000</f>
-        <v>0.26097560975609757</v>
-      </c>
-      <c r="H4" s="5">
-        <f>SQRT(G4)</f>
-        <v>0.51085771967945981</v>
-      </c>
-      <c r="I4" s="5">
-        <f>2*H4</f>
-        <v>1.0217154393589196</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>160</v>
-      </c>
-      <c r="C8" s="5">
-        <v>144</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E8">
-        <f>C8/D8</f>
-        <v>80</v>
-      </c>
-      <c r="F8">
-        <f>E8/B8</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>160</v>
-      </c>
-      <c r="C9" s="5">
-        <v>144</v>
-      </c>
-      <c r="D9" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E9">
-        <f t="shared" ref="E9:E16" si="0">C9/D9</f>
-        <v>80</v>
-      </c>
-      <c r="F9">
-        <f t="shared" ref="F9:F16" si="1">E9/B9</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>160</v>
-      </c>
-      <c r="C10" s="5">
-        <v>144</v>
-      </c>
-      <c r="D10" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>4</v>
-      </c>
-      <c r="B11">
-        <v>250</v>
-      </c>
-      <c r="C11" s="5">
-        <v>216</v>
-      </c>
-      <c r="D11" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="1"/>
-        <v>0.48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>5</v>
-      </c>
-      <c r="B12">
-        <v>280</v>
-      </c>
-      <c r="C12" s="5">
-        <v>252</v>
-      </c>
-      <c r="D12" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>140</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>6</v>
-      </c>
-      <c r="B13">
-        <v>360</v>
-      </c>
-      <c r="C13" s="5">
-        <v>324</v>
-      </c>
-      <c r="D13" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>180</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>7</v>
-      </c>
-      <c r="B14">
-        <v>560</v>
-      </c>
-      <c r="C14" s="5">
-        <v>504</v>
-      </c>
-      <c r="D14" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>280</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>8</v>
-      </c>
-      <c r="B15">
-        <v>810</v>
-      </c>
-      <c r="C15" s="5">
-        <v>720</v>
-      </c>
-      <c r="D15" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="1"/>
-        <v>0.49382716049382713</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>9</v>
-      </c>
-      <c r="B16">
-        <v>30500</v>
-      </c>
-      <c r="C16" s="5">
-        <v>7000</v>
-      </c>
-      <c r="D16" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>17500</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="1"/>
-        <v>0.57377049180327866</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>169</v>
-      </c>
-      <c r="C2">
-        <v>287</v>
-      </c>
-      <c r="D2">
-        <f>B2*C2</f>
-        <v>48503</v>
-      </c>
-      <c r="E2">
-        <f>D2/$D$4*$E$4</f>
-        <v>18.546941608010311</v>
-      </c>
-      <c r="F2" s="2">
-        <f>E2/$E$4*$F$4</f>
-        <v>85436143.055417866</v>
-      </c>
-      <c r="G2" s="2">
-        <f>E2/F2*1000000</f>
-        <v>0.21708542713567841</v>
-      </c>
-      <c r="H2">
-        <f>SQRT(G2)</f>
-        <v>0.46592427188941166</v>
-      </c>
-      <c r="I2">
-        <f>2*H2</f>
-        <v>0.93184854377882331</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>228</v>
-      </c>
-      <c r="C3">
-        <v>325</v>
-      </c>
-      <c r="D3">
-        <f>B3*C3</f>
-        <v>74100</v>
-      </c>
-      <c r="F3">
-        <f>B8</f>
-        <v>1006632960</v>
-      </c>
-      <c r="G3" s="2">
-        <f t="shared" ref="G3:G4" si="0">E3/F3*1000000</f>
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H4" si="1">SQRT(G3)</f>
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I4" si="2">2*H3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1078</v>
-      </c>
-      <c r="C4" s="1">
-        <v>524</v>
-      </c>
-      <c r="D4">
-        <f>B4*C4</f>
-        <v>564872</v>
-      </c>
-      <c r="E4">
-        <v>216</v>
-      </c>
-      <c r="F4" s="2">
-        <v>995000000</v>
-      </c>
-      <c r="G4" s="2">
-        <f t="shared" si="0"/>
-        <v>0.21708542713567841</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="1"/>
-        <v>0.46592427188941166</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="2"/>
-        <v>0.93184854377882331</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="E6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2">
-        <v>2270000000</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7">
-        <v>20</v>
-      </c>
-      <c r="F7">
-        <f>E7*POWER(2,20)*8</f>
-        <v>167772160</v>
-      </c>
-      <c r="G7">
-        <v>6</v>
-      </c>
-      <c r="H7">
-        <f>G7*F7</f>
-        <v>1006632960</v>
-      </c>
-      <c r="I7">
-        <f>E3/H7*1000000</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <f>H7</f>
-        <v>1006632960</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8">
-        <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2">
-        <f>B7-B8</f>
-        <v>1263367040</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="D14">
-        <v>0.1125</v>
-      </c>
-      <c r="F14" s="5">
-        <v>1</v>
-      </c>
-      <c r="G14" s="5">
-        <v>112.5</v>
-      </c>
-      <c r="H14">
-        <v>112.5</v>
-      </c>
-      <c r="I14">
-        <v>112.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="3">
-        <v>0.1993</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="5">
-        <v>2</v>
-      </c>
-      <c r="G15" s="5">
-        <v>112.5</v>
-      </c>
-      <c r="H15">
-        <v>112.5</v>
-      </c>
-      <c r="I15">
-        <v>112.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="D16">
-        <v>0.42</v>
-      </c>
-      <c r="F16" s="5">
-        <v>3</v>
-      </c>
-      <c r="G16" s="5">
-        <v>112.5</v>
-      </c>
-      <c r="H16">
-        <v>199.3</v>
-      </c>
-      <c r="I16">
-        <v>131.49469999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D17">
-        <v>0.71819999999999995</v>
-      </c>
-      <c r="F17" s="5">
-        <v>4</v>
-      </c>
-      <c r="G17" s="5">
-        <v>168.8</v>
-      </c>
-      <c r="H17">
-        <v>199.3</v>
-      </c>
-      <c r="I17">
-        <v>247.32849999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F18" s="5">
-        <v>5</v>
-      </c>
-      <c r="G18" s="5">
-        <v>225</v>
-      </c>
-      <c r="H18">
-        <v>420</v>
-      </c>
-      <c r="I18">
-        <v>374.14409999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F19" s="5">
-        <v>6</v>
-      </c>
-      <c r="G19" s="5">
-        <v>337.6</v>
-      </c>
-      <c r="H19">
-        <v>420</v>
-      </c>
-      <c r="I19">
-        <v>540.39850000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F20" s="5">
-        <v>7</v>
-      </c>
-      <c r="G20" s="5">
-        <v>450.1</v>
-      </c>
-      <c r="H20">
-        <v>718.2</v>
-      </c>
-      <c r="I20">
-        <v>718.20759999999996</v>
-      </c>
-    </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F21" s="5">
-        <v>8</v>
-      </c>
-      <c r="G21" s="5">
-        <v>566.5</v>
-      </c>
-      <c r="H21">
-        <v>718.2</v>
-      </c>
-    </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F22" s="5">
-        <v>9</v>
-      </c>
-      <c r="G22" s="5">
-        <v>19400</v>
-      </c>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G23" s="6">
-        <v>145900</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updating merom validation data
</commit_message>
<xml_diff>
--- a/data/processor_wla_validation.xlsx
+++ b/data/processor_wla_validation.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="15120" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="15120" windowHeight="7995"/>
   </bookViews>
   <sheets>
-    <sheet name="Merom 65nm Data" sheetId="1" r:id="rId1"/>
+    <sheet name="65nm Merom (2)" sheetId="9" r:id="rId1"/>
     <sheet name="65nm Merom" sheetId="2" r:id="rId2"/>
     <sheet name="45nm Penryn" sheetId="7" r:id="rId3"/>
     <sheet name="Sandy Bridge EP-4 32nm Data" sheetId="3" r:id="rId4"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="50">
   <si>
     <t>w (px)</t>
   </si>
@@ -159,6 +159,18 @@
   </si>
   <si>
     <t>Core Power</t>
+  </si>
+  <si>
+    <t>65nm</t>
+  </si>
+  <si>
+    <t>Codename Merom</t>
+  </si>
+  <si>
+    <t>Intel Core 2 Duo E6850</t>
+  </si>
+  <si>
+    <t>bP (um)</t>
   </si>
 </sst>
 </file>
@@ -202,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -219,6 +231,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,11 +457,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="136654208"/>
-        <c:axId val="136660480"/>
+        <c:axId val="147251200"/>
+        <c:axId val="147253120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="136654208"/>
+        <c:axId val="147251200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -472,19 +485,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136660480"/>
+        <c:crossAx val="147253120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="136660480"/>
+        <c:axId val="147253120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -514,14 +526,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136654208"/>
+        <c:crossAx val="147251200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -879,335 +890,632 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J21"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>278</v>
-      </c>
-      <c r="C3">
-        <v>193</v>
-      </c>
-      <c r="D3">
-        <f>B3*C3</f>
-        <v>53654</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3" si="0">D3/$D$5*$E$5</f>
-        <v>28.655223284146206</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="5"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>261</v>
-      </c>
-      <c r="C4">
-        <v>393</v>
-      </c>
-      <c r="D4">
-        <f>B4*C4</f>
-        <v>102573</v>
-      </c>
-      <c r="E4">
-        <f>D4/$D$5*$E$5</f>
-        <v>54.781604687902657</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B7">
+        <v>323</v>
+      </c>
+      <c r="C7">
+        <v>480</v>
+      </c>
+      <c r="D7">
+        <f>B7*C7</f>
+        <v>155040</v>
+      </c>
+      <c r="E7">
+        <f>D7/$D$8*$E$8</f>
+        <v>56.323326550365437</v>
+      </c>
+      <c r="F7">
+        <f>H11</f>
+        <v>201326592</v>
+      </c>
+      <c r="G7">
+        <f>E7/F7*1000000</f>
+        <v>0.27976098930023829</v>
+      </c>
+      <c r="H7">
+        <f>SQRT(G7)</f>
+        <v>0.52892437011376048</v>
+      </c>
+      <c r="I7">
+        <f>SQRT(6)*H7</f>
+        <v>1.2955948193017095</v>
+      </c>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
-        <v>599</v>
-      </c>
-      <c r="C5" s="1">
-        <v>447</v>
-      </c>
-      <c r="D5">
-        <f>B5*C5</f>
-        <v>267753</v>
-      </c>
-      <c r="E5">
+      <c r="B8" s="3">
+        <v>717</v>
+      </c>
+      <c r="C8" s="3">
+        <v>549</v>
+      </c>
+      <c r="D8">
+        <f>B8*C8</f>
+        <v>393633</v>
+      </c>
+      <c r="E8" s="1">
         <v>143</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="F8" s="8">
+        <v>291000000</v>
+      </c>
+      <c r="G8" s="2">
+        <f>E8/F8*1000000</f>
+        <v>0.49140893470790376</v>
+      </c>
+      <c r="H8">
+        <f>SQRT(G8)</f>
+        <v>0.70100565954056593</v>
+      </c>
+      <c r="I8">
+        <f>2*H8</f>
+        <v>1.4020113190811319</v>
+      </c>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="E7" s="1" t="s">
+      <c r="C10" s="1"/>
+      <c r="E10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="J10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B11" s="2">
         <f>291000000</f>
         <v>291000000</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E8">
+      <c r="E11">
         <v>4</v>
       </c>
-      <c r="F8">
-        <f>E8*POWER(2,20)*8</f>
+      <c r="F11">
+        <f>E11*POWER(2,20)*8</f>
         <v>33554432</v>
       </c>
-      <c r="G8">
+      <c r="G11">
         <v>6</v>
       </c>
-      <c r="H8">
-        <f>G8*F8</f>
+      <c r="H11">
+        <f>G11*F11</f>
         <v>201326592</v>
       </c>
-      <c r="I8">
-        <f>E4/H8*1000000</f>
-        <v>0.27210317397069261</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="I11">
+        <f>E7/H11*1000000</f>
+        <v>0.27976098930023829</v>
+      </c>
+      <c r="J11">
+        <f>SQRT(I11)</f>
+        <v>0.52892437011376048</v>
+      </c>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9">
-        <f>H8</f>
+      <c r="B12">
+        <f>H11</f>
         <v>201326592</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="J9">
-        <f>I9*H8/1000000</f>
-        <v>114.75615744</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="D12" s="1"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2">
-        <f>B8-B9</f>
+      <c r="B13" s="2">
+        <f>B11-B12</f>
         <v>89673408</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="2">
-        <f>B10*0.9/2</f>
+      <c r="B14" s="2">
+        <f>B13*0.9/2</f>
         <v>40353033.600000001</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D16" s="1"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D12" s="1" t="s">
+      <c r="I19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="2">
-        <f>B11</f>
+      <c r="B20">
+        <v>83</v>
+      </c>
+      <c r="C20">
+        <v>261</v>
+      </c>
+      <c r="D20">
+        <f>B20*C20</f>
+        <v>21663</v>
+      </c>
+      <c r="E20">
+        <f>D20/$D$8*$E$8</f>
+        <v>7.8697898804216111</v>
+      </c>
+      <c r="F20">
+        <f>SUM(E20:E25)</f>
+        <v>29.45276945784525</v>
+      </c>
+      <c r="G20" s="2">
+        <f>B14</f>
         <v>40353033.600000001</v>
       </c>
-      <c r="F12" s="2">
-        <f>E3/E12*1000000</f>
-        <v>0.710113236298205</v>
-      </c>
-      <c r="G12">
-        <f>SQRT(F12)</f>
-        <v>0.84268216801959506</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="H20" s="2">
+        <f>F20/G20*1000000</f>
+        <v>0.7298774548103677</v>
+      </c>
+      <c r="I20">
+        <f>SQRT(H20)</f>
+        <v>0.85432865737394514</v>
+      </c>
+      <c r="J20">
+        <f>2*I20</f>
+        <v>1.7086573147478903</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>102</v>
+      </c>
+      <c r="C21">
+        <v>239</v>
+      </c>
+      <c r="D21">
+        <f>B21*C21</f>
+        <v>24378</v>
+      </c>
+      <c r="E21">
+        <f>D21/$D$8*$E$8</f>
+        <v>8.8561020036429881</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>74</v>
+      </c>
+      <c r="C22">
+        <v>223</v>
+      </c>
+      <c r="D22">
+        <f>B22*C22</f>
+        <v>16502</v>
+      </c>
+      <c r="E22">
+        <f>D22/$D$8*$E$8</f>
+        <v>5.9948886399260219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>33</v>
+      </c>
+      <c r="C23">
+        <v>180</v>
+      </c>
+      <c r="D23">
+        <f>B23*C23</f>
+        <v>5940</v>
+      </c>
+      <c r="E23">
+        <f>D23/$D$8*$E$8</f>
+        <v>2.1578983469373756</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>51</v>
+      </c>
+      <c r="C24">
+        <v>161</v>
+      </c>
+      <c r="D24">
+        <f>B24*C24</f>
+        <v>8211</v>
+      </c>
+      <c r="E24">
+        <f>D24/$D$8*$E$8</f>
+        <v>2.9829130179634329</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>30</v>
+      </c>
+      <c r="C25">
+        <v>146</v>
+      </c>
+      <c r="D25">
+        <f>B25*C25</f>
+        <v>4380</v>
+      </c>
+      <c r="E25">
+        <f>D25/$D$8*$E$8</f>
+        <v>1.5911775689538223</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
         <v>1</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="B28">
+        <v>210</v>
+      </c>
+      <c r="C28" s="5">
+        <v>170</v>
+      </c>
+      <c r="D28" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="E28">
+        <f>C28/D28</f>
+        <v>106.25</v>
+      </c>
+      <c r="F28">
+        <f>E28/B28</f>
+        <v>0.50595238095238093</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>210</v>
+      </c>
+      <c r="C29" s="5">
+        <v>190</v>
+      </c>
+      <c r="D29" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E29">
+        <f t="shared" ref="E29:E35" si="0">C29/D29</f>
+        <v>105.55555555555556</v>
+      </c>
+      <c r="F29">
+        <f t="shared" ref="F29:F35" si="1">E29/B29</f>
+        <v>0.50264550264550267</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>220</v>
+      </c>
+      <c r="C30" s="5">
+        <v>200</v>
+      </c>
+      <c r="D30" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>111.11111111111111</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>0.50505050505050508</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>280</v>
+      </c>
+      <c r="C31" s="5">
+        <v>250</v>
+      </c>
+      <c r="D31" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>138.88888888888889</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>0.49603174603174605</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>330</v>
+      </c>
+      <c r="C32" s="5">
+        <v>300</v>
+      </c>
+      <c r="D32" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>166.66666666666666</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>0.50505050505050497</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
         <v>6</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17">
-        <v>114</v>
-      </c>
-      <c r="C17">
-        <v>149</v>
-      </c>
-      <c r="D17">
-        <f>B17*C17</f>
-        <v>16986</v>
-      </c>
-      <c r="E17">
-        <f t="shared" ref="E17:E21" si="1">D17/$D$5*$E$5</f>
-        <v>9.0717863105175294</v>
-      </c>
-      <c r="F17">
-        <f>SUM(E17:E21)</f>
-        <v>16.255085844042831</v>
-      </c>
-      <c r="G17" s="2">
-        <f>B11</f>
-        <v>40353033.600000001</v>
-      </c>
-      <c r="H17" s="2">
-        <f>F17/G17*1000000</f>
-        <v>0.40282190442412813</v>
-      </c>
-      <c r="I17">
-        <f>SQRT(H17)</f>
-        <v>0.63468252254503443</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>36</v>
-      </c>
-      <c r="C18">
-        <v>13</v>
-      </c>
-      <c r="D18">
-        <f t="shared" ref="D18:D21" si="2">B18*C18</f>
-        <v>468</v>
-      </c>
-      <c r="E18">
+      <c r="B33">
+        <v>480</v>
+      </c>
+      <c r="C33" s="5">
+        <v>430</v>
+      </c>
+      <c r="D33" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>238.88888888888889</v>
+      </c>
+      <c r="F33">
         <f t="shared" si="1"/>
-        <v>0.24994677930779485</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>46</v>
-      </c>
-      <c r="C19">
-        <v>137</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="2"/>
-        <v>6302</v>
-      </c>
-      <c r="E19">
+        <v>0.49768518518518517</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>7</v>
+      </c>
+      <c r="B34">
+        <v>720</v>
+      </c>
+      <c r="C34" s="5">
+        <v>650</v>
+      </c>
+      <c r="D34" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>361.11111111111109</v>
+      </c>
+      <c r="F34">
         <f t="shared" si="1"/>
-        <v>3.3657363316190669</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <v>69</v>
-      </c>
-      <c r="C20">
-        <v>89</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="2"/>
-        <v>6141</v>
-      </c>
-      <c r="E20">
+        <v>0.50154320987654322</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>8</v>
+      </c>
+      <c r="B35">
+        <v>1080</v>
+      </c>
+      <c r="C35" s="5">
+        <v>975</v>
+      </c>
+      <c r="D35" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>541.66666666666663</v>
+      </c>
+      <c r="F35">
         <f t="shared" si="1"/>
-        <v>3.2797503669426673</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <v>49</v>
-      </c>
-      <c r="C21">
-        <v>11</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="2"/>
-        <v>539</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="1"/>
-        <v>0.28786605565577233</v>
-      </c>
+        <v>0.50154320987654322</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1217,10 +1525,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P33"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,658 +1539,673 @@
     <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="1"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B6">
         <v>278</v>
       </c>
-      <c r="C3">
+      <c r="C6">
         <v>193</v>
       </c>
-      <c r="D3">
-        <f>B3*C3</f>
+      <c r="D6">
+        <f>B6*C6</f>
         <v>53654</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3" si="0">D3/$D$5*$E$5</f>
+      <c r="E6">
+        <f>D6/$D$8*$E$8</f>
         <v>48.595636064223967</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F6" s="2">
         <v>404000000</v>
       </c>
-      <c r="G3" s="2">
-        <f>E3/F3*1000000</f>
+      <c r="G6" s="2">
+        <f>E6/F6*1000000</f>
         <v>0.12028622788174251</v>
       </c>
-      <c r="H3">
-        <f>SQRT(G3)</f>
+      <c r="H6">
+        <f>SQRT(G6)</f>
         <v>0.34682304981321888</v>
       </c>
-      <c r="I3">
-        <f>2*H3</f>
+      <c r="I6">
+        <f>2*H6</f>
         <v>0.69364609962643775</v>
       </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="4" t="s">
+      <c r="L6" s="5"/>
+      <c r="M6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N6" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>196</v>
-      </c>
-      <c r="C4">
-        <v>300</v>
-      </c>
-      <c r="D4">
-        <f>B4*C4</f>
-        <v>58800</v>
-      </c>
-      <c r="E4">
-        <f>D4/$D$5*$E$5</f>
-        <v>53.256484149855908</v>
-      </c>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5">
-        <v>1</v>
-      </c>
-      <c r="N4" s="5">
-        <v>210</v>
-      </c>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>455</v>
-      </c>
-      <c r="C5" s="1">
-        <v>347</v>
-      </c>
-      <c r="D5">
-        <f>B5*C5</f>
-        <v>157885</v>
-      </c>
-      <c r="E5">
-        <v>143</v>
-      </c>
-      <c r="F5" s="2">
-        <v>291000000</v>
-      </c>
-      <c r="G5" s="2">
-        <f>E5/F5*1000000</f>
-        <v>0.49140893470790376</v>
-      </c>
-      <c r="H5">
-        <f>SQRT(G5)</f>
-        <v>0.70100565954056593</v>
-      </c>
-      <c r="I5">
-        <f>2*H5</f>
-        <v>1.4020113190811319</v>
-      </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5">
-        <v>2</v>
-      </c>
-      <c r="N5" s="5">
-        <v>210</v>
-      </c>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L6" s="5"/>
-      <c r="M6" s="5">
-        <v>3</v>
-      </c>
-      <c r="N6" s="5">
-        <v>220</v>
       </c>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="E7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>17</v>
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>196</v>
+      </c>
+      <c r="C7">
+        <v>300</v>
+      </c>
+      <c r="D7">
+        <f>B7*C7</f>
+        <v>58800</v>
+      </c>
+      <c r="E7">
+        <f>D7/$D$8*$E$8</f>
+        <v>53.256484149855908</v>
       </c>
       <c r="L7" s="5"/>
       <c r="M7" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N7" s="5">
-        <v>280</v>
+        <v>210</v>
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3">
+        <v>455</v>
+      </c>
+      <c r="C8" s="3">
+        <v>347</v>
+      </c>
+      <c r="D8">
+        <f>B8*C8</f>
+        <v>157885</v>
+      </c>
+      <c r="E8" s="1">
+        <v>143</v>
+      </c>
+      <c r="F8" s="8">
+        <v>291000000</v>
+      </c>
+      <c r="G8" s="2">
+        <f>E8/F8*1000000</f>
+        <v>0.49140893470790376</v>
+      </c>
+      <c r="H8">
+        <f>SQRT(G8)</f>
+        <v>0.70100565954056593</v>
+      </c>
+      <c r="I8">
+        <f>2*H8</f>
+        <v>1.4020113190811319</v>
+      </c>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5">
+        <v>2</v>
+      </c>
+      <c r="N8" s="5">
+        <v>210</v>
+      </c>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L9" s="5"/>
+      <c r="M9" s="5">
+        <v>3</v>
+      </c>
+      <c r="N9" s="5">
+        <v>220</v>
+      </c>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5">
+        <v>4</v>
+      </c>
+      <c r="N10" s="5">
+        <v>280</v>
+      </c>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B11" s="2">
         <f>291000000</f>
         <v>291000000</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E8">
+      <c r="E11">
         <v>4</v>
       </c>
-      <c r="F8">
-        <f>E8*POWER(2,20)*8</f>
+      <c r="F11">
+        <f>E11*POWER(2,20)*8</f>
         <v>33554432</v>
       </c>
-      <c r="G8">
+      <c r="G11">
         <v>6</v>
       </c>
-      <c r="H8">
-        <f>G8*F8</f>
+      <c r="H11">
+        <f>G11*F11</f>
         <v>201326592</v>
       </c>
-      <c r="I8">
-        <f>E4/H8*1000000</f>
+      <c r="I11">
+        <f>E7/H11*1000000</f>
         <v>0.26452781831153188</v>
       </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5">
+      <c r="L11" s="5"/>
+      <c r="M11" s="5">
         <v>5</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N11" s="5">
         <v>330</v>
       </c>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9">
-        <f>H8</f>
+      <c r="B12">
+        <f>H11</f>
         <v>201326592</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I9">
+      <c r="I12">
         <v>0.56999999999999995</v>
       </c>
-      <c r="J9">
-        <f>I9*H8/1000000</f>
+      <c r="J12">
+        <f>I12*H11/1000000</f>
         <v>114.75615744</v>
       </c>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5">
+      <c r="L12" s="5"/>
+      <c r="M12" s="5">
         <v>6</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N12" s="5">
         <v>480</v>
       </c>
-      <c r="O9" s="5"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2">
-        <f>B8-B9</f>
+      <c r="B13" s="2">
+        <f>B11-B12</f>
         <v>89673408</v>
       </c>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5">
+      <c r="L13" s="5"/>
+      <c r="M13" s="5">
         <v>7</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N13" s="5">
         <v>720</v>
       </c>
-      <c r="O10" s="5"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="O13" s="5"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="2">
-        <f>B10*0.9/2</f>
+      <c r="B14" s="2">
+        <f>B13*0.9/2</f>
         <v>40353033.600000001</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M14" s="5">
         <v>8</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N14" s="5">
         <v>1080</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D12" s="1"/>
-      <c r="E12" s="1" t="s">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
+      <c r="E15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D13" s="1" t="s">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="2">
-        <f>B8</f>
+      <c r="E16" s="2">
+        <f>B11</f>
         <v>291000000</v>
       </c>
-      <c r="F13" s="2">
-        <f>E5/E13*1000000</f>
+      <c r="F16" s="2">
+        <f>E8/E16*1000000</f>
         <v>0.49140893470790376</v>
       </c>
-      <c r="G13">
-        <f>SQRT(F13)</f>
+      <c r="G16">
+        <f>SQRT(F16)</f>
         <v>0.70100565954056593</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B17">
+      <c r="B20">
         <v>109</v>
       </c>
-      <c r="C17">
+      <c r="C20">
         <v>146</v>
       </c>
-      <c r="D17">
-        <f>B17*C17</f>
+      <c r="D20">
+        <f>B20*C20</f>
         <v>15914</v>
       </c>
-      <c r="E17">
-        <f t="shared" ref="E17:E21" si="1">D17/$D$5*$E$5</f>
+      <c r="E20">
+        <f>D20/$D$8*$E$8</f>
         <v>14.413668176204199</v>
       </c>
-      <c r="F17">
-        <f>SUM(E17:E21)</f>
+      <c r="F20">
+        <f>SUM(E20:E24)</f>
         <v>27.112803622890077</v>
       </c>
-      <c r="G17" s="2">
-        <f>B11</f>
+      <c r="G20" s="2">
+        <f>B14</f>
         <v>40353033.600000001</v>
       </c>
-      <c r="H17" s="2">
-        <f>F17/G17*1000000</f>
+      <c r="H20" s="2">
+        <f>F20/G20*1000000</f>
         <v>0.67189009608660688</v>
       </c>
-      <c r="I17">
-        <f>SQRT(H17)</f>
+      <c r="I20">
+        <f>SQRT(H20)</f>
         <v>0.81968902401252564</v>
       </c>
-      <c r="J17">
-        <f>2*I17</f>
+      <c r="J20">
+        <f>2*I20</f>
         <v>1.6393780480250513</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>40</v>
-      </c>
-      <c r="C18">
-        <v>15</v>
-      </c>
-      <c r="D18">
-        <f t="shared" ref="D18:D21" si="2">B18*C18</f>
-        <v>600</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="1"/>
-        <v>0.54343351173322352</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>47</v>
-      </c>
-      <c r="C19">
-        <v>140</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="2"/>
-        <v>6580</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="1"/>
-        <v>5.9596541786743513</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <v>68</v>
-      </c>
-      <c r="C20">
-        <v>92</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="2"/>
-        <v>6256</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="1"/>
-        <v>5.6662000823384107</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21">
+        <v>40</v>
+      </c>
+      <c r="C21">
+        <v>15</v>
+      </c>
+      <c r="D21">
+        <f>B21*C21</f>
+        <v>600</v>
+      </c>
+      <c r="E21">
+        <f>D21/$D$8*$E$8</f>
+        <v>0.54343351173322352</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>47</v>
+      </c>
+      <c r="C22">
+        <v>140</v>
+      </c>
+      <c r="D22">
+        <f>B22*C22</f>
+        <v>6580</v>
+      </c>
+      <c r="E22">
+        <f>D22/$D$8*$E$8</f>
+        <v>5.9596541786743513</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>68</v>
+      </c>
+      <c r="C23">
+        <v>92</v>
+      </c>
+      <c r="D23">
+        <f>B23*C23</f>
+        <v>6256</v>
+      </c>
+      <c r="E23">
+        <f>D23/$D$8*$E$8</f>
+        <v>5.6662000823384107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24">
         <v>45</v>
       </c>
-      <c r="C21">
+      <c r="C24">
         <v>13</v>
       </c>
-      <c r="D21">
-        <f t="shared" si="2"/>
+      <c r="D24">
+        <f>B24*C24</f>
         <v>585</v>
       </c>
-      <c r="E21">
-        <f t="shared" si="1"/>
+      <c r="E24">
+        <f>D24/$D$8*$E$8</f>
         <v>0.52984767393989296</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
-        <v>1</v>
-      </c>
-      <c r="B25">
-        <v>210</v>
-      </c>
-      <c r="C25" s="5">
-        <v>170</v>
-      </c>
-      <c r="D25" s="5">
-        <v>1.6</v>
-      </c>
-      <c r="E25">
-        <f>C25/D25</f>
-        <v>106.25</v>
-      </c>
-      <c r="F25">
-        <f>E25/B25</f>
-        <v>0.50595238095238093</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
-        <v>2</v>
-      </c>
-      <c r="B26">
-        <v>210</v>
-      </c>
-      <c r="C26" s="5">
-        <v>190</v>
-      </c>
-      <c r="D26" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E26">
-        <f t="shared" ref="E26:E33" si="3">C26/D26</f>
-        <v>105.55555555555556</v>
-      </c>
-      <c r="F26">
-        <f t="shared" ref="F26:F33" si="4">E26/B26</f>
-        <v>0.50264550264550267</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
-        <v>3</v>
-      </c>
-      <c r="B27">
-        <v>220</v>
-      </c>
-      <c r="C27" s="5">
-        <v>200</v>
-      </c>
-      <c r="D27" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="3"/>
-        <v>111.11111111111111</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="4"/>
-        <v>0.50505050505050508</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B28">
-        <v>280</v>
+        <v>210</v>
       </c>
       <c r="C28" s="5">
-        <v>250</v>
+        <v>170</v>
       </c>
       <c r="D28" s="5">
-        <v>1.8</v>
+        <v>1.6</v>
       </c>
       <c r="E28">
-        <f t="shared" si="3"/>
-        <v>138.88888888888889</v>
+        <f>C28/D28</f>
+        <v>106.25</v>
       </c>
       <c r="F28">
-        <f t="shared" si="4"/>
-        <v>0.49603174603174605</v>
+        <f>E28/B28</f>
+        <v>0.50595238095238093</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B29">
-        <v>330</v>
+        <v>210</v>
       </c>
       <c r="C29" s="5">
-        <v>300</v>
+        <v>190</v>
       </c>
       <c r="D29" s="5">
         <v>1.8</v>
       </c>
       <c r="E29">
-        <f t="shared" si="3"/>
-        <v>166.66666666666666</v>
+        <f t="shared" ref="E29:E35" si="0">C29/D29</f>
+        <v>105.55555555555556</v>
       </c>
       <c r="F29">
-        <f t="shared" si="4"/>
-        <v>0.50505050505050497</v>
+        <f t="shared" ref="F29:F35" si="1">E29/B29</f>
+        <v>0.50264550264550267</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B30">
-        <v>480</v>
+        <v>220</v>
       </c>
       <c r="C30" s="5">
-        <v>430</v>
+        <v>200</v>
       </c>
       <c r="D30" s="5">
         <v>1.8</v>
       </c>
       <c r="E30">
-        <f t="shared" si="3"/>
-        <v>238.88888888888889</v>
+        <f t="shared" si="0"/>
+        <v>111.11111111111111</v>
       </c>
       <c r="F30">
-        <f t="shared" si="4"/>
-        <v>0.49768518518518517</v>
+        <f t="shared" si="1"/>
+        <v>0.50505050505050508</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B31">
-        <v>720</v>
+        <v>280</v>
       </c>
       <c r="C31" s="5">
-        <v>650</v>
+        <v>250</v>
       </c>
       <c r="D31" s="5">
         <v>1.8</v>
       </c>
       <c r="E31">
-        <f t="shared" si="3"/>
-        <v>361.11111111111109</v>
+        <f t="shared" si="0"/>
+        <v>138.88888888888889</v>
       </c>
       <c r="F31">
-        <f t="shared" si="4"/>
-        <v>0.50154320987654322</v>
+        <f t="shared" si="1"/>
+        <v>0.49603174603174605</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B32">
-        <v>1080</v>
+        <v>330</v>
       </c>
       <c r="C32" s="5">
-        <v>975</v>
+        <v>300</v>
       </c>
       <c r="D32" s="5">
         <v>1.8</v>
       </c>
       <c r="E32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
+        <v>166.66666666666666</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>0.50505050505050497</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>480</v>
+      </c>
+      <c r="C33" s="5">
+        <v>430</v>
+      </c>
+      <c r="D33" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>238.88888888888889</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>0.49768518518518517</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>7</v>
+      </c>
+      <c r="B34">
+        <v>720</v>
+      </c>
+      <c r="C34" s="5">
+        <v>650</v>
+      </c>
+      <c r="D34" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>361.11111111111109</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>0.50154320987654322</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>8</v>
+      </c>
+      <c r="B35">
+        <v>1080</v>
+      </c>
+      <c r="C35" s="5">
+        <v>975</v>
+      </c>
+      <c r="D35" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
         <v>541.66666666666663</v>
       </c>
-      <c r="F32">
-        <f t="shared" si="4"/>
+      <c r="F35">
+        <f t="shared" si="1"/>
         <v>0.50154320987654322</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2336,7 +2659,7 @@
         <v>14094</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3" si="0">D3/$D$5*$E$5</f>
+        <f>D3/$D$5*$E$5</f>
         <v>20.525242718446602</v>
       </c>
       <c r="F3" s="2">
@@ -2391,15 +2714,15 @@
         <v>1006632960</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G5" si="1">E4/F4*1000000</f>
+        <f>E4/F4*1000000</f>
         <v>0.10720155771496227</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H5" si="2">SQRT(G4)</f>
+        <f>SQRT(G4)</f>
         <v>0.32741648968089904</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I5" si="3">2*H4</f>
+        <f>2*H4</f>
         <v>0.65483297936179807</v>
       </c>
       <c r="L4" s="5">
@@ -2437,15 +2760,15 @@
         <v>2270000000</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" si="1"/>
+        <f>E5/F5*1000000</f>
         <v>0.19162995594713658</v>
       </c>
       <c r="H5">
-        <f t="shared" si="2"/>
+        <f>SQRT(G5)</f>
         <v>0.43775558928143521</v>
       </c>
       <c r="I5">
-        <f t="shared" si="3"/>
+        <f>2*H5</f>
         <v>0.87551117856287042</v>
       </c>
       <c r="L5" s="5">
@@ -2893,15 +3216,15 @@
         <v>1006632960</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G4" si="0">E3/F3*1000000</f>
+        <f>E3/F3*1000000</f>
         <v>0</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H4" si="1">SQRT(G3)</f>
+        <f>SQRT(G3)</f>
         <v>0</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I4" si="2">2*H3</f>
+        <f>2*H3</f>
         <v>0</v>
       </c>
     </row>
@@ -2926,15 +3249,15 @@
         <v>995000000</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" si="0"/>
+        <f>E4/F4*1000000</f>
         <v>0.21708542713567841</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
+        <f>SQRT(G4)</f>
         <v>0.46592427188941166</v>
       </c>
       <c r="I4">
-        <f t="shared" si="2"/>
+        <f>2*H4</f>
         <v>0.93184854377882331</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding best fits for merom and penryn full chip cases
</commit_message>
<xml_diff>
--- a/data/processor_wla_validation.xlsx
+++ b/data/processor_wla_validation.xlsx
@@ -4,24 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="15120" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="15120" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="65nm Merom (2)" sheetId="9" r:id="rId1"/>
-    <sheet name="65nm Merom" sheetId="2" r:id="rId2"/>
-    <sheet name="45nm Penryn" sheetId="7" r:id="rId3"/>
-    <sheet name="Sandy Bridge EP-4 32nm Data" sheetId="3" r:id="rId4"/>
-    <sheet name="32nm Sandy Bridge (standard)" sheetId="6" r:id="rId5"/>
-    <sheet name="22nm - Ivy Bridge EP10" sheetId="4" r:id="rId6"/>
-    <sheet name="22nm Ivy Bridge (standard)" sheetId="5" r:id="rId7"/>
-    <sheet name="Sheet1" sheetId="8" r:id="rId8"/>
+    <sheet name="65nm Merom" sheetId="9" r:id="rId1"/>
+    <sheet name="45nm Penryn" sheetId="7" r:id="rId2"/>
+    <sheet name="Sandy Bridge EP-4 32nm Data" sheetId="3" r:id="rId3"/>
+    <sheet name="32nm Sandy Bridge (standard)" sheetId="6" r:id="rId4"/>
+    <sheet name="22nm - Ivy Bridge EP10" sheetId="4" r:id="rId5"/>
+    <sheet name="22nm Ivy Bridge (standard)" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="52">
   <si>
     <t>w (px)</t>
   </si>
@@ -116,9 +115,6 @@
     <t>Single-tier</t>
   </si>
   <si>
-    <t>Chip</t>
-  </si>
-  <si>
     <t>my</t>
   </si>
   <si>
@@ -128,12 +124,6 @@
     <t>TP (um)</t>
   </si>
   <si>
-    <t>Metal Layer</t>
-  </si>
-  <si>
-    <t>Pitch</t>
-  </si>
-  <si>
     <t>Thickness (nm)</t>
   </si>
   <si>
@@ -171,6 +161,21 @@
   </si>
   <si>
     <t>bP (um)</t>
+  </si>
+  <si>
+    <t>Intel Wolfdale (Penryn) 45nm Core 2 Duo E8600</t>
+  </si>
+  <si>
+    <t>Cache (MB)</t>
+  </si>
+  <si>
+    <t>Die shrink of Merom</t>
+  </si>
+  <si>
+    <t>derived from area</t>
+  </si>
+  <si>
+    <t>derived from transistor count</t>
   </si>
 </sst>
 </file>
@@ -892,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,17 +913,29 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="M2">
+        <v>75</v>
+      </c>
+      <c r="N2">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -949,7 +966,7 @@
         <v>19</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>20</v>
@@ -1066,7 +1083,7 @@
         <v>15</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="5"/>
@@ -1101,12 +1118,12 @@
         <v>201326592</v>
       </c>
       <c r="I11">
-        <f>E7/H11*1000000</f>
-        <v>0.27976098930023829</v>
+        <f>E7/F11*1000000</f>
+        <v>1.6785659358014295</v>
       </c>
       <c r="J11">
         <f>SQRT(I11)</f>
-        <v>0.52892437011376048</v>
+        <v>1.2955948193017095</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
@@ -1191,7 +1208,7 @@
         <v>19</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>27</v>
@@ -1324,16 +1341,16 @@
         <v>22</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1525,687 +1542,492 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5">
+        <v>385</v>
+      </c>
+      <c r="C5" s="5">
+        <v>237</v>
+      </c>
+      <c r="D5" s="5">
+        <f>B5*C5</f>
+        <v>91245</v>
+      </c>
+      <c r="E5" s="5">
+        <f>D5*E7/D7</f>
+        <v>21.676765097690943</v>
+      </c>
+      <c r="F5" s="6">
+        <f>F7*E5/E7</f>
+        <v>83060501.776198953</v>
+      </c>
+      <c r="G5" s="6">
+        <f>E5/F5*1000000</f>
+        <v>0.26097560975609752</v>
+      </c>
+      <c r="H5" s="5">
+        <f>SQRT(G5)</f>
+        <v>0.51085771967945981</v>
+      </c>
+      <c r="I5" s="5">
+        <f>2*H5</f>
+        <v>1.0217154393589196</v>
+      </c>
+      <c r="J5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5" s="7">
+        <v>65</v>
+      </c>
+      <c r="N5" s="5">
+        <v>1333</v>
+      </c>
+      <c r="O5" s="5">
+        <v>1.3625</v>
+      </c>
+      <c r="P5" s="5">
+        <v>3.3</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5">
+        <v>511</v>
+      </c>
+      <c r="C6" s="5">
+        <v>512</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" ref="D6" si="0">B6*C6</f>
+        <v>261632</v>
+      </c>
+      <c r="E6" s="5">
+        <f>D6/D7*E7</f>
+        <v>62.155026642984019</v>
+      </c>
+      <c r="F6" s="5">
+        <f>P11</f>
+        <v>301989888</v>
+      </c>
+      <c r="G6" s="6">
+        <f t="shared" ref="G6" si="1">E6/F6*1000000</f>
+        <v>0.20581823800333349</v>
+      </c>
+      <c r="H6" s="5">
+        <f t="shared" ref="H6" si="2">SQRT(G6)</f>
+        <v>0.45367194976473196</v>
+      </c>
+      <c r="I6" s="5">
+        <f>SQRT(6)*H6</f>
+        <v>1.1112647875371562</v>
+      </c>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7">
+        <v>800</v>
+      </c>
+      <c r="C7" s="7">
+        <v>563</v>
+      </c>
+      <c r="D7" s="7">
+        <f>B7*C7</f>
+        <v>450400</v>
+      </c>
+      <c r="E7" s="5">
+        <v>107</v>
+      </c>
+      <c r="F7" s="6">
+        <v>410000000</v>
+      </c>
+      <c r="G7" s="6">
+        <f>E7/F7*1000000</f>
+        <v>0.26097560975609757</v>
+      </c>
+      <c r="H7" s="5">
+        <f>SQRT(G7)</f>
+        <v>0.51085771967945981</v>
+      </c>
+      <c r="I7" s="5">
+        <f>2*H7</f>
+        <v>1.0217154393589196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5">
+        <v>385</v>
+      </c>
+      <c r="C8" s="5">
+        <v>237</v>
+      </c>
+      <c r="D8" s="5">
+        <f>B8*C8</f>
+        <v>91245</v>
+      </c>
+      <c r="E8" s="5">
+        <f>D8*E7/D7</f>
+        <v>21.676765097690943</v>
+      </c>
+      <c r="F8" s="2">
+        <f>0.9/2*(F7-F6)</f>
+        <v>48604550.399999999</v>
+      </c>
+      <c r="G8" s="6">
+        <f t="shared" ref="G8" si="3">E8/F8*1000000</f>
+        <v>0.44598221605380683</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" ref="H8" si="4">SQRT(G8)</f>
+        <v>0.66781899947052037</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" ref="I8" si="5">2*H8</f>
+        <v>1.3356379989410407</v>
+      </c>
+      <c r="J8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R10" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
         <v>1</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="B11">
+        <v>160</v>
+      </c>
+      <c r="C11" s="5">
+        <v>144</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E11">
+        <f>C11/D11</f>
+        <v>80</v>
+      </c>
+      <c r="F11">
+        <f>E11/B11</f>
+        <v>0.5</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11">
         <v>6</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="N11">
+        <f>M11*POWER(2,20)*8</f>
+        <v>50331648</v>
+      </c>
+      <c r="O11">
+        <v>6</v>
+      </c>
+      <c r="P11">
+        <f>O11*N11</f>
+        <v>301989888</v>
+      </c>
+      <c r="Q11">
+        <f>E6/N11*1000000</f>
+        <v>1.2349094280200008</v>
+      </c>
+      <c r="R11">
+        <f>SQRT(Q11)</f>
+        <v>1.1112647875371562</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>160</v>
+      </c>
+      <c r="C12" s="5">
+        <v>144</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="E12:E19" si="6">C12/D12</f>
+        <v>80</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:F19" si="7">E12/B12</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>160</v>
+      </c>
+      <c r="C13" s="5">
+        <v>144</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="6"/>
+        <v>80</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>250</v>
+      </c>
+      <c r="C14" s="5">
+        <v>216</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="6"/>
+        <v>120</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="7"/>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
         <v>5</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="1"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>278</v>
-      </c>
-      <c r="C6">
-        <v>193</v>
-      </c>
-      <c r="D6">
-        <f>B6*C6</f>
-        <v>53654</v>
-      </c>
-      <c r="E6">
-        <f>D6/$D$8*$E$8</f>
-        <v>48.595636064223967</v>
-      </c>
-      <c r="F6" s="2">
-        <v>404000000</v>
-      </c>
-      <c r="G6" s="2">
-        <f>E6/F6*1000000</f>
-        <v>0.12028622788174251</v>
-      </c>
-      <c r="H6">
-        <f>SQRT(G6)</f>
-        <v>0.34682304981321888</v>
-      </c>
-      <c r="I6">
-        <f>2*H6</f>
-        <v>0.69364609962643775</v>
-      </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>196</v>
-      </c>
-      <c r="C7">
-        <v>300</v>
-      </c>
-      <c r="D7">
-        <f>B7*C7</f>
-        <v>58800</v>
-      </c>
-      <c r="E7">
-        <f>D7/$D$8*$E$8</f>
-        <v>53.256484149855908</v>
-      </c>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5">
-        <v>1</v>
-      </c>
-      <c r="N7" s="5">
-        <v>210</v>
-      </c>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="3">
-        <v>455</v>
-      </c>
-      <c r="C8" s="3">
-        <v>347</v>
-      </c>
-      <c r="D8">
-        <f>B8*C8</f>
-        <v>157885</v>
-      </c>
-      <c r="E8" s="1">
-        <v>143</v>
-      </c>
-      <c r="F8" s="8">
-        <v>291000000</v>
-      </c>
-      <c r="G8" s="2">
-        <f>E8/F8*1000000</f>
-        <v>0.49140893470790376</v>
-      </c>
-      <c r="H8">
-        <f>SQRT(G8)</f>
-        <v>0.70100565954056593</v>
-      </c>
-      <c r="I8">
-        <f>2*H8</f>
-        <v>1.4020113190811319</v>
-      </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5">
-        <v>2</v>
-      </c>
-      <c r="N8" s="5">
-        <v>210</v>
-      </c>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L9" s="5"/>
-      <c r="M9" s="5">
-        <v>3</v>
-      </c>
-      <c r="N9" s="5">
-        <v>220</v>
-      </c>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="B15">
+        <v>280</v>
+      </c>
+      <c r="C15" s="5">
+        <v>252</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="6"/>
+        <v>140</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>360</v>
+      </c>
+      <c r="C16" s="5">
+        <v>324</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="6"/>
+        <v>180</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5">
-        <v>4</v>
-      </c>
-      <c r="N10" s="5">
+      <c r="B17">
+        <v>560</v>
+      </c>
+      <c r="C17" s="5">
+        <v>504</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="6"/>
         <v>280</v>
       </c>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="F17">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
         <v>8</v>
       </c>
-      <c r="B11" s="2">
-        <f>291000000</f>
-        <v>291000000</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="B18">
+        <v>810</v>
+      </c>
+      <c r="C18" s="5">
+        <v>720</v>
+      </c>
+      <c r="D18" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="6"/>
+        <v>400</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="7"/>
+        <v>0.49382716049382713</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
         <v>9</v>
       </c>
-      <c r="E11">
-        <v>4</v>
-      </c>
-      <c r="F11">
-        <f>E11*POWER(2,20)*8</f>
-        <v>33554432</v>
-      </c>
-      <c r="G11">
-        <v>6</v>
-      </c>
-      <c r="H11">
-        <f>G11*F11</f>
-        <v>201326592</v>
-      </c>
-      <c r="I11">
-        <f>E7/H11*1000000</f>
-        <v>0.26452781831153188</v>
-      </c>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5">
-        <v>5</v>
-      </c>
-      <c r="N11" s="5">
-        <v>330</v>
-      </c>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <f>H11</f>
-        <v>201326592</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="J12">
-        <f>I12*H11/1000000</f>
-        <v>114.75615744</v>
-      </c>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5">
-        <v>6</v>
-      </c>
-      <c r="N12" s="5">
-        <v>480</v>
-      </c>
-      <c r="O12" s="5"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="2">
-        <f>B11-B12</f>
-        <v>89673408</v>
-      </c>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5">
-        <v>7</v>
-      </c>
-      <c r="N13" s="5">
-        <v>720</v>
-      </c>
-      <c r="O13" s="5"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="2">
-        <f>B13*0.9/2</f>
-        <v>40353033.600000001</v>
-      </c>
-      <c r="M14" s="5">
-        <v>8</v>
-      </c>
-      <c r="N14" s="5">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="2">
-        <f>B11</f>
-        <v>291000000</v>
-      </c>
-      <c r="F16" s="2">
-        <f>E8/E16*1000000</f>
-        <v>0.49140893470790376</v>
-      </c>
-      <c r="G16">
-        <f>SQRT(F16)</f>
-        <v>0.70100565954056593</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20">
-        <v>109</v>
-      </c>
-      <c r="C20">
-        <v>146</v>
-      </c>
-      <c r="D20">
-        <f>B20*C20</f>
-        <v>15914</v>
-      </c>
-      <c r="E20">
-        <f>D20/$D$8*$E$8</f>
-        <v>14.413668176204199</v>
-      </c>
-      <c r="F20">
-        <f>SUM(E20:E24)</f>
-        <v>27.112803622890077</v>
-      </c>
-      <c r="G20" s="2">
-        <f>B14</f>
-        <v>40353033.600000001</v>
-      </c>
-      <c r="H20" s="2">
-        <f>F20/G20*1000000</f>
-        <v>0.67189009608660688</v>
-      </c>
-      <c r="I20">
-        <f>SQRT(H20)</f>
-        <v>0.81968902401252564</v>
-      </c>
-      <c r="J20">
-        <f>2*I20</f>
-        <v>1.6393780480250513</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <v>40</v>
-      </c>
-      <c r="C21">
-        <v>15</v>
-      </c>
-      <c r="D21">
-        <f>B21*C21</f>
-        <v>600</v>
-      </c>
-      <c r="E21">
-        <f>D21/$D$8*$E$8</f>
-        <v>0.54343351173322352</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <v>47</v>
-      </c>
-      <c r="C22">
-        <v>140</v>
-      </c>
-      <c r="D22">
-        <f>B22*C22</f>
-        <v>6580</v>
-      </c>
-      <c r="E22">
-        <f>D22/$D$8*$E$8</f>
-        <v>5.9596541786743513</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <v>68</v>
-      </c>
-      <c r="C23">
-        <v>92</v>
-      </c>
-      <c r="D23">
-        <f>B23*C23</f>
-        <v>6256</v>
-      </c>
-      <c r="E23">
-        <f>D23/$D$8*$E$8</f>
-        <v>5.6662000823384107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <v>45</v>
-      </c>
-      <c r="C24">
-        <v>13</v>
-      </c>
-      <c r="D24">
-        <f>B24*C24</f>
-        <v>585</v>
-      </c>
-      <c r="E24">
-        <f>D24/$D$8*$E$8</f>
-        <v>0.52984767393989296</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
-        <v>1</v>
-      </c>
-      <c r="B28">
-        <v>210</v>
-      </c>
-      <c r="C28" s="5">
-        <v>170</v>
-      </c>
-      <c r="D28" s="5">
-        <v>1.6</v>
-      </c>
-      <c r="E28">
-        <f>C28/D28</f>
-        <v>106.25</v>
-      </c>
-      <c r="F28">
-        <f>E28/B28</f>
-        <v>0.50595238095238093</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
-        <v>2</v>
-      </c>
-      <c r="B29">
-        <v>210</v>
-      </c>
-      <c r="C29" s="5">
-        <v>190</v>
-      </c>
-      <c r="D29" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E29">
-        <f t="shared" ref="E29:E35" si="0">C29/D29</f>
-        <v>105.55555555555556</v>
-      </c>
-      <c r="F29">
-        <f t="shared" ref="F29:F35" si="1">E29/B29</f>
-        <v>0.50264550264550267</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
-        <v>3</v>
-      </c>
-      <c r="B30">
-        <v>220</v>
-      </c>
-      <c r="C30" s="5">
-        <v>200</v>
-      </c>
-      <c r="D30" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E30">
-        <f t="shared" si="0"/>
-        <v>111.11111111111111</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="1"/>
-        <v>0.50505050505050508</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
-        <v>4</v>
-      </c>
-      <c r="B31">
-        <v>280</v>
-      </c>
-      <c r="C31" s="5">
-        <v>250</v>
-      </c>
-      <c r="D31" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="0"/>
-        <v>138.88888888888889</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="1"/>
-        <v>0.49603174603174605</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
-        <v>5</v>
-      </c>
-      <c r="B32">
-        <v>330</v>
-      </c>
-      <c r="C32" s="5">
-        <v>300</v>
-      </c>
-      <c r="D32" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E32">
-        <f t="shared" si="0"/>
-        <v>166.66666666666666</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="1"/>
-        <v>0.50505050505050497</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
-        <v>6</v>
-      </c>
-      <c r="B33">
-        <v>480</v>
-      </c>
-      <c r="C33" s="5">
-        <v>430</v>
-      </c>
-      <c r="D33" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="0"/>
-        <v>238.88888888888889</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="1"/>
-        <v>0.49768518518518517</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
-        <v>7</v>
-      </c>
-      <c r="B34">
-        <v>720</v>
-      </c>
-      <c r="C34" s="5">
-        <v>650</v>
-      </c>
-      <c r="D34" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E34">
-        <f t="shared" si="0"/>
-        <v>361.11111111111109</v>
-      </c>
-      <c r="F34">
-        <f t="shared" si="1"/>
-        <v>0.50154320987654322</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
-        <v>8</v>
-      </c>
-      <c r="B35">
-        <v>1080</v>
-      </c>
-      <c r="C35" s="5">
-        <v>975</v>
-      </c>
-      <c r="D35" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="0"/>
-        <v>541.66666666666663</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="1"/>
-        <v>0.50154320987654322</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+      <c r="B19">
+        <v>30500</v>
+      </c>
+      <c r="C19" s="5">
+        <v>7000</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="6"/>
+        <v>17500</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="7"/>
+        <v>0.57377049180327866</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2214,378 +2036,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:F16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5">
-        <v>385</v>
-      </c>
-      <c r="C2" s="5">
-        <v>237</v>
-      </c>
-      <c r="D2" s="5">
-        <f>B2*C2</f>
-        <v>91245</v>
-      </c>
-      <c r="E2" s="5">
-        <f>D2*E4/D4</f>
-        <v>21.676765097690943</v>
-      </c>
-      <c r="F2" s="6">
-        <f>F4*E2/E4</f>
-        <v>83060501.776198953</v>
-      </c>
-      <c r="G2" s="6">
-        <f>E2/F2*1000000</f>
-        <v>0.26097560975609752</v>
-      </c>
-      <c r="H2" s="5">
-        <f>SQRT(G2)</f>
-        <v>0.51085771967945981</v>
-      </c>
-      <c r="I2" s="5">
-        <f>2*H2</f>
-        <v>1.0217154393589196</v>
-      </c>
-      <c r="K2" s="7">
-        <v>35</v>
-      </c>
-      <c r="L2">
-        <v>1066</v>
-      </c>
-      <c r="M2">
-        <v>1.2</v>
-      </c>
-      <c r="N2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="7">
-        <v>800</v>
-      </c>
-      <c r="C4" s="7">
-        <v>563</v>
-      </c>
-      <c r="D4" s="7">
-        <f>B4*C4</f>
-        <v>450400</v>
-      </c>
-      <c r="E4" s="5">
-        <v>107</v>
-      </c>
-      <c r="F4" s="6">
-        <v>410000000</v>
-      </c>
-      <c r="G4" s="6">
-        <f>E4/F4*1000000</f>
-        <v>0.26097560975609757</v>
-      </c>
-      <c r="H4" s="5">
-        <f>SQRT(G4)</f>
-        <v>0.51085771967945981</v>
-      </c>
-      <c r="I4" s="5">
-        <f>2*H4</f>
-        <v>1.0217154393589196</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>160</v>
-      </c>
-      <c r="C8" s="5">
-        <v>144</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E8">
-        <f>C8/D8</f>
-        <v>80</v>
-      </c>
-      <c r="F8">
-        <f>E8/B8</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>160</v>
-      </c>
-      <c r="C9" s="5">
-        <v>144</v>
-      </c>
-      <c r="D9" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E9">
-        <f t="shared" ref="E9:E16" si="0">C9/D9</f>
-        <v>80</v>
-      </c>
-      <c r="F9">
-        <f t="shared" ref="F9:F16" si="1">E9/B9</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>160</v>
-      </c>
-      <c r="C10" s="5">
-        <v>144</v>
-      </c>
-      <c r="D10" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>4</v>
-      </c>
-      <c r="B11">
-        <v>250</v>
-      </c>
-      <c r="C11" s="5">
-        <v>216</v>
-      </c>
-      <c r="D11" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="1"/>
-        <v>0.48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>5</v>
-      </c>
-      <c r="B12">
-        <v>280</v>
-      </c>
-      <c r="C12" s="5">
-        <v>252</v>
-      </c>
-      <c r="D12" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>140</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>6</v>
-      </c>
-      <c r="B13">
-        <v>360</v>
-      </c>
-      <c r="C13" s="5">
-        <v>324</v>
-      </c>
-      <c r="D13" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>180</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>7</v>
-      </c>
-      <c r="B14">
-        <v>560</v>
-      </c>
-      <c r="C14" s="5">
-        <v>504</v>
-      </c>
-      <c r="D14" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>280</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>8</v>
-      </c>
-      <c r="B15">
-        <v>810</v>
-      </c>
-      <c r="C15" s="5">
-        <v>720</v>
-      </c>
-      <c r="D15" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="1"/>
-        <v>0.49382716049382713</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>9</v>
-      </c>
-      <c r="B16">
-        <v>30500</v>
-      </c>
-      <c r="C16" s="5">
-        <v>7000</v>
-      </c>
-      <c r="D16" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>17500</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="1"/>
-        <v>0.57377049180327866</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O24"/>
   <sheetViews>
@@ -2626,7 +2076,7 @@
         <v>19</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>27</v>
@@ -3126,7 +2576,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
@@ -3156,7 +2606,7 @@
         <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>27</v>
@@ -3510,7 +2960,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I18"/>
   <sheetViews>
@@ -3540,7 +2990,7 @@
         <v>19</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>27</v>
@@ -3620,7 +3070,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="4"/>
     </row>
@@ -3740,7 +3190,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I17"/>
   <sheetViews>
@@ -3770,7 +3220,7 @@
         <v>19</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>27</v>
@@ -3858,7 +3308,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="4"/>
     </row>
@@ -3971,7 +3421,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -3983,13 +3433,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
45nm test case + power comparison
Lowered wiring efficiency on lower levels to reflect patterning
challenges and power/gnd resource congestion
</commit_message>
<xml_diff>
--- a/data/processor_wla_validation.xlsx
+++ b/data/processor_wla_validation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="15120" windowHeight="7995" tabRatio="897" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="15120" windowHeight="7995" tabRatio="897" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="65nm Merom" sheetId="9" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="68">
   <si>
     <t>w (px)</t>
   </si>
@@ -213,6 +213,18 @@
   </si>
   <si>
     <t>misc2</t>
+  </si>
+  <si>
+    <t>2nd die</t>
+  </si>
+  <si>
+    <t>GPU</t>
+  </si>
+  <si>
+    <t>GPU area calculation</t>
+  </si>
+  <si>
+    <t>Atot (px^2)</t>
   </si>
 </sst>
 </file>
@@ -502,11 +514,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="125332480"/>
-        <c:axId val="125334656"/>
+        <c:axId val="144633216"/>
+        <c:axId val="144635392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="125332480"/>
+        <c:axId val="144633216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -530,19 +542,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125334656"/>
+        <c:crossAx val="144635392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125334656"/>
+        <c:axId val="144635392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -572,14 +583,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125332480"/>
+        <c:crossAx val="144633216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2113,8 +2123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2755,10 +2765,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3045,15 +3055,15 @@
         <v>62157972.30135534</v>
       </c>
       <c r="G10" s="6">
-        <f t="shared" ref="G10:G12" si="6">E10/F10*1000000</f>
+        <f t="shared" ref="G10:G14" si="6">E10/F10*1000000</f>
         <v>0.21204188481675393</v>
       </c>
       <c r="H10" s="5">
-        <f t="shared" ref="H10:H12" si="7">SQRT(G10)</f>
+        <f t="shared" ref="H10:H14" si="7">SQRT(G10)</f>
         <v>0.4604800590869858</v>
       </c>
       <c r="I10" s="5">
-        <f t="shared" ref="I10:I12" si="8">2*H10</f>
+        <f t="shared" ref="I10:I14" si="8">2*H10</f>
         <v>0.92096011817397161</v>
       </c>
       <c r="L10" s="5">
@@ -3184,6 +3194,37 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="5">
+        <v>379</v>
+      </c>
+      <c r="C13" s="5">
+        <v>512</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" ref="D13" si="10">D11+D12</f>
+        <v>125123</v>
+      </c>
+      <c r="E13">
+        <v>114</v>
+      </c>
+      <c r="F13" s="2">
+        <v>177000000</v>
+      </c>
+      <c r="G13" s="6">
+        <f t="shared" si="6"/>
+        <v>0.64406779661016944</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" si="7"/>
+        <v>0.8025383458814721</v>
+      </c>
+      <c r="I13" s="5">
+        <f t="shared" si="8"/>
+        <v>1.6050766917629442</v>
+      </c>
       <c r="L13" s="5">
         <v>7</v>
       </c>
@@ -3206,6 +3247,33 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14">
+        <f>F30</f>
+        <v>80429</v>
+      </c>
+      <c r="E14">
+        <f>D14/D13*E13</f>
+        <v>73.279141324936262</v>
+      </c>
+      <c r="F14" s="2">
+        <f>E14/E13*F13</f>
+        <v>113775508.89924315</v>
+      </c>
+      <c r="G14" s="6">
+        <f t="shared" si="6"/>
+        <v>0.64406779661016944</v>
+      </c>
+      <c r="H14" s="5">
+        <f t="shared" si="7"/>
+        <v>0.8025383458814721</v>
+      </c>
+      <c r="I14" s="5">
+        <f t="shared" si="8"/>
+        <v>1.6050766917629442</v>
+      </c>
       <c r="L14" s="5">
         <v>8</v>
       </c>
@@ -3368,8 +3436,94 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>59</v>
+      </c>
+      <c r="F25">
+        <f>D25*E25</f>
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>270</v>
+      </c>
+      <c r="E26">
+        <v>213</v>
+      </c>
+      <c r="F26">
+        <f t="shared" ref="F26:F29" si="11">D26*E26</f>
+        <v>57510</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>29</v>
+      </c>
+      <c r="E27">
+        <v>44</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="11"/>
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>103</v>
+      </c>
+      <c r="E28">
+        <v>179</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="11"/>
+        <v>18437</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>51</v>
+      </c>
+      <c r="E29">
+        <v>27</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="11"/>
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F30" s="1">
+        <f>SUM(F25:F29)</f>
+        <v>80429</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
WLATDRI with GNR updtes
</commit_message>
<xml_diff>
--- a/data/processor_wla_validation.xlsx
+++ b/data/processor_wla_validation.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wsw\Documents\GitHub\VirtualPlatform3D\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="15120" windowHeight="7995" tabRatio="897" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="15120" windowHeight="7995" tabRatio="897" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="65nm Merom" sheetId="9" r:id="rId1"/>
@@ -16,12 +21,13 @@
     <sheet name="22nm - Ivy Bridge EP10" sheetId="4" r:id="rId7"/>
     <sheet name="22nm Ivy Bridge (standard)" sheetId="5" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="69">
   <si>
     <t>w (px)</t>
   </si>
@@ -225,6 +231,9 @@
   </si>
   <si>
     <t>Atot (px^2)</t>
+  </si>
+  <si>
+    <t>Wfrac</t>
   </si>
 </sst>
 </file>
@@ -298,6 +307,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -514,11 +526,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="144633216"/>
-        <c:axId val="144635392"/>
+        <c:axId val="161706808"/>
+        <c:axId val="161711024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="144633216"/>
+        <c:axId val="161706808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -542,18 +554,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144635392"/>
+        <c:crossAx val="161711024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="144635392"/>
+        <c:axId val="161711024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -583,13 +596,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144633216"/>
+        <c:crossAx val="161706808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -703,7 +717,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -738,7 +752,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2767,8 +2781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3529,10 +3543,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:O12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3545,10 +3559,10 @@
     <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L1" s="3"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3585,8 +3599,14 @@
       <c r="O2" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -3632,8 +3652,16 @@
       <c r="O3" s="5">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3">
+        <f>N3/O3</f>
+        <v>55.882352941176471</v>
+      </c>
+      <c r="Q3">
+        <f>P3/M3</f>
+        <v>0.49673202614379086</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -3679,8 +3707,16 @@
       <c r="O4" s="5">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <f t="shared" ref="P4:P11" si="0">N4/O4</f>
+        <v>55.882352941176471</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" ref="Q4:Q11" si="1">P4/M4</f>
+        <v>0.49673202614379086</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3725,8 +3761,16 @@
       <c r="O5" s="5">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>55.882352941176471</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="1"/>
+        <v>0.49673202614379086</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L6" s="5">
         <v>4</v>
       </c>
@@ -3739,8 +3783,16 @@
       <c r="O6" s="5">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>83.888888888888886</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="1"/>
+        <v>0.49697209057398628</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -3775,8 +3827,16 @@
       <c r="O7" s="5">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>113.33333333333333</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="1"/>
+        <v>0.50370370370370365</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -3816,8 +3876,16 @@
       <c r="O8" s="5">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>168.33333333333334</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="1"/>
+        <v>0.4986176935229068</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -3847,8 +3915,16 @@
       <c r="O9" s="5">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>228.23529411764707</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="1"/>
+        <v>0.50707685873727404</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -3868,8 +3944,16 @@
       <c r="O10" s="5">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="1"/>
+        <v>0.49426301853486321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -3889,8 +3973,16 @@
       <c r="O11" s="5">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>5333.333333333333</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="1"/>
+        <v>0.274914089347079</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -3905,7 +3997,7 @@
       </c>
       <c r="O12" s="5"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F14" s="4" t="s">
         <v>25</v>
       </c>
@@ -3919,7 +4011,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="D15">
         <v>0.1125</v>
@@ -3937,7 +4029,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="3">
@@ -4070,15 +4162,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14:G22"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4104,7 +4196,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -4139,7 +4231,7 @@
         <v>0.93184854377882331</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -4170,7 +4262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -4203,7 +4295,7 @@
         <v>0.93184854377882331</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
@@ -4224,7 +4316,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -4253,7 +4345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -4268,7 +4360,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -4277,7 +4369,7 @@
         <v>1263367040</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -4286,12 +4378,12 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F13" s="4" t="s">
         <v>25</v>
       </c>
@@ -4304,8 +4396,35 @@
       <c r="I13" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L13" s="5">
+        <v>112.5</v>
+      </c>
+      <c r="M13" s="5">
+        <v>112.5</v>
+      </c>
+      <c r="N13" s="5">
+        <v>112.5</v>
+      </c>
+      <c r="O13" s="5">
+        <v>168.8</v>
+      </c>
+      <c r="P13" s="5">
+        <v>225</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>337.6</v>
+      </c>
+      <c r="R13" s="5">
+        <v>450.1</v>
+      </c>
+      <c r="S13" s="5">
+        <v>566.5</v>
+      </c>
+      <c r="T13" s="5">
+        <v>19400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="D14">
         <v>0.1125</v>
@@ -4323,7 +4442,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="3">
@@ -4343,7 +4462,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="D16">
         <v>0.42</v>
@@ -4458,7 +4577,7 @@
   <dimension ref="A2:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I17"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated processor data spreadsheet with SB info
</commit_message>
<xml_diff>
--- a/data/processor_wla_validation.xlsx
+++ b/data/processor_wla_validation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="15120" windowHeight="7995" tabRatio="897" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="15120" windowHeight="7995" tabRatio="897" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="65nm Merom" sheetId="9" r:id="rId1"/>
@@ -17,17 +17,17 @@
     <sheet name="45nm Nehalem" sheetId="8" r:id="rId3"/>
     <sheet name="32nm Nehalem" sheetId="10" r:id="rId4"/>
     <sheet name="Sandy Bridge EP-4 32nm Data" sheetId="3" r:id="rId5"/>
-    <sheet name="32nm Sandy Bridge (standard)" sheetId="6" r:id="rId6"/>
-    <sheet name="22nm - Ivy Bridge EP10" sheetId="4" r:id="rId7"/>
-    <sheet name="22nm Ivy Bridge (standard)" sheetId="5" r:id="rId8"/>
+    <sheet name="32nm SB Core i7 2700k" sheetId="11" r:id="rId6"/>
+    <sheet name="32nm Sandy Bridge (standard)" sheetId="6" r:id="rId7"/>
+    <sheet name="22nm - Ivy Bridge EP10" sheetId="4" r:id="rId8"/>
+    <sheet name="22nm Ivy Bridge (standard)" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="80">
   <si>
     <t>w (px)</t>
   </si>
@@ -234,6 +234,39 @@
   </si>
   <si>
     <t>Wfrac</t>
+  </si>
+  <si>
+    <t>Intel Core i7 2700k 32nm Sandy Bridge</t>
+  </si>
+  <si>
+    <t>High-level consumer-grade part</t>
+  </si>
+  <si>
+    <t>Gpu fmax (GHz)</t>
+  </si>
+  <si>
+    <t>20 Gb/s</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>w (mm)</t>
+  </si>
+  <si>
+    <t>h (mm)</t>
+  </si>
+  <si>
+    <t>mem io</t>
+  </si>
+  <si>
+    <t>sys agent</t>
+  </si>
+  <si>
+    <t>package</t>
+  </si>
+  <si>
+    <t>3.9 (Turbo)</t>
   </si>
 </sst>
 </file>
@@ -277,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -297,6 +330,15 @@
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -526,11 +568,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="161706808"/>
-        <c:axId val="161711024"/>
+        <c:axId val="261206376"/>
+        <c:axId val="261206760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="161706808"/>
+        <c:axId val="261206376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -561,12 +603,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161711024"/>
+        <c:crossAx val="261206760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="161711024"/>
+        <c:axId val="261206760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -603,7 +645,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161706808"/>
+        <c:crossAx val="261206376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2782,7 +2824,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="L2" sqref="L2:Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3545,8 +3587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4162,10 +4204,606 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="11" customWidth="1"/>
+    <col min="2" max="6" width="9.140625" style="5"/>
+    <col min="7" max="7" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" s="7">
+        <v>95</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N2" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="O2" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="P2" s="5">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>4</v>
+      </c>
+      <c r="R2" s="5">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1558</v>
+      </c>
+      <c r="C4" s="7">
+        <v>757</v>
+      </c>
+      <c r="D4" s="5">
+        <f>B4*C4</f>
+        <v>1179406</v>
+      </c>
+      <c r="E4" s="4">
+        <v>216</v>
+      </c>
+      <c r="F4" s="5">
+        <f>SQRT($E$4/$D$4)*B4</f>
+        <v>21.084468730903918</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" ref="G4" si="0">SQRT($E$4/$D$4)*C4</f>
+        <v>10.244507592615061</v>
+      </c>
+      <c r="H4" s="6">
+        <v>995000000</v>
+      </c>
+      <c r="I4" s="6">
+        <f>E4/H4*1000000</f>
+        <v>0.21708542713567841</v>
+      </c>
+      <c r="J4" s="5">
+        <f>SQRT(I4)</f>
+        <v>0.46592427188941166</v>
+      </c>
+      <c r="K4" s="5">
+        <f>2*J4</f>
+        <v>0.93184854377882331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5">
+        <v>244</v>
+      </c>
+      <c r="C5" s="5">
+        <v>418</v>
+      </c>
+      <c r="D5" s="5">
+        <f>B5*C5</f>
+        <v>101992</v>
+      </c>
+      <c r="E5" s="5">
+        <f>D5/$D$4*$E$4</f>
+        <v>18.679124915423525</v>
+      </c>
+      <c r="F5" s="5">
+        <f t="shared" ref="F5:F9" si="1">SQRT($E$4/$D$4)*B5</f>
+        <v>3.3020605714637714</v>
+      </c>
+      <c r="G5" s="5">
+        <f t="shared" ref="G5:G9" si="2">SQRT($E$4/$D$4)*C5</f>
+        <v>5.6568086839010512</v>
+      </c>
+      <c r="H5" s="6">
+        <f>E5/$E$4*$H$4</f>
+        <v>86045043.013177812</v>
+      </c>
+      <c r="I5" s="6">
+        <f>E5/H5*1000000</f>
+        <v>0.21708542713567841</v>
+      </c>
+      <c r="J5" s="5">
+        <f>SQRT(I5)</f>
+        <v>0.46592427188941166</v>
+      </c>
+      <c r="K5" s="5">
+        <f>2*J5</f>
+        <v>0.93184854377882331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5">
+        <v>978</v>
+      </c>
+      <c r="C6" s="5">
+        <v>257</v>
+      </c>
+      <c r="D6" s="5">
+        <f>B6*C6</f>
+        <v>251346</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" ref="E6:E9" si="3">D6/$D$4*$E$4</f>
+        <v>46.032270481920555</v>
+      </c>
+      <c r="F6" s="5">
+        <f t="shared" si="1"/>
+        <v>13.235308356112984</v>
+      </c>
+      <c r="G6" s="5">
+        <f t="shared" si="2"/>
+        <v>3.4779900281401197</v>
+      </c>
+      <c r="H6" s="5">
+        <f>I13</f>
+        <v>402653184</v>
+      </c>
+      <c r="I6" s="6">
+        <f>E6/H6*1000000</f>
+        <v>0.11432238042831559</v>
+      </c>
+      <c r="J6" s="5">
+        <f>SQRT(I6)</f>
+        <v>0.33811592749871394</v>
+      </c>
+      <c r="K6" s="5">
+        <f>SQRT(H13)*J6</f>
+        <v>0.82821149627972046</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="5">
+        <v>361</v>
+      </c>
+      <c r="C7" s="5">
+        <v>674</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" ref="D7:D9" si="4">B7*C7</f>
+        <v>243314</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="3"/>
+        <v>44.561265586235784</v>
+      </c>
+      <c r="F7" s="5">
+        <f t="shared" si="1"/>
+        <v>4.8854256815509078</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" si="2"/>
+        <v>9.1212656769122216</v>
+      </c>
+      <c r="H7" s="6">
+        <f>E7/$E$4*$H$4</f>
+        <v>205270644.71437317</v>
+      </c>
+      <c r="I7" s="6">
+        <f>E7/H7*1000000</f>
+        <v>0.21708542713567841</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" ref="J7:J9" si="5">SQRT(I7)</f>
+        <v>0.46592427188941166</v>
+      </c>
+      <c r="K7" s="5">
+        <f>2*J7</f>
+        <v>0.93184854377882331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="5">
+        <v>997</v>
+      </c>
+      <c r="C8" s="5">
+        <v>86</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="4"/>
+        <v>85742</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="3"/>
+        <v>15.703050518650915</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="1"/>
+        <v>13.492436023563032</v>
+      </c>
+      <c r="G8" s="5">
+        <f t="shared" si="2"/>
+        <v>1.1638410210896899</v>
+      </c>
+      <c r="H8" s="6">
+        <f t="shared" ref="H8" si="6">E8/$E$4*$H$4</f>
+        <v>72335811.416933611</v>
+      </c>
+      <c r="I8" s="6">
+        <f t="shared" ref="I8" si="7">E8/H8*1000000</f>
+        <v>0.21708542713567841</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" si="5"/>
+        <v>0.46592427188941166</v>
+      </c>
+      <c r="K8" s="5">
+        <f t="shared" ref="K8:K9" si="8">2*J8</f>
+        <v>0.93184854377882331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="5">
+        <v>222</v>
+      </c>
+      <c r="C9" s="5">
+        <v>673</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="4"/>
+        <v>149406</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="3"/>
+        <v>27.362669004566705</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="1"/>
+        <v>3.0043337986268739</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="2"/>
+        <v>9.1077326417832705</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" ref="H9" si="9">E9/$E$4*$H$4</f>
+        <v>126045628.05344385</v>
+      </c>
+      <c r="I9" s="6">
+        <f t="shared" ref="I9" si="10">E9/H9*1000000</f>
+        <v>0.21708542713567841</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="5"/>
+        <v>0.46592427188941166</v>
+      </c>
+      <c r="K9" s="5">
+        <f t="shared" si="8"/>
+        <v>0.93184854377882331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="5">
+        <v>37.5</v>
+      </c>
+      <c r="G10" s="5">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1160000000</v>
+      </c>
+      <c r="C13" s="5">
+        <f>E4</f>
+        <v>216</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="5">
+        <v>8</v>
+      </c>
+      <c r="G13" s="5">
+        <f>F13*POWER(2,20)*8</f>
+        <v>67108864</v>
+      </c>
+      <c r="H13" s="5">
+        <v>6</v>
+      </c>
+      <c r="I13" s="5">
+        <f>H13*G13</f>
+        <v>402653184</v>
+      </c>
+      <c r="J13" s="5">
+        <f>E6/I13*1000000</f>
+        <v>0.11432238042831559</v>
+      </c>
+      <c r="K13" s="5">
+        <f>J13*H13</f>
+        <v>0.68593428256989353</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="5">
+        <f>I13</f>
+        <v>402653184</v>
+      </c>
+      <c r="C14" s="5">
+        <f>E6</f>
+        <v>46.032270481920555</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="6">
+        <f>H5</f>
+        <v>86045043.013177812</v>
+      </c>
+      <c r="C15" s="5">
+        <f>E5</f>
+        <v>18.679124915423525</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="6">
+        <f>H7</f>
+        <v>205270644.71437317</v>
+      </c>
+      <c r="C16" s="5">
+        <f>E7</f>
+        <v>44.561265586235784</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="F20" s="5">
+        <v>1</v>
+      </c>
+      <c r="G20" s="5">
+        <v>112.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="5">
+        <v>2</v>
+      </c>
+      <c r="G21" s="5">
+        <v>112.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="F22" s="5">
+        <v>3</v>
+      </c>
+      <c r="G22" s="5">
+        <v>112.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F23" s="5">
+        <v>4</v>
+      </c>
+      <c r="G23" s="5">
+        <v>168.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F24" s="5">
+        <v>5</v>
+      </c>
+      <c r="G24" s="5">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F25" s="5">
+        <v>6</v>
+      </c>
+      <c r="G25" s="5">
+        <v>337.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F26" s="5">
+        <v>7</v>
+      </c>
+      <c r="G26" s="5">
+        <v>450.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F27" s="5">
+        <v>8</v>
+      </c>
+      <c r="G27" s="5">
+        <v>566.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F28" s="5">
+        <v>9</v>
+      </c>
+      <c r="G28" s="5">
+        <v>19400</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F29" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="6">
+        <v>145900</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4572,7 +5210,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I18"/>
   <sheetViews>
@@ -4802,7 +5440,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I17"/>
   <sheetViews>

</xml_diff>

<commit_message>
Alternate penryn data added to cpu validation spreadsheet
</commit_message>
<xml_diff>
--- a/data/processor_wla_validation.xlsx
+++ b/data/processor_wla_validation.xlsx
@@ -9,25 +9,26 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="15120" windowHeight="7995" tabRatio="897" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="15120" windowHeight="7995" tabRatio="897" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="65nm Merom" sheetId="9" r:id="rId1"/>
     <sheet name="45nm Penryn" sheetId="7" r:id="rId2"/>
-    <sheet name="45nm Nehalem" sheetId="8" r:id="rId3"/>
-    <sheet name="32nm Nehalem" sheetId="10" r:id="rId4"/>
-    <sheet name="Sandy Bridge EP-4 32nm Data" sheetId="3" r:id="rId5"/>
-    <sheet name="32nm SB Core i7 2700k" sheetId="11" r:id="rId6"/>
-    <sheet name="32nm Sandy Bridge (standard)" sheetId="6" r:id="rId7"/>
-    <sheet name="22nm - Ivy Bridge EP10" sheetId="4" r:id="rId8"/>
-    <sheet name="22nm Ivy Bridge (standard)" sheetId="5" r:id="rId9"/>
+    <sheet name="45nm Penryn 2" sheetId="12" r:id="rId3"/>
+    <sheet name="45nm Nehalem" sheetId="8" r:id="rId4"/>
+    <sheet name="32nm Nehalem" sheetId="10" r:id="rId5"/>
+    <sheet name="Sandy Bridge EP-4 32nm Data" sheetId="3" r:id="rId6"/>
+    <sheet name="32nm SB Core i7 2700k" sheetId="11" r:id="rId7"/>
+    <sheet name="32nm Sandy Bridge (standard)" sheetId="6" r:id="rId8"/>
+    <sheet name="22nm - Ivy Bridge EP10" sheetId="4" r:id="rId9"/>
+    <sheet name="22nm Ivy Bridge (standard)" sheetId="5" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="81">
   <si>
     <t>w (px)</t>
   </si>
@@ -267,6 +268,9 @@
   </si>
   <si>
     <t>3.9 (Turbo)</t>
+  </si>
+  <si>
+    <t>45nm_penryn_die.jpg</t>
   </si>
 </sst>
 </file>
@@ -568,11 +572,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="261206376"/>
-        <c:axId val="261206760"/>
+        <c:axId val="369096088"/>
+        <c:axId val="369096472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="261206376"/>
+        <c:axId val="369096088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -596,19 +600,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261206760"/>
+        <c:crossAx val="369096472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="261206760"/>
+        <c:axId val="369096472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -638,14 +641,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261206376"/>
+        <c:crossAx val="369096088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1674,18 +1676,250 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>136</v>
+      </c>
+      <c r="C3">
+        <v>238</v>
+      </c>
+      <c r="D3">
+        <f>B3*C3</f>
+        <v>32368</v>
+      </c>
+      <c r="E3">
+        <f>D3*E5/D5</f>
+        <v>11.951408632721634</v>
+      </c>
+      <c r="F3" s="2">
+        <f>F5*E3/E5</f>
+        <v>104574825.53631429</v>
+      </c>
+      <c r="G3" s="2">
+        <f>E3/F3*1000000</f>
+        <v>0.11428571428571428</v>
+      </c>
+      <c r="H3">
+        <f>SQRT(G3)</f>
+        <v>0.33806170189140661</v>
+      </c>
+      <c r="I3">
+        <f>2*H3</f>
+        <v>0.67612340378281321</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1022</v>
+      </c>
+      <c r="C5" s="3">
+        <v>424</v>
+      </c>
+      <c r="D5" s="3">
+        <f>B5*C5</f>
+        <v>433328</v>
+      </c>
+      <c r="E5">
+        <v>160</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1400000000</v>
+      </c>
+      <c r="G5" s="2">
+        <f>E5/F5*1000000</f>
+        <v>0.11428571428571428</v>
+      </c>
+      <c r="H5">
+        <f>SQRT(G5)</f>
+        <v>0.33806170189140661</v>
+      </c>
+      <c r="I5">
+        <f>2*H5</f>
+        <v>0.67612340378281321</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>90</v>
+      </c>
+      <c r="C9" s="5">
+        <v>90</v>
+      </c>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>80</v>
+      </c>
+      <c r="C10" s="5">
+        <v>90</v>
+      </c>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>80</v>
+      </c>
+      <c r="C11" s="5">
+        <v>90</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>112</v>
+      </c>
+      <c r="C12" s="5">
+        <v>115.836</v>
+      </c>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>160</v>
+      </c>
+      <c r="C13" s="5">
+        <v>210.5411</v>
+      </c>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>240</v>
+      </c>
+      <c r="C14" s="5">
+        <v>322.54140000000001</v>
+      </c>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>320</v>
+      </c>
+      <c r="C15" s="5">
+        <v>493.471</v>
+      </c>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>360</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>14000</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
@@ -1701,6 +1935,46 @@
         <v>47</v>
       </c>
     </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M3" s="7">
+        <v>65</v>
+      </c>
+      <c r="N3" s="5">
+        <v>1333</v>
+      </c>
+      <c r="O3" s="5">
+        <v>1.3625</v>
+      </c>
+      <c r="P3" s="5">
+        <v>3.3</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>6</v>
+      </c>
+      <c r="R3" s="5">
+        <v>2</v>
+      </c>
+    </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>0</v>
@@ -1715,34 +1989,22 @@
         <v>5</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1763,42 +2025,32 @@
         <f>D5*E7/D7</f>
         <v>21.676765097690943</v>
       </c>
-      <c r="F5" s="6">
-        <f>F7*E5/E7</f>
+      <c r="F5">
+        <f>B5*SQRT($E$5/$D$5)</f>
+        <v>5.9340804166074266</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G8" si="0">C5*SQRT($E$5/$D$5)</f>
+        <v>3.6529274252882082</v>
+      </c>
+      <c r="H5" s="6">
+        <f>H7*E5/E7</f>
         <v>83060501.776198953</v>
       </c>
-      <c r="G5" s="6">
-        <f>E5/F5*1000000</f>
+      <c r="I5" s="6">
+        <f>E5/H5*1000000</f>
         <v>0.26097560975609752</v>
       </c>
-      <c r="H5" s="5">
-        <f>SQRT(G5)</f>
+      <c r="J5" s="5">
+        <f>SQRT(I5)</f>
         <v>0.51085771967945981</v>
       </c>
-      <c r="I5" s="5">
-        <f>2*H5</f>
+      <c r="K5" s="5">
+        <f>2*J5</f>
         <v>1.0217154393589196</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>48</v>
-      </c>
-      <c r="M5" s="7">
-        <v>65</v>
-      </c>
-      <c r="N5" s="5">
-        <v>1333</v>
-      </c>
-      <c r="O5" s="5">
-        <v>1.3625</v>
-      </c>
-      <c r="P5" s="5">
-        <v>3.3</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>6</v>
-      </c>
-      <c r="R5" s="5">
-        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1812,30 +2064,37 @@
         <v>512</v>
       </c>
       <c r="D6" s="5">
-        <f t="shared" ref="D6" si="0">B6*C6</f>
+        <f t="shared" ref="D6" si="1">B6*C6</f>
         <v>261632</v>
       </c>
       <c r="E6" s="5">
         <f>D6/D7*E7</f>
         <v>62.155026642984019</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6">
+        <f t="shared" ref="F6:F8" si="2">B6*SQRT($E$5/$D$5)</f>
+        <v>7.8761430984062208</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>7.8915562942935127</v>
+      </c>
+      <c r="H6" s="5">
         <f>P11</f>
         <v>301989888</v>
       </c>
-      <c r="G6" s="6">
-        <f t="shared" ref="G6" si="1">E6/F6*1000000</f>
+      <c r="I6" s="6">
+        <f>E6/H6*1000000</f>
         <v>0.20581823800333349</v>
       </c>
-      <c r="H6" s="5">
-        <f t="shared" ref="H6" si="2">SQRT(G6)</f>
+      <c r="J6" s="5">
+        <f t="shared" ref="J6" si="3">SQRT(I6)</f>
         <v>0.45367194976473196</v>
       </c>
-      <c r="I6" s="5">
-        <f>SQRT(6)*H6</f>
+      <c r="K6" s="5">
+        <f>SQRT(6)*J6</f>
         <v>1.1112647875371562</v>
       </c>
-      <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1854,19 +2113,27 @@
       <c r="E7" s="5">
         <v>107</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>12.330556709833614</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>8.6776292845454055</v>
+      </c>
+      <c r="H7" s="6">
         <v>410000000</v>
       </c>
-      <c r="G7" s="6">
-        <f>E7/F7*1000000</f>
+      <c r="I7" s="6">
+        <f>E7/H7*1000000</f>
         <v>0.26097560975609757</v>
       </c>
-      <c r="H7" s="5">
-        <f>SQRT(G7)</f>
+      <c r="J7" s="5">
+        <f>SQRT(I7)</f>
         <v>0.51085771967945981</v>
       </c>
-      <c r="I7" s="5">
-        <f>2*H7</f>
+      <c r="K7" s="5">
+        <f>2*J7</f>
         <v>1.0217154393589196</v>
       </c>
     </row>
@@ -1888,45 +2155,35 @@
         <f>D8*E7/D7</f>
         <v>21.676765097690943</v>
       </c>
-      <c r="F8" s="2">
-        <f>0.9/2*(F7-F6)</f>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>5.9340804166074266</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>3.6529274252882082</v>
+      </c>
+      <c r="H8" s="2">
+        <f>0.9/2*(H7-H6)</f>
         <v>48604550.399999999</v>
       </c>
-      <c r="G8" s="6">
-        <f t="shared" ref="G8" si="3">E8/F8*1000000</f>
+      <c r="I8" s="6">
+        <f>E8/H8*1000000</f>
         <v>0.44598221605380683</v>
       </c>
-      <c r="H8" s="5">
-        <f t="shared" ref="H8" si="4">SQRT(G8)</f>
+      <c r="J8" s="5">
+        <f t="shared" ref="J8" si="4">SQRT(I8)</f>
         <v>0.66781899947052037</v>
       </c>
-      <c r="I8" s="5">
-        <f t="shared" ref="I8" si="5">2*H8</f>
+      <c r="K8" s="5">
+        <f t="shared" ref="K8" si="5">2*J8</f>
         <v>1.3356379989410407</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="M10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1947,26 +2204,6 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>160</v>
-      </c>
-      <c r="C11" s="5">
-        <v>144</v>
-      </c>
-      <c r="D11" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="E11">
-        <f>C11/D11</f>
-        <v>80</v>
-      </c>
-      <c r="F11">
-        <f>E11/B11</f>
-        <v>0.5</v>
-      </c>
       <c r="L11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1993,178 +2230,220 @@
         <v>1.1112647875371562</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>160</v>
+      </c>
+      <c r="C16" s="5">
+        <v>144</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E16">
+        <f>C16/D16</f>
+        <v>80</v>
+      </c>
+      <c r="F16">
+        <f>E16/B16</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
         <v>2</v>
       </c>
-      <c r="B12">
+      <c r="B17">
         <v>160</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C17" s="5">
         <v>144</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D17" s="5">
         <v>1.8</v>
       </c>
-      <c r="E12">
-        <f t="shared" ref="E12:E19" si="6">C12/D12</f>
+      <c r="E17">
+        <f t="shared" ref="E17:E24" si="6">C17/D17</f>
         <v>80</v>
       </c>
-      <c r="F12">
-        <f t="shared" ref="F12:F19" si="7">E12/B12</f>
+      <c r="F17">
+        <f t="shared" ref="F17:F24" si="7">E17/B17</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
         <v>3</v>
       </c>
-      <c r="B13">
+      <c r="B18">
         <v>160</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C18" s="5">
         <v>144</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D18" s="5">
         <v>1.8</v>
       </c>
-      <c r="E13">
+      <c r="E18">
         <f t="shared" si="6"/>
         <v>80</v>
       </c>
-      <c r="F13">
+      <c r="F18">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
         <v>4</v>
       </c>
-      <c r="B14">
+      <c r="B19">
         <v>250</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C19" s="5">
         <v>216</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D19" s="5">
         <v>1.8</v>
       </c>
-      <c r="E14">
+      <c r="E19">
         <f t="shared" si="6"/>
         <v>120</v>
       </c>
-      <c r="F14">
+      <c r="F19">
         <f t="shared" si="7"/>
         <v>0.48</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
         <v>5</v>
       </c>
-      <c r="B15">
+      <c r="B20">
         <v>280</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C20" s="5">
         <v>252</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D20" s="5">
         <v>1.8</v>
       </c>
-      <c r="E15">
+      <c r="E20">
         <f t="shared" si="6"/>
         <v>140</v>
       </c>
-      <c r="F15">
+      <c r="F20">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
         <v>6</v>
       </c>
-      <c r="B16">
+      <c r="B21">
         <v>360</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C21" s="5">
         <v>324</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D21" s="5">
         <v>1.8</v>
       </c>
-      <c r="E16">
+      <c r="E21">
         <f t="shared" si="6"/>
         <v>180</v>
       </c>
-      <c r="F16">
+      <c r="F21">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
         <v>7</v>
       </c>
-      <c r="B17">
+      <c r="B22">
         <v>560</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C22" s="5">
         <v>504</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D22" s="5">
         <v>1.8</v>
       </c>
-      <c r="E17">
+      <c r="E22">
         <f t="shared" si="6"/>
         <v>280</v>
       </c>
-      <c r="F17">
+      <c r="F22">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
         <v>8</v>
       </c>
-      <c r="B18">
+      <c r="B23">
         <v>810</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C23" s="5">
         <v>720</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D23" s="5">
         <v>1.8</v>
       </c>
-      <c r="E18">
+      <c r="E23">
         <f t="shared" si="6"/>
         <v>400</v>
       </c>
-      <c r="F18">
+      <c r="F23">
         <f t="shared" si="7"/>
         <v>0.49382716049382713</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
         <v>9</v>
       </c>
-      <c r="B19">
+      <c r="B24">
         <v>30500</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C24" s="5">
         <v>7000</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D24" s="5">
         <v>0.4</v>
       </c>
-      <c r="E19">
+      <c r="E24">
         <f t="shared" si="6"/>
         <v>17500</v>
       </c>
-      <c r="F19">
+      <c r="F24">
         <f t="shared" si="7"/>
         <v>0.57377049180327866</v>
       </c>
@@ -2176,6 +2455,555 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M3" s="7">
+        <v>65</v>
+      </c>
+      <c r="N3" s="5">
+        <v>1333</v>
+      </c>
+      <c r="O3" s="5">
+        <v>1.3625</v>
+      </c>
+      <c r="P3" s="5">
+        <v>3.3</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>6</v>
+      </c>
+      <c r="R3" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5">
+        <v>500</v>
+      </c>
+      <c r="C5" s="5">
+        <v>310</v>
+      </c>
+      <c r="D5" s="5">
+        <f>B5*C5</f>
+        <v>155000</v>
+      </c>
+      <c r="E5" s="5">
+        <f>D5*E7/D7</f>
+        <v>22.588966614365411</v>
+      </c>
+      <c r="F5">
+        <f>B5*SQRT($E$5/$D$5)</f>
+        <v>6.0360431675017212</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G8" si="0">C5*SQRT($E$5/$D$5)</f>
+        <v>3.7423467638510672</v>
+      </c>
+      <c r="H5" s="6">
+        <f>H7*E5/E7</f>
+        <v>86555853.382147834</v>
+      </c>
+      <c r="I5" s="6">
+        <f>E5/H5*1000000</f>
+        <v>0.26097560975609757</v>
+      </c>
+      <c r="J5" s="5">
+        <f>SQRT(I5)</f>
+        <v>0.51085771967945981</v>
+      </c>
+      <c r="K5" s="5">
+        <f>2*J5</f>
+        <v>1.0217154393589196</v>
+      </c>
+      <c r="L5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5">
+        <v>511</v>
+      </c>
+      <c r="C6" s="5">
+        <v>514</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" ref="D6" si="1">B6*C6</f>
+        <v>262654</v>
+      </c>
+      <c r="E6" s="5">
+        <f>D6/D7*E7</f>
+        <v>38.277951207287309</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F8" si="2">B6*SQRT($E$5/$D$5)</f>
+        <v>6.1688361171867596</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>6.2050523761917695</v>
+      </c>
+      <c r="H6" s="5">
+        <f>P11</f>
+        <v>301989888</v>
+      </c>
+      <c r="I6" s="6">
+        <f>E6/H6*1000000</f>
+        <v>0.12675242691333857</v>
+      </c>
+      <c r="J6" s="5">
+        <f t="shared" ref="J6" si="3">SQRT(I6)</f>
+        <v>0.35602307075994188</v>
+      </c>
+      <c r="K6" s="5">
+        <f>SQRT(6)*J6</f>
+        <v>0.87207486002064716</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7">
+        <v>1024</v>
+      </c>
+      <c r="C7" s="7">
+        <v>717</v>
+      </c>
+      <c r="D7" s="7">
+        <f>B7*C7</f>
+        <v>734208</v>
+      </c>
+      <c r="E7" s="5">
+        <v>107</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>12.361816407043525</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>8.6556859021974688</v>
+      </c>
+      <c r="H7" s="6">
+        <v>410000000</v>
+      </c>
+      <c r="I7" s="6">
+        <f>E7/H7*1000000</f>
+        <v>0.26097560975609757</v>
+      </c>
+      <c r="J7" s="5">
+        <f>SQRT(I7)</f>
+        <v>0.51085771967945981</v>
+      </c>
+      <c r="K7" s="5">
+        <f>2*J7</f>
+        <v>1.0217154393589196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5">
+        <v>500</v>
+      </c>
+      <c r="C8" s="5">
+        <v>310</v>
+      </c>
+      <c r="D8" s="5">
+        <f>B8*C8</f>
+        <v>155000</v>
+      </c>
+      <c r="E8" s="5">
+        <f>D8*E7/D7</f>
+        <v>22.588966614365411</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>6.0360431675017212</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>3.7423467638510672</v>
+      </c>
+      <c r="H8" s="2">
+        <f>0.9/2*(H7-H6)</f>
+        <v>48604550.399999999</v>
+      </c>
+      <c r="I8" s="6">
+        <f>E8/H8*1000000</f>
+        <v>0.46475003736204523</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" ref="J8" si="4">SQRT(I8)</f>
+        <v>0.68172577871314599</v>
+      </c>
+      <c r="K8" s="5">
+        <f t="shared" ref="K8" si="5">2*J8</f>
+        <v>1.363451557426292</v>
+      </c>
+      <c r="L8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11">
+        <v>6</v>
+      </c>
+      <c r="N11">
+        <f>M11*POWER(2,20)*8</f>
+        <v>50331648</v>
+      </c>
+      <c r="O11">
+        <v>6</v>
+      </c>
+      <c r="P11">
+        <f>O11*N11</f>
+        <v>301989888</v>
+      </c>
+      <c r="Q11">
+        <f>E6/N11*1000000</f>
+        <v>0.7605145614800316</v>
+      </c>
+      <c r="R11">
+        <f>SQRT(Q11)</f>
+        <v>0.87207486002064727</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>160</v>
+      </c>
+      <c r="C16" s="5">
+        <v>144</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E16">
+        <f>C16/D16</f>
+        <v>80</v>
+      </c>
+      <c r="F16">
+        <f>E16/B16</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>160</v>
+      </c>
+      <c r="C17" s="5">
+        <v>144</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ref="E17:E24" si="6">C17/D17</f>
+        <v>80</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ref="F17:F24" si="7">E17/B17</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>160</v>
+      </c>
+      <c r="C18" s="5">
+        <v>144</v>
+      </c>
+      <c r="D18" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="6"/>
+        <v>80</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>250</v>
+      </c>
+      <c r="C19" s="5">
+        <v>216</v>
+      </c>
+      <c r="D19" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="6"/>
+        <v>120</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="7"/>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>280</v>
+      </c>
+      <c r="C20" s="5">
+        <v>252</v>
+      </c>
+      <c r="D20" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="6"/>
+        <v>140</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>360</v>
+      </c>
+      <c r="C21" s="5">
+        <v>324</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="6"/>
+        <v>180</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>560</v>
+      </c>
+      <c r="C22" s="5">
+        <v>504</v>
+      </c>
+      <c r="D22" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="6"/>
+        <v>280</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>810</v>
+      </c>
+      <c r="C23" s="5">
+        <v>720</v>
+      </c>
+      <c r="D23" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="6"/>
+        <v>400</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="7"/>
+        <v>0.49382716049382713</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <v>30500</v>
+      </c>
+      <c r="C24" s="5">
+        <v>7000</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="6"/>
+        <v>17500</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="7"/>
+        <v>0.57377049180327866</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q28"/>
   <sheetViews>
@@ -2819,7 +3647,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q30"/>
   <sheetViews>
@@ -3583,7 +4411,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q24"/>
   <sheetViews>
@@ -4202,11 +5030,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -4798,7 +5626,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T23"/>
   <sheetViews>
@@ -5210,7 +6038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I18"/>
   <sheetViews>
@@ -5438,235 +6266,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>136</v>
-      </c>
-      <c r="C3">
-        <v>238</v>
-      </c>
-      <c r="D3">
-        <f>B3*C3</f>
-        <v>32368</v>
-      </c>
-      <c r="E3">
-        <f>D3*E5/D5</f>
-        <v>11.951408632721634</v>
-      </c>
-      <c r="F3" s="2">
-        <f>F5*E3/E5</f>
-        <v>104574825.53631429</v>
-      </c>
-      <c r="G3" s="2">
-        <f>E3/F3*1000000</f>
-        <v>0.11428571428571428</v>
-      </c>
-      <c r="H3">
-        <f>SQRT(G3)</f>
-        <v>0.33806170189140661</v>
-      </c>
-      <c r="I3">
-        <f>2*H3</f>
-        <v>0.67612340378281321</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1022</v>
-      </c>
-      <c r="C5" s="3">
-        <v>424</v>
-      </c>
-      <c r="D5" s="3">
-        <f>B5*C5</f>
-        <v>433328</v>
-      </c>
-      <c r="E5">
-        <v>160</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1400000000</v>
-      </c>
-      <c r="G5" s="2">
-        <f>E5/F5*1000000</f>
-        <v>0.11428571428571428</v>
-      </c>
-      <c r="H5">
-        <f>SQRT(G5)</f>
-        <v>0.33806170189140661</v>
-      </c>
-      <c r="I5">
-        <f>2*H5</f>
-        <v>0.67612340378281321</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <v>90</v>
-      </c>
-      <c r="C9" s="5">
-        <v>90</v>
-      </c>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>80</v>
-      </c>
-      <c r="C10" s="5">
-        <v>90</v>
-      </c>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>3</v>
-      </c>
-      <c r="B11">
-        <v>80</v>
-      </c>
-      <c r="C11" s="5">
-        <v>90</v>
-      </c>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>4</v>
-      </c>
-      <c r="B12">
-        <v>112</v>
-      </c>
-      <c r="C12" s="5">
-        <v>115.836</v>
-      </c>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>5</v>
-      </c>
-      <c r="B13">
-        <v>160</v>
-      </c>
-      <c r="C13" s="5">
-        <v>210.5411</v>
-      </c>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>6</v>
-      </c>
-      <c r="B14">
-        <v>240</v>
-      </c>
-      <c r="C14" s="5">
-        <v>322.54140000000001</v>
-      </c>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>7</v>
-      </c>
-      <c r="B15">
-        <v>320</v>
-      </c>
-      <c r="C15" s="5">
-        <v>493.471</v>
-      </c>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>8</v>
-      </c>
-      <c r="B16">
-        <v>360</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>9</v>
-      </c>
-      <c r="B17">
-        <v>14000</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added power comparison data and some block sizes to cpu validation spreadsheet
</commit_message>
<xml_diff>
--- a/data/processor_wla_validation.xlsx
+++ b/data/processor_wla_validation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="15120" windowHeight="7995" tabRatio="897" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="15120" windowHeight="7995" tabRatio="897" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="65nm Merom" sheetId="9" r:id="rId1"/>
@@ -22,13 +22,14 @@
     <sheet name="32nm Sandy Bridge (standard)" sheetId="6" r:id="rId8"/>
     <sheet name="22nm - Ivy Bridge EP10" sheetId="4" r:id="rId9"/>
     <sheet name="22nm Ivy Bridge (standard)" sheetId="5" r:id="rId10"/>
+    <sheet name="Power data" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="98">
   <si>
     <t>w (px)</t>
   </si>
@@ -271,6 +272,57 @@
   </si>
   <si>
     <t>45nm_penryn_die.jpg</t>
+  </si>
+  <si>
+    <t>h(mm)</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>before top</t>
+  </si>
+  <si>
+    <t>big middle</t>
+  </si>
+  <si>
+    <t>leftest</t>
+  </si>
+  <si>
+    <t>rightest</t>
+  </si>
+  <si>
+    <t>Simulated</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Actual TDP</t>
+  </si>
+  <si>
+    <t>Penryn</t>
+  </si>
+  <si>
+    <t>Merom</t>
+  </si>
+  <si>
+    <t>45nm</t>
+  </si>
+  <si>
+    <t>Nehalem</t>
+  </si>
+  <si>
+    <t>32nm</t>
+  </si>
+  <si>
+    <t>Sandy Bridge</t>
+  </si>
+  <si>
+    <t>pcie_con</t>
   </si>
 </sst>
 </file>
@@ -572,11 +624,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="369096088"/>
-        <c:axId val="369096472"/>
+        <c:axId val="229747896"/>
+        <c:axId val="229761976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="369096088"/>
+        <c:axId val="229747896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -600,18 +652,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="369096472"/>
+        <c:crossAx val="229761976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="369096472"/>
+        <c:axId val="229761976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -641,13 +694,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="369096088"/>
+        <c:crossAx val="229747896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1008,7 +1062,7 @@
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,15 +1150,21 @@
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L6" s="5"/>
@@ -1132,19 +1192,27 @@
         <v>56.323326550365437</v>
       </c>
       <c r="F7">
+        <f>B7*SQRT($E$7/$D$7)</f>
+        <v>6.1563711029997279</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7:G8" si="0">C7*SQRT($E$7/$D$7)</f>
+        <v>9.1487867784516084</v>
+      </c>
+      <c r="H7">
         <f>H11</f>
         <v>201326592</v>
       </c>
-      <c r="G7">
-        <f>E7/F7*1000000</f>
+      <c r="I7">
+        <f>E7/H7*1000000</f>
         <v>0.27976098930023829</v>
       </c>
-      <c r="H7">
-        <f>SQRT(G7)</f>
+      <c r="J7">
+        <f>SQRT(I7)</f>
         <v>0.52892437011376048</v>
       </c>
-      <c r="I7">
-        <f>SQRT(6)*H7</f>
+      <c r="K7">
+        <f>SQRT(6)*J7</f>
         <v>1.2955948193017095</v>
       </c>
       <c r="L7" s="5"/>
@@ -1170,19 +1238,27 @@
       <c r="E8" s="1">
         <v>143</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8">
+        <f t="shared" ref="F8" si="1">B8*SQRT($E$7/$D$7)</f>
+        <v>13.666000250312088</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>10.463924877854026</v>
+      </c>
+      <c r="H8" s="8">
         <v>291000000</v>
       </c>
-      <c r="G8" s="2">
-        <f>E8/F8*1000000</f>
+      <c r="I8" s="2">
+        <f>E8/H8*1000000</f>
         <v>0.49140893470790376</v>
       </c>
-      <c r="H8">
-        <f>SQRT(G8)</f>
+      <c r="J8">
+        <f>SQRT(I8)</f>
         <v>0.70100565954056593</v>
       </c>
-      <c r="I8">
-        <f>2*H8</f>
+      <c r="K8">
+        <f>2*J8</f>
         <v>1.4020113190811319</v>
       </c>
       <c r="L8" s="5"/>
@@ -1316,12 +1392,12 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>0</v>
       </c>
@@ -1338,19 +1414,25 @@
         <v>17</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1361,35 +1443,43 @@
         <v>261</v>
       </c>
       <c r="D20">
-        <f t="shared" ref="D20:D25" si="0">B20*C20</f>
+        <f>B20*C20</f>
         <v>21663</v>
       </c>
       <c r="E20">
-        <f t="shared" ref="E20:E25" si="1">D20/$D$8*$E$8</f>
+        <f>D20/$D$8*$E$8</f>
         <v>7.8697898804216111</v>
       </c>
       <c r="F20">
         <f>SUM(E20:E25)</f>
         <v>29.45276945784525</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20">
+        <f>B20*SQRT($E$7/$D$7)</f>
+        <v>1.5819777137739237</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ref="H20:H25" si="2">C20*SQRT($E$7/$D$7)</f>
+        <v>4.9746528107830619</v>
+      </c>
+      <c r="I20" s="2">
         <f>B14</f>
         <v>40353033.600000001</v>
       </c>
-      <c r="H20" s="2">
-        <f>F20/G20*1000000</f>
+      <c r="J20" s="2">
+        <f>F20/I20*1000000</f>
         <v>0.7298774548103677</v>
       </c>
-      <c r="I20">
-        <f>SQRT(H20)</f>
+      <c r="K20">
+        <f>SQRT(J20)</f>
         <v>0.85432865737394514</v>
       </c>
-      <c r="J20">
-        <f>2*I20</f>
+      <c r="L20">
+        <f>2*K20</f>
         <v>1.7086573147478903</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>102</v>
       </c>
@@ -1397,15 +1487,23 @@
         <v>239</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
+        <f>B21*C21</f>
         <v>24378</v>
       </c>
       <c r="E21">
-        <f t="shared" si="1"/>
+        <f>D21/$D$8*$E$8</f>
         <v>8.8561020036429881</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <f t="shared" ref="G21:G25" si="3">B21*SQRT($E$7/$D$7)</f>
+        <v>1.9441171904209666</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>4.5553334167706963</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>74</v>
       </c>
@@ -1413,15 +1511,23 @@
         <v>223</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f>B22*C22</f>
         <v>16502</v>
       </c>
       <c r="E22">
-        <f t="shared" si="1"/>
+        <f>D22/$D$8*$E$8</f>
         <v>5.9948886399260219</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <f t="shared" si="3"/>
+        <v>1.4104379616779561</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>4.2503738574889756</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>33</v>
       </c>
@@ -1429,15 +1535,23 @@
         <v>180</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
+        <f>B23*C23</f>
         <v>5940</v>
       </c>
       <c r="E23">
-        <f t="shared" si="1"/>
+        <f>D23/$D$8*$E$8</f>
         <v>2.1578983469373756</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>0.62897909101854799</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="2"/>
+        <v>3.4307950419193527</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>51</v>
       </c>
@@ -1445,15 +1559,23 @@
         <v>161</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
+        <f>B24*C24</f>
         <v>8211</v>
       </c>
       <c r="E24">
-        <f t="shared" si="1"/>
+        <f>D24/$D$8*$E$8</f>
         <v>2.9829130179634329</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>0.97205859521048332</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>3.06865556527231</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>30</v>
       </c>
@@ -1461,15 +1583,23 @@
         <v>146</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
+        <f>B25*C25</f>
         <v>4380</v>
       </c>
       <c r="E25">
-        <f t="shared" si="1"/>
+        <f>D25/$D$8*$E$8</f>
         <v>1.5911775689538223</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>0.57179917365322552</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="2"/>
+        <v>2.7827559784456972</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>25</v>
       </c>
@@ -1489,7 +1619,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>1</v>
       </c>
@@ -1511,7 +1641,7 @@
         <v>0.50595238095238093</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>2</v>
       </c>
@@ -1525,15 +1655,15 @@
         <v>1.8</v>
       </c>
       <c r="E29">
-        <f t="shared" ref="E29:E35" si="2">C29/D29</f>
+        <f t="shared" ref="E29:E35" si="4">C29/D29</f>
         <v>105.55555555555556</v>
       </c>
       <c r="F29">
-        <f t="shared" ref="F29:F35" si="3">E29/B29</f>
+        <f t="shared" ref="F29:F35" si="5">E29/B29</f>
         <v>0.50264550264550267</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>3</v>
       </c>
@@ -1547,15 +1677,15 @@
         <v>1.8</v>
       </c>
       <c r="E30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>111.11111111111111</v>
       </c>
       <c r="F30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.50505050505050508</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>4</v>
       </c>
@@ -1569,15 +1699,15 @@
         <v>1.8</v>
       </c>
       <c r="E31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>138.88888888888889</v>
       </c>
       <c r="F31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.49603174603174605</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>5</v>
       </c>
@@ -1591,11 +1721,11 @@
         <v>1.8</v>
       </c>
       <c r="E32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>166.66666666666666</v>
       </c>
       <c r="F32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.50505050505050497</v>
       </c>
     </row>
@@ -1613,11 +1743,11 @@
         <v>1.8</v>
       </c>
       <c r="E33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>238.88888888888889</v>
       </c>
       <c r="F33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.49768518518518517</v>
       </c>
     </row>
@@ -1635,11 +1765,11 @@
         <v>1.8</v>
       </c>
       <c r="E34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>361.11111111111109</v>
       </c>
       <c r="F34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.50154320987654322</v>
       </c>
     </row>
@@ -1657,11 +1787,11 @@
         <v>1.8</v>
       </c>
       <c r="E35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>541.66666666666663</v>
       </c>
       <c r="F35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.50154320987654322</v>
       </c>
     </row>
@@ -1681,7 +1811,7 @@
   <dimension ref="A2:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1904,6 +2034,144 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5">
+        <v>65</v>
+      </c>
+      <c r="D5">
+        <v>65</v>
+      </c>
+      <c r="E5">
+        <v>95</v>
+      </c>
+      <c r="F5">
+        <v>73</v>
+      </c>
+      <c r="G5">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6">
+        <v>58.88</v>
+      </c>
+      <c r="D6">
+        <v>59.49</v>
+      </c>
+      <c r="E6">
+        <v>103.11</v>
+      </c>
+      <c r="F6">
+        <v>59.18</v>
+      </c>
+      <c r="G6">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <v>105</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10">
+        <v>105</v>
+      </c>
+      <c r="G10">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11">
+        <v>74.31</v>
+      </c>
+      <c r="D11">
+        <v>81.94</v>
+      </c>
+      <c r="E11">
+        <v>113.5</v>
+      </c>
+      <c r="F11">
+        <v>68.849999999999994</v>
+      </c>
+      <c r="G11">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2458,8 +2726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3008,7 +3276,7 @@
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3081,15 +3349,21 @@
         <v>5</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>27</v>
       </c>
       <c r="L6" s="4" t="s">
@@ -3129,20 +3403,28 @@
         <f t="shared" ref="E7" si="0">D7/$D$9*$E$9</f>
         <v>32.15457155752739</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7">
+        <f>B7*SQRT($E$7/$D$7)</f>
+        <v>4.2223544734215661</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7:G12" si="1">C7*SQRT($E$7/$D$7)</f>
+        <v>7.6153178895638955</v>
+      </c>
+      <c r="H7" s="6">
         <f>B22</f>
         <v>33083477.357149027</v>
       </c>
-      <c r="G7" s="6">
-        <f>E7/F7*1000000</f>
+      <c r="I7" s="6">
+        <f>E7/H7*1000000</f>
         <v>0.97192236506478036</v>
       </c>
-      <c r="H7" s="5">
-        <f>SQRT(G7)</f>
+      <c r="J7" s="5">
+        <f>SQRT(I7)</f>
         <v>0.98586123012560967</v>
       </c>
-      <c r="I7" s="5">
-        <f>2*H7</f>
+      <c r="K7" s="5">
+        <f>2*J7</f>
         <v>1.9717224602512193</v>
       </c>
       <c r="L7" s="5">
@@ -3184,20 +3466,28 @@
         <f>D8/$D$9*$E$9</f>
         <v>84.785226585232351</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8">
+        <f t="shared" ref="F8:F12" si="2">B8*SQRT($E$7/$D$7)</f>
+        <v>18.284302853655888</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>4.6370500020611836</v>
+      </c>
+      <c r="H8" s="6">
         <f>H18</f>
         <v>402653184</v>
       </c>
-      <c r="G8" s="6">
-        <f t="shared" ref="G8" si="1">E8/F8*1000000</f>
+      <c r="I8" s="6">
+        <f>E8/H8*1000000</f>
         <v>0.21056638803390748</v>
       </c>
-      <c r="H8" s="5">
-        <f t="shared" ref="H8" si="2">SQRT(G8)</f>
+      <c r="J8" s="5">
+        <f t="shared" ref="J8" si="3">SQRT(I8)</f>
         <v>0.45887513337934044</v>
       </c>
-      <c r="I8" s="5">
-        <f>SQRT(G18)*H8</f>
+      <c r="K8" s="5">
+        <f>SQRT(G18)*J8</f>
         <v>1.1240099324309571</v>
       </c>
       <c r="L8" s="5">
@@ -3213,11 +3503,11 @@
         <v>1.8</v>
       </c>
       <c r="P8">
-        <f t="shared" ref="P8:P15" si="3">N8/O8</f>
+        <f t="shared" ref="P8:P15" si="4">N8/O8</f>
         <v>80</v>
       </c>
       <c r="Q8">
-        <f t="shared" ref="Q8:Q15" si="4">P8/M8</f>
+        <f t="shared" ref="Q8:Q15" si="5">P8/M8</f>
         <v>0.5</v>
       </c>
     </row>
@@ -3238,19 +3528,27 @@
       <c r="E9" s="4">
         <v>296</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>23.298348790843995</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>12.70476301377739</v>
+      </c>
+      <c r="H9" s="9">
         <v>774000000</v>
       </c>
-      <c r="G9" s="9">
-        <f>E9/F9*1000000</f>
+      <c r="I9" s="9">
+        <f>E9/H9*1000000</f>
         <v>0.38242894056847543</v>
       </c>
-      <c r="H9" s="4">
-        <f>SQRT(G9)</f>
+      <c r="J9" s="4">
+        <f>SQRT(I9)</f>
         <v>0.61840839302881023</v>
       </c>
-      <c r="I9" s="4">
-        <f>2*H9</f>
+      <c r="K9" s="4">
+        <f>2*J9</f>
         <v>1.2368167860576205</v>
       </c>
       <c r="L9" s="5">
@@ -3266,11 +3564,11 @@
         <v>1.8</v>
       </c>
       <c r="P9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3285,27 +3583,35 @@
         <v>373</v>
       </c>
       <c r="D10" s="5">
-        <f t="shared" ref="D10:D11" si="5">B10*C10</f>
+        <f t="shared" ref="D10:D11" si="6">B10*C10</f>
         <v>38792</v>
       </c>
       <c r="E10" s="5">
         <f>D10/$D$9*$E$9</f>
         <v>55.133492744855133</v>
       </c>
-      <c r="F10" s="6">
-        <f>E10/$E$9*$F$9</f>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>3.9207577253200254</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>14.061948380234321</v>
+      </c>
+      <c r="H10" s="6">
+        <f>E10/$E$9*$H$9</f>
         <v>144166633.05580363</v>
       </c>
-      <c r="G10" s="6">
-        <f t="shared" ref="G10:G12" si="6">E10/F10*1000000</f>
+      <c r="I10" s="6">
+        <f>E10/H10*1000000</f>
         <v>0.38242894056847543</v>
       </c>
-      <c r="H10" s="5">
-        <f t="shared" ref="H10:H12" si="7">SQRT(G10)</f>
+      <c r="J10" s="5">
+        <f t="shared" ref="J10:J12" si="7">SQRT(I10)</f>
         <v>0.61840839302881023</v>
       </c>
-      <c r="I10" s="5">
-        <f t="shared" ref="I10:I12" si="8">2*H10</f>
+      <c r="K10" s="5">
+        <f t="shared" ref="K10:K12" si="8">2*J10</f>
         <v>1.2368167860576205</v>
       </c>
       <c r="L10" s="5">
@@ -3321,11 +3627,11 @@
         <v>1.8</v>
       </c>
       <c r="P10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>120</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.48</v>
       </c>
     </row>
@@ -3340,26 +3646,34 @@
         <v>47</v>
       </c>
       <c r="D11" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>25521</v>
       </c>
       <c r="E11" s="5">
         <f t="shared" ref="E11:E12" si="9">D11/$D$9*$E$9</f>
         <v>36.271959897438855</v>
       </c>
-      <c r="F11" s="6">
-        <f>E11/$E$9*$F$9</f>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>20.470879277392054</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>1.7718808950965499</v>
+      </c>
+      <c r="H11" s="6">
+        <f>E11/$E$9*$H$9</f>
         <v>94846273.515600249</v>
       </c>
-      <c r="G11" s="6">
-        <f t="shared" si="6"/>
+      <c r="I11" s="6">
+        <f>E11/H11*1000000</f>
         <v>0.38242894056847543</v>
       </c>
-      <c r="H11" s="5">
+      <c r="J11" s="5">
         <f t="shared" si="7"/>
         <v>0.61840839302881023</v>
       </c>
-      <c r="I11" s="5">
+      <c r="K11" s="5">
         <f t="shared" si="8"/>
         <v>1.2368167860576205</v>
       </c>
@@ -3376,11 +3690,11 @@
         <v>1.8</v>
       </c>
       <c r="P11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>140</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3398,19 +3712,19 @@
         <f t="shared" si="9"/>
         <v>91.405452642293994</v>
       </c>
-      <c r="F12" s="6">
-        <f>E12/$E$9*$F$9</f>
+      <c r="H12" s="6">
+        <f>E12/$E$9*$H$9</f>
         <v>239012906.57140389</v>
       </c>
-      <c r="G12" s="6">
-        <f t="shared" si="6"/>
+      <c r="I12" s="6">
+        <f>E12/H12*1000000</f>
         <v>0.38242894056847543</v>
       </c>
-      <c r="H12" s="5">
+      <c r="J12" s="5">
         <f t="shared" si="7"/>
         <v>0.61840839302881023</v>
       </c>
-      <c r="I12" s="5">
+      <c r="K12" s="5">
         <f t="shared" si="8"/>
         <v>1.2368167860576205</v>
       </c>
@@ -3427,11 +3741,11 @@
         <v>1.8</v>
       </c>
       <c r="P12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>180</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3449,11 +3763,11 @@
         <v>1.8</v>
       </c>
       <c r="P13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>280</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3471,11 +3785,11 @@
         <v>1.8</v>
       </c>
       <c r="P14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.49382716049382713</v>
       </c>
     </row>
@@ -3493,11 +3807,11 @@
         <v>0.4</v>
       </c>
       <c r="P15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17500</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.57377049180327866</v>
       </c>
     </row>
@@ -3539,7 +3853,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="2">
-        <f>F9</f>
+        <f>H9</f>
         <v>774000000</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -3595,7 +3909,7 @@
         <v>57</v>
       </c>
       <c r="B21" s="2">
-        <f>F12</f>
+        <f>H12</f>
         <v>239012906.57140389</v>
       </c>
       <c r="E21" s="1"/>
@@ -3611,7 +3925,7 @@
         <v>33083477.357149027</v>
       </c>
       <c r="C22" s="2">
-        <f>E7/E9*F9</f>
+        <f>E7/E9*H9</f>
         <v>84079859.410561487</v>
       </c>
       <c r="F22" s="5"/>
@@ -3652,7 +3966,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:Q4"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3723,15 +4037,21 @@
         <v>5</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>27</v>
       </c>
       <c r="L6" s="4" t="s">
@@ -3771,20 +4091,28 @@
         <f t="shared" ref="E7" si="0">D7/$D$9*$E$9</f>
         <v>18.264882163602056</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7">
+        <f>B7*SQRT($E$7/$D$7)</f>
+        <v>3.065763343760207</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7:G14" si="1">C7*SQRT($E$7/$D$7)</f>
+        <v>5.9576947453484435</v>
+      </c>
+      <c r="H7" s="6">
         <f>B22</f>
         <v>37956390.262902811</v>
       </c>
-      <c r="G7" s="6">
-        <f>E7/F7*1000000</f>
+      <c r="I7" s="6">
+        <f>E7/H7*1000000</f>
         <v>0.48120703884356153</v>
       </c>
-      <c r="H7" s="5">
-        <f>SQRT(G7)</f>
+      <c r="J7" s="5">
+        <f>SQRT(I7)</f>
         <v>0.6936908813322844</v>
       </c>
-      <c r="I7" s="5">
-        <f>2*H7</f>
+      <c r="K7" s="5">
+        <f>2*J7</f>
         <v>1.3873817626645688</v>
       </c>
       <c r="L7" s="5">
@@ -3826,20 +4154,28 @@
         <f>D8/$D$9*$E$9</f>
         <v>20.837369122054088</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8">
+        <f>B8*SQRT($E$7/$D$7)</f>
+        <v>6.0209063606837052</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>3.4608359396055945</v>
+      </c>
+      <c r="H8" s="6">
         <f>H18</f>
         <v>201326592</v>
       </c>
-      <c r="G8" s="6">
-        <f t="shared" ref="G8" si="1">E8/F8*1000000</f>
+      <c r="I8" s="6">
+        <f>E8/H8*1000000</f>
         <v>0.1035003320478106</v>
       </c>
-      <c r="H8" s="5">
-        <f t="shared" ref="H8" si="2">SQRT(G8)</f>
+      <c r="J8" s="5">
+        <f t="shared" ref="J8" si="2">SQRT(I8)</f>
         <v>0.32171467490279426</v>
       </c>
-      <c r="I8" s="5">
-        <f>SQRT(G18)*H8</f>
+      <c r="K8" s="5">
+        <f>SQRT(G18)*J8</f>
         <v>0.78803679627721923</v>
       </c>
       <c r="L8" s="5">
@@ -3880,19 +4216,27 @@
       <c r="E9" s="4">
         <v>81</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9">
+        <f t="shared" ref="F8:F14" si="5">B9*SQRT($E$7/$D$7)</f>
+        <v>8.4861593587589237</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>9.5449539156245624</v>
+      </c>
+      <c r="H9" s="9">
         <v>382000000</v>
       </c>
-      <c r="G9" s="9">
-        <f>E9/F9*1000000</f>
+      <c r="I9" s="9">
+        <f>E9/H9*1000000</f>
         <v>0.21204188481675393</v>
       </c>
-      <c r="H9" s="4">
-        <f>SQRT(G9)</f>
+      <c r="J9" s="4">
+        <f>SQRT(I9)</f>
         <v>0.4604800590869858</v>
       </c>
-      <c r="I9" s="4">
-        <f>2*H9</f>
+      <c r="K9" s="4">
+        <f>2*J9</f>
         <v>0.92096011817397161</v>
       </c>
       <c r="L9" s="5">
@@ -3927,27 +4271,35 @@
         <v>593</v>
       </c>
       <c r="D10" s="5">
-        <f t="shared" ref="D10:D11" si="5">B10*C10</f>
+        <f t="shared" ref="D10:D11" si="6">B10*C10</f>
         <v>52777</v>
       </c>
       <c r="E10" s="5">
         <f>D10/$D$9*$E$9</f>
         <v>13.18009360316697</v>
       </c>
-      <c r="F10" s="6">
-        <f>E10/$E$9*$F$9</f>
+      <c r="F10">
+        <f t="shared" si="5"/>
+        <v>1.4064584412095795</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>9.3711219734525919</v>
+      </c>
+      <c r="H10" s="6">
+        <f>E10/$E$9*$H$9</f>
         <v>62157972.30135534</v>
       </c>
-      <c r="G10" s="6">
-        <f t="shared" ref="G10:G14" si="6">E10/F10*1000000</f>
+      <c r="I10" s="6">
+        <f>E10/H10*1000000</f>
         <v>0.21204188481675393</v>
       </c>
-      <c r="H10" s="5">
-        <f t="shared" ref="H10:H14" si="7">SQRT(G10)</f>
+      <c r="J10" s="5">
+        <f t="shared" ref="J10:J14" si="7">SQRT(I10)</f>
         <v>0.4604800590869858</v>
       </c>
-      <c r="I10" s="5">
-        <f t="shared" ref="I10:I14" si="8">2*H10</f>
+      <c r="K10" s="5">
+        <f t="shared" ref="K10:K14" si="8">2*J10</f>
         <v>0.92096011817397161</v>
       </c>
       <c r="L10" s="5">
@@ -3982,26 +4334,34 @@
         <v>593</v>
       </c>
       <c r="D11" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>36173</v>
       </c>
       <c r="E11" s="5">
         <f t="shared" ref="E11:E12" si="9">D11/$D$9*$E$9</f>
         <v>9.0335473010470242</v>
       </c>
-      <c r="F11" s="6">
-        <f>E11/$E$9*$F$9</f>
+      <c r="F11">
+        <f t="shared" si="5"/>
+        <v>0.96397713386274542</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>9.3711219734525919</v>
+      </c>
+      <c r="H11" s="6">
+        <f>E11/$E$9*$H$9</f>
         <v>42602655.172839053</v>
       </c>
-      <c r="G11" s="6">
-        <f t="shared" si="6"/>
+      <c r="I11" s="6">
+        <f>E11/H11*1000000</f>
         <v>0.21204188481675393</v>
       </c>
-      <c r="H11" s="5">
+      <c r="J11" s="5">
         <f t="shared" si="7"/>
         <v>0.4604800590869858</v>
       </c>
-      <c r="I11" s="5">
+      <c r="K11" s="5">
         <f t="shared" si="8"/>
         <v>0.92096011817397161</v>
       </c>
@@ -4040,19 +4400,19 @@
         <f t="shared" si="9"/>
         <v>22.213640904213992</v>
       </c>
-      <c r="F12" s="6">
-        <f>E12/$E$9*$F$9</f>
+      <c r="H12" s="6">
+        <f>E12/$E$9*$H$9</f>
         <v>104760627.47419438</v>
       </c>
-      <c r="G12" s="6">
-        <f t="shared" si="6"/>
+      <c r="I12" s="6">
+        <f>E12/H12*1000000</f>
         <v>0.21204188481675396</v>
       </c>
-      <c r="H12" s="5">
+      <c r="J12" s="5">
         <f t="shared" si="7"/>
         <v>0.4604800590869858</v>
       </c>
-      <c r="I12" s="5">
+      <c r="K12" s="5">
         <f t="shared" si="8"/>
         <v>0.92096011817397161</v>
       </c>
@@ -4094,18 +4454,26 @@
       <c r="E13">
         <v>114</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13">
+        <f>B13*SQRT($E$13/$D$13)</f>
+        <v>11.439921946188761</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ref="G13" si="11">C13*SQRT($E$13/$D$13)</f>
+        <v>15.454459199072945</v>
+      </c>
+      <c r="H13" s="2">
         <v>177000000</v>
       </c>
-      <c r="G13" s="6">
-        <f t="shared" si="6"/>
+      <c r="I13" s="6">
+        <f>E13/H13*1000000</f>
         <v>0.64406779661016944</v>
       </c>
-      <c r="H13" s="5">
+      <c r="J13" s="5">
         <f t="shared" si="7"/>
         <v>0.8025383458814721</v>
       </c>
-      <c r="I13" s="5">
+      <c r="K13" s="5">
         <f t="shared" si="8"/>
         <v>1.6050766917629442</v>
       </c>
@@ -4142,19 +4510,27 @@
         <f>D14/D13*E13</f>
         <v>73.279141324936262</v>
       </c>
-      <c r="F14" s="2">
-        <f>E14/E13*F13</f>
+      <c r="F14">
+        <f t="shared" ref="F14:F15" si="12">B14*SQRT($E$13/$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14:G15" si="13">C14*SQRT($E$13/$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <f>E14/E13*H13</f>
         <v>113775508.89924315</v>
       </c>
-      <c r="G14" s="6">
-        <f t="shared" si="6"/>
+      <c r="I14" s="6">
+        <f>E14/H14*1000000</f>
         <v>0.64406779661016944</v>
       </c>
-      <c r="H14" s="5">
+      <c r="J14" s="5">
         <f t="shared" si="7"/>
         <v>0.8025383458814721</v>
       </c>
-      <c r="I14" s="5">
+      <c r="K14" s="5">
         <f t="shared" si="8"/>
         <v>1.6050766917629442</v>
       </c>
@@ -4180,6 +4556,47 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="5">
+        <v>189</v>
+      </c>
+      <c r="C15" s="5">
+        <v>176</v>
+      </c>
+      <c r="D15">
+        <f>C15*B15</f>
+        <v>33264</v>
+      </c>
+      <c r="E15">
+        <f>E13/D13*D15</f>
+        <v>30.306945965170275</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="12"/>
+        <v>5.7048687277827863</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="13"/>
+        <v>5.312470349681325</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" ref="H15" si="14">E15/E14*H14</f>
+        <v>47055521.366974905</v>
+      </c>
+      <c r="I15" s="6">
+        <f t="shared" ref="I15" si="15">E15/H15*1000000</f>
+        <v>0.64406779661016944</v>
+      </c>
+      <c r="J15" s="5">
+        <f t="shared" ref="J15" si="16">SQRT(I15)</f>
+        <v>0.8025383458814721</v>
+      </c>
+      <c r="K15" s="5">
+        <f t="shared" ref="K15" si="17">2*J15</f>
+        <v>1.6050766917629442</v>
+      </c>
       <c r="L15" s="5">
         <v>9</v>
       </c>
@@ -4245,7 +4662,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="2">
-        <f>F9</f>
+        <f>H9</f>
         <v>382000000</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -4302,7 +4719,7 @@
         <v>57</v>
       </c>
       <c r="B21" s="2">
-        <f>F12</f>
+        <f>H12</f>
         <v>104760627.47419438</v>
       </c>
       <c r="E21" s="1"/>
@@ -4335,8 +4752,17 @@
       <c r="F24" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="G24" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>85</v>
+      </c>
       <c r="D25">
         <v>31</v>
       </c>
@@ -4347,8 +4773,19 @@
         <f>D25*E25</f>
         <v>1829</v>
       </c>
+      <c r="G25">
+        <f>D25*SQRT($E$13/$D$13)</f>
+        <v>0.93571920931886965</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ref="H25:H29" si="18">E25*SQRT($E$13/$D$13)</f>
+        <v>1.7808849467681713</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>84</v>
+      </c>
       <c r="D26">
         <v>270</v>
       </c>
@@ -4356,11 +4793,22 @@
         <v>213</v>
       </c>
       <c r="F26">
-        <f t="shared" ref="F26:F29" si="11">D26*E26</f>
+        <f t="shared" ref="F26:F29" si="19">D26*E26</f>
         <v>57510</v>
       </c>
+      <c r="G26">
+        <f t="shared" ref="G26:G29" si="20">D26*SQRT($E$13/$D$13)</f>
+        <v>8.149812468261123</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="18"/>
+        <v>6.429296502739331</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>86</v>
+      </c>
       <c r="D27">
         <v>29</v>
       </c>
@@ -4368,11 +4816,22 @@
         <v>44</v>
       </c>
       <c r="F27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>1276</v>
       </c>
+      <c r="G27">
+        <f t="shared" si="20"/>
+        <v>0.87535022807249097</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="18"/>
+        <v>1.3281175874203313</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>83</v>
+      </c>
       <c r="D28">
         <v>103</v>
       </c>
@@ -4380,11 +4839,22 @@
         <v>179</v>
       </c>
       <c r="F28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>18437</v>
       </c>
+      <c r="G28">
+        <f t="shared" si="20"/>
+        <v>3.1090025341885026</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="18"/>
+        <v>5.4030238215508932</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
       <c r="D29">
         <v>51</v>
       </c>
@@ -4392,8 +4862,16 @@
         <v>27</v>
       </c>
       <c r="F29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>1377</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="20"/>
+        <v>1.5394090217826566</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="18"/>
+        <v>0.81498124682611228</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -5035,7 +5513,7 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated cpu validation spreadsheet to include gulftown test case
</commit_message>
<xml_diff>
--- a/data/processor_wla_validation.xlsx
+++ b/data/processor_wla_validation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="15120" windowHeight="7995" tabRatio="897" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="15120" windowHeight="7995" tabRatio="897" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="65nm Merom" sheetId="9" r:id="rId1"/>
@@ -17,19 +17,21 @@
     <sheet name="45nm Penryn 2" sheetId="12" r:id="rId3"/>
     <sheet name="45nm Nehalem" sheetId="8" r:id="rId4"/>
     <sheet name="32nm Nehalem" sheetId="10" r:id="rId5"/>
-    <sheet name="Sandy Bridge EP-4 32nm Data" sheetId="3" r:id="rId6"/>
-    <sheet name="32nm SB Core i7 2700k" sheetId="11" r:id="rId7"/>
-    <sheet name="32nm Sandy Bridge (standard)" sheetId="6" r:id="rId8"/>
-    <sheet name="22nm - Ivy Bridge EP10" sheetId="4" r:id="rId9"/>
-    <sheet name="22nm Ivy Bridge (standard)" sheetId="5" r:id="rId10"/>
-    <sheet name="Power data" sheetId="13" r:id="rId11"/>
+    <sheet name="32nm Nehalem (2)" sheetId="14" r:id="rId6"/>
+    <sheet name="32nm Gulftown (Nehalem)" sheetId="15" r:id="rId7"/>
+    <sheet name="Sandy Bridge EP-4 32nm Data" sheetId="3" r:id="rId8"/>
+    <sheet name="32nm SB Core i7 2700k" sheetId="11" r:id="rId9"/>
+    <sheet name="32nm Sandy Bridge (standard)" sheetId="6" r:id="rId10"/>
+    <sheet name="22nm - Ivy Bridge EP10" sheetId="4" r:id="rId11"/>
+    <sheet name="22nm Ivy Bridge (standard)" sheetId="5" r:id="rId12"/>
+    <sheet name="Power data" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="106">
   <si>
     <t>w (px)</t>
   </si>
@@ -323,6 +325,30 @@
   </si>
   <si>
     <t>pcie_con</t>
+  </si>
+  <si>
+    <t>Using Intel_32nm_nehalem_clarkdale_2core_both_dice.jpg</t>
+  </si>
+  <si>
+    <t>using Intel_32nm_nehalem_clarkdale_2core</t>
+  </si>
+  <si>
+    <t>Intel 32nm Nehalem Core i7 980 (Gulftown)</t>
+  </si>
+  <si>
+    <t>memcon</t>
+  </si>
+  <si>
+    <t>queue</t>
+  </si>
+  <si>
+    <t>io_left</t>
+  </si>
+  <si>
+    <t>io_right</t>
+  </si>
+  <si>
+    <t>Using 32nm_intel_core_i7_980_gulftown_block_diagram.jpg</t>
   </si>
 </sst>
 </file>
@@ -624,11 +650,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="229747896"/>
-        <c:axId val="229761976"/>
+        <c:axId val="253399064"/>
+        <c:axId val="253401416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="229747896"/>
+        <c:axId val="253399064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -659,12 +685,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="229761976"/>
+        <c:crossAx val="253401416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="229761976"/>
+        <c:axId val="253401416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -701,7 +727,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="229747896"/>
+        <c:crossAx val="253399064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1443,11 +1469,11 @@
         <v>261</v>
       </c>
       <c r="D20">
-        <f>B20*C20</f>
+        <f t="shared" ref="D20:D25" si="2">B20*C20</f>
         <v>21663</v>
       </c>
       <c r="E20">
-        <f>D20/$D$8*$E$8</f>
+        <f t="shared" ref="E20:E25" si="3">D20/$D$8*$E$8</f>
         <v>7.8697898804216111</v>
       </c>
       <c r="F20">
@@ -1459,7 +1485,7 @@
         <v>1.5819777137739237</v>
       </c>
       <c r="H20">
-        <f t="shared" ref="H20:H25" si="2">C20*SQRT($E$7/$D$7)</f>
+        <f t="shared" ref="H20:H25" si="4">C20*SQRT($E$7/$D$7)</f>
         <v>4.9746528107830619</v>
       </c>
       <c r="I20" s="2">
@@ -1487,19 +1513,19 @@
         <v>239</v>
       </c>
       <c r="D21">
-        <f>B21*C21</f>
+        <f t="shared" si="2"/>
         <v>24378</v>
       </c>
       <c r="E21">
-        <f>D21/$D$8*$E$8</f>
+        <f t="shared" si="3"/>
         <v>8.8561020036429881</v>
       </c>
       <c r="G21">
-        <f t="shared" ref="G21:G25" si="3">B21*SQRT($E$7/$D$7)</f>
+        <f t="shared" ref="G21:G25" si="5">B21*SQRT($E$7/$D$7)</f>
         <v>1.9441171904209666</v>
       </c>
       <c r="H21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.5553334167706963</v>
       </c>
     </row>
@@ -1511,19 +1537,19 @@
         <v>223</v>
       </c>
       <c r="D22">
-        <f>B22*C22</f>
+        <f t="shared" si="2"/>
         <v>16502</v>
       </c>
       <c r="E22">
-        <f>D22/$D$8*$E$8</f>
+        <f t="shared" si="3"/>
         <v>5.9948886399260219</v>
       </c>
       <c r="G22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.4104379616779561</v>
       </c>
       <c r="H22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.2503738574889756</v>
       </c>
     </row>
@@ -1535,19 +1561,19 @@
         <v>180</v>
       </c>
       <c r="D23">
-        <f>B23*C23</f>
+        <f t="shared" si="2"/>
         <v>5940</v>
       </c>
       <c r="E23">
-        <f>D23/$D$8*$E$8</f>
+        <f t="shared" si="3"/>
         <v>2.1578983469373756</v>
       </c>
       <c r="G23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.62897909101854799</v>
       </c>
       <c r="H23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.4307950419193527</v>
       </c>
     </row>
@@ -1559,19 +1585,19 @@
         <v>161</v>
       </c>
       <c r="D24">
-        <f>B24*C24</f>
+        <f t="shared" si="2"/>
         <v>8211</v>
       </c>
       <c r="E24">
-        <f>D24/$D$8*$E$8</f>
+        <f t="shared" si="3"/>
         <v>2.9829130179634329</v>
       </c>
       <c r="G24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.97205859521048332</v>
       </c>
       <c r="H24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.06865556527231</v>
       </c>
     </row>
@@ -1583,19 +1609,19 @@
         <v>146</v>
       </c>
       <c r="D25">
-        <f>B25*C25</f>
+        <f t="shared" si="2"/>
         <v>4380</v>
       </c>
       <c r="E25">
-        <f>D25/$D$8*$E$8</f>
+        <f t="shared" si="3"/>
         <v>1.5911775689538223</v>
       </c>
       <c r="G25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.57179917365322552</v>
       </c>
       <c r="H25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.7827559784456972</v>
       </c>
     </row>
@@ -1655,11 +1681,11 @@
         <v>1.8</v>
       </c>
       <c r="E29">
-        <f t="shared" ref="E29:E35" si="4">C29/D29</f>
+        <f t="shared" ref="E29:E35" si="6">C29/D29</f>
         <v>105.55555555555556</v>
       </c>
       <c r="F29">
-        <f t="shared" ref="F29:F35" si="5">E29/B29</f>
+        <f t="shared" ref="F29:F35" si="7">E29/B29</f>
         <v>0.50264550264550267</v>
       </c>
     </row>
@@ -1677,11 +1703,11 @@
         <v>1.8</v>
       </c>
       <c r="E30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>111.11111111111111</v>
       </c>
       <c r="F30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.50505050505050508</v>
       </c>
     </row>
@@ -1699,11 +1725,11 @@
         <v>1.8</v>
       </c>
       <c r="E31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>138.88888888888889</v>
       </c>
       <c r="F31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.49603174603174605</v>
       </c>
     </row>
@@ -1721,11 +1747,11 @@
         <v>1.8</v>
       </c>
       <c r="E32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>166.66666666666666</v>
       </c>
       <c r="F32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.50505050505050497</v>
       </c>
     </row>
@@ -1743,11 +1769,11 @@
         <v>1.8</v>
       </c>
       <c r="E33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>238.88888888888889</v>
       </c>
       <c r="F33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.49768518518518517</v>
       </c>
     </row>
@@ -1765,11 +1791,11 @@
         <v>1.8</v>
       </c>
       <c r="E34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>361.11111111111109</v>
       </c>
       <c r="F34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.50154320987654322</v>
       </c>
     </row>
@@ -1787,11 +1813,11 @@
         <v>1.8</v>
       </c>
       <c r="E35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>541.66666666666663</v>
       </c>
       <c r="F35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.50154320987654322</v>
       </c>
     </row>
@@ -1807,6 +1833,648 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>169</v>
+      </c>
+      <c r="C2">
+        <v>287</v>
+      </c>
+      <c r="D2">
+        <f>B2*C2</f>
+        <v>48503</v>
+      </c>
+      <c r="E2">
+        <f>D2/$D$4*$E$4</f>
+        <v>18.546941608010311</v>
+      </c>
+      <c r="F2" s="2">
+        <f>E2/$E$4*$F$4</f>
+        <v>85436143.055417866</v>
+      </c>
+      <c r="G2" s="2">
+        <f>E2/F2*1000000</f>
+        <v>0.21708542713567841</v>
+      </c>
+      <c r="H2">
+        <f>SQRT(G2)</f>
+        <v>0.46592427188941166</v>
+      </c>
+      <c r="I2">
+        <f>2*H2</f>
+        <v>0.93184854377882331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>228</v>
+      </c>
+      <c r="C3">
+        <v>325</v>
+      </c>
+      <c r="D3">
+        <f>B3*C3</f>
+        <v>74100</v>
+      </c>
+      <c r="F3">
+        <f>B8</f>
+        <v>1006632960</v>
+      </c>
+      <c r="G3" s="2">
+        <f>E3/F3*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f>SQRT(G3)</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f>2*H3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1078</v>
+      </c>
+      <c r="C4" s="1">
+        <v>524</v>
+      </c>
+      <c r="D4">
+        <f>B4*C4</f>
+        <v>564872</v>
+      </c>
+      <c r="E4">
+        <v>216</v>
+      </c>
+      <c r="F4" s="2">
+        <v>995000000</v>
+      </c>
+      <c r="G4" s="2">
+        <f>E4/F4*1000000</f>
+        <v>0.21708542713567841</v>
+      </c>
+      <c r="H4">
+        <f>SQRT(G4)</f>
+        <v>0.46592427188941166</v>
+      </c>
+      <c r="I4">
+        <f>2*H4</f>
+        <v>0.93184854377882331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2270000000</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <f>E7*POWER(2,20)*8</f>
+        <v>167772160</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <f>G7*F7</f>
+        <v>1006632960</v>
+      </c>
+      <c r="I7">
+        <f>E3/H7*1000000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <f>H7</f>
+        <v>1006632960</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2">
+        <f>B7-B8</f>
+        <v>1263367040</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L13" s="5">
+        <v>112.5</v>
+      </c>
+      <c r="M13" s="5">
+        <v>112.5</v>
+      </c>
+      <c r="N13" s="5">
+        <v>112.5</v>
+      </c>
+      <c r="O13" s="5">
+        <v>168.8</v>
+      </c>
+      <c r="P13" s="5">
+        <v>225</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>337.6</v>
+      </c>
+      <c r="R13" s="5">
+        <v>450.1</v>
+      </c>
+      <c r="S13" s="5">
+        <v>566.5</v>
+      </c>
+      <c r="T13" s="5">
+        <v>19400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="D14">
+        <v>0.1125</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1</v>
+      </c>
+      <c r="G14" s="5">
+        <v>112.5</v>
+      </c>
+      <c r="H14">
+        <v>112.5</v>
+      </c>
+      <c r="I14">
+        <v>112.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="3">
+        <v>0.1993</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="5">
+        <v>2</v>
+      </c>
+      <c r="G15" s="5">
+        <v>112.5</v>
+      </c>
+      <c r="H15">
+        <v>112.5</v>
+      </c>
+      <c r="I15">
+        <v>112.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="D16">
+        <v>0.42</v>
+      </c>
+      <c r="F16" s="5">
+        <v>3</v>
+      </c>
+      <c r="G16" s="5">
+        <v>112.5</v>
+      </c>
+      <c r="H16">
+        <v>199.3</v>
+      </c>
+      <c r="I16">
+        <v>131.49469999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>0.71819999999999995</v>
+      </c>
+      <c r="F17" s="5">
+        <v>4</v>
+      </c>
+      <c r="G17" s="5">
+        <v>168.8</v>
+      </c>
+      <c r="H17">
+        <v>199.3</v>
+      </c>
+      <c r="I17">
+        <v>247.32849999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F18" s="5">
+        <v>5</v>
+      </c>
+      <c r="G18" s="5">
+        <v>225</v>
+      </c>
+      <c r="H18">
+        <v>420</v>
+      </c>
+      <c r="I18">
+        <v>374.14409999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F19" s="5">
+        <v>6</v>
+      </c>
+      <c r="G19" s="5">
+        <v>337.6</v>
+      </c>
+      <c r="H19">
+        <v>420</v>
+      </c>
+      <c r="I19">
+        <v>540.39850000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F20" s="5">
+        <v>7</v>
+      </c>
+      <c r="G20" s="5">
+        <v>450.1</v>
+      </c>
+      <c r="H20">
+        <v>718.2</v>
+      </c>
+      <c r="I20">
+        <v>718.20759999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F21" s="5">
+        <v>8</v>
+      </c>
+      <c r="G21" s="5">
+        <v>566.5</v>
+      </c>
+      <c r="H21">
+        <v>718.2</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F22" s="5">
+        <v>9</v>
+      </c>
+      <c r="G22" s="5">
+        <v>19400</v>
+      </c>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F23" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="6">
+        <v>145900</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>79</v>
+      </c>
+      <c r="C3">
+        <v>144</v>
+      </c>
+      <c r="D3">
+        <f>B3*C3</f>
+        <v>11376</v>
+      </c>
+      <c r="E3">
+        <f>D3*E5/D5</f>
+        <v>11.516760404949382</v>
+      </c>
+      <c r="F3" s="2">
+        <f>F5*E3/E5</f>
+        <v>95058974.771010771</v>
+      </c>
+      <c r="G3" s="2">
+        <f>E3/F3</f>
+        <v>1.2115384615384617E-7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>635</v>
+      </c>
+      <c r="C5" s="3">
+        <v>539</v>
+      </c>
+      <c r="D5" s="3">
+        <f>B5*C5</f>
+        <v>342265</v>
+      </c>
+      <c r="E5">
+        <v>346.5</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2860000000</v>
+      </c>
+      <c r="G5" s="2">
+        <f>E5/F5*1000000</f>
+        <v>0.12115384615384614</v>
+      </c>
+      <c r="H5">
+        <f>SQRT(G5)</f>
+        <v>0.34807161066919279</v>
+      </c>
+      <c r="I5">
+        <f>2*H5</f>
+        <v>0.69614322133838558</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>90</v>
+      </c>
+      <c r="C9" s="5">
+        <v>90</v>
+      </c>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>80</v>
+      </c>
+      <c r="C10" s="5">
+        <v>90</v>
+      </c>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>80</v>
+      </c>
+      <c r="C11" s="5">
+        <v>90</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>112</v>
+      </c>
+      <c r="C12" s="5">
+        <v>115.836</v>
+      </c>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>160</v>
+      </c>
+      <c r="C13" s="5">
+        <v>210.5411</v>
+      </c>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>240</v>
+      </c>
+      <c r="C14" s="5">
+        <v>322.54140000000001</v>
+      </c>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>320</v>
+      </c>
+      <c r="C15" s="5">
+        <v>493.471</v>
+      </c>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>360</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>14000</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I17"/>
   <sheetViews>
@@ -2037,11 +2705,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -3408,7 +4076,7 @@
         <v>4.2223544734215661</v>
       </c>
       <c r="G7">
-        <f t="shared" ref="G7:G12" si="1">C7*SQRT($E$7/$D$7)</f>
+        <f t="shared" ref="G7:G11" si="1">C7*SQRT($E$7/$D$7)</f>
         <v>7.6153178895638955</v>
       </c>
       <c r="H7" s="6">
@@ -3416,7 +4084,7 @@
         <v>33083477.357149027</v>
       </c>
       <c r="I7" s="6">
-        <f>E7/H7*1000000</f>
+        <f t="shared" ref="I7:I12" si="2">E7/H7*1000000</f>
         <v>0.97192236506478036</v>
       </c>
       <c r="J7" s="5">
@@ -3467,7 +4135,7 @@
         <v>84.785226585232351</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:F12" si="2">B8*SQRT($E$7/$D$7)</f>
+        <f t="shared" ref="F8:F11" si="3">B8*SQRT($E$7/$D$7)</f>
         <v>18.284302853655888</v>
       </c>
       <c r="G8">
@@ -3479,11 +4147,11 @@
         <v>402653184</v>
       </c>
       <c r="I8" s="6">
-        <f>E8/H8*1000000</f>
+        <f t="shared" si="2"/>
         <v>0.21056638803390748</v>
       </c>
       <c r="J8" s="5">
-        <f t="shared" ref="J8" si="3">SQRT(I8)</f>
+        <f t="shared" ref="J8" si="4">SQRT(I8)</f>
         <v>0.45887513337934044</v>
       </c>
       <c r="K8" s="5">
@@ -3503,11 +4171,11 @@
         <v>1.8</v>
       </c>
       <c r="P8">
-        <f t="shared" ref="P8:P15" si="4">N8/O8</f>
+        <f t="shared" ref="P8:P15" si="5">N8/O8</f>
         <v>80</v>
       </c>
       <c r="Q8">
-        <f t="shared" ref="Q8:Q15" si="5">P8/M8</f>
+        <f t="shared" ref="Q8:Q15" si="6">P8/M8</f>
         <v>0.5</v>
       </c>
     </row>
@@ -3529,7 +4197,7 @@
         <v>296</v>
       </c>
       <c r="F9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23.298348790843995</v>
       </c>
       <c r="G9">
@@ -3540,7 +4208,7 @@
         <v>774000000</v>
       </c>
       <c r="I9" s="9">
-        <f>E9/H9*1000000</f>
+        <f t="shared" si="2"/>
         <v>0.38242894056847543</v>
       </c>
       <c r="J9" s="4">
@@ -3564,11 +4232,11 @@
         <v>1.8</v>
       </c>
       <c r="P9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>80</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3583,7 +4251,7 @@
         <v>373</v>
       </c>
       <c r="D10" s="5">
-        <f t="shared" ref="D10:D11" si="6">B10*C10</f>
+        <f t="shared" ref="D10:D11" si="7">B10*C10</f>
         <v>38792</v>
       </c>
       <c r="E10" s="5">
@@ -3591,7 +4259,7 @@
         <v>55.133492744855133</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.9207577253200254</v>
       </c>
       <c r="G10">
@@ -3603,15 +4271,15 @@
         <v>144166633.05580363</v>
       </c>
       <c r="I10" s="6">
-        <f>E10/H10*1000000</f>
+        <f t="shared" si="2"/>
         <v>0.38242894056847543</v>
       </c>
       <c r="J10" s="5">
-        <f t="shared" ref="J10:J12" si="7">SQRT(I10)</f>
+        <f t="shared" ref="J10:J12" si="8">SQRT(I10)</f>
         <v>0.61840839302881023</v>
       </c>
       <c r="K10" s="5">
-        <f t="shared" ref="K10:K12" si="8">2*J10</f>
+        <f t="shared" ref="K10:K12" si="9">2*J10</f>
         <v>1.2368167860576205</v>
       </c>
       <c r="L10" s="5">
@@ -3627,11 +4295,11 @@
         <v>1.8</v>
       </c>
       <c r="P10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>120</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.48</v>
       </c>
     </row>
@@ -3646,15 +4314,15 @@
         <v>47</v>
       </c>
       <c r="D11" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>25521</v>
       </c>
       <c r="E11" s="5">
-        <f t="shared" ref="E11:E12" si="9">D11/$D$9*$E$9</f>
+        <f t="shared" ref="E11:E12" si="10">D11/$D$9*$E$9</f>
         <v>36.271959897438855</v>
       </c>
       <c r="F11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20.470879277392054</v>
       </c>
       <c r="G11">
@@ -3666,15 +4334,15 @@
         <v>94846273.515600249</v>
       </c>
       <c r="I11" s="6">
-        <f>E11/H11*1000000</f>
+        <f t="shared" si="2"/>
         <v>0.38242894056847543</v>
       </c>
       <c r="J11" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.61840839302881023</v>
       </c>
       <c r="K11" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.2368167860576205</v>
       </c>
       <c r="L11" s="5">
@@ -3690,11 +4358,11 @@
         <v>1.8</v>
       </c>
       <c r="P11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>140</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3709,7 +4377,7 @@
         <v>64313</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>91.405452642293994</v>
       </c>
       <c r="H12" s="6">
@@ -3717,15 +4385,15 @@
         <v>239012906.57140389</v>
       </c>
       <c r="I12" s="6">
-        <f>E12/H12*1000000</f>
+        <f t="shared" si="2"/>
         <v>0.38242894056847543</v>
       </c>
       <c r="J12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.61840839302881023</v>
       </c>
       <c r="K12" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.2368167860576205</v>
       </c>
       <c r="L12" s="5">
@@ -3741,11 +4409,11 @@
         <v>1.8</v>
       </c>
       <c r="P12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>180</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3763,11 +4431,11 @@
         <v>1.8</v>
       </c>
       <c r="P13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>280</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3785,11 +4453,11 @@
         <v>1.8</v>
       </c>
       <c r="P14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>400</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49382716049382713</v>
       </c>
     </row>
@@ -3807,11 +4475,11 @@
         <v>0.4</v>
       </c>
       <c r="P15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17500</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.57377049180327866</v>
       </c>
     </row>
@@ -3966,7 +4634,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3979,6 +4647,9 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
       <c r="L2" s="4" t="s">
         <v>37</v>
       </c>
@@ -4096,7 +4767,7 @@
         <v>3.065763343760207</v>
       </c>
       <c r="G7">
-        <f t="shared" ref="G7:G14" si="1">C7*SQRT($E$7/$D$7)</f>
+        <f t="shared" ref="G7:G11" si="1">C7*SQRT($E$7/$D$7)</f>
         <v>5.9576947453484435</v>
       </c>
       <c r="H7" s="6">
@@ -4104,7 +4775,7 @@
         <v>37956390.262902811</v>
       </c>
       <c r="I7" s="6">
-        <f>E7/H7*1000000</f>
+        <f t="shared" ref="I7:I14" si="2">E7/H7*1000000</f>
         <v>0.48120703884356153</v>
       </c>
       <c r="J7" s="5">
@@ -4167,11 +4838,11 @@
         <v>201326592</v>
       </c>
       <c r="I8" s="6">
-        <f>E8/H8*1000000</f>
+        <f t="shared" si="2"/>
         <v>0.1035003320478106</v>
       </c>
       <c r="J8" s="5">
-        <f t="shared" ref="J8" si="2">SQRT(I8)</f>
+        <f t="shared" ref="J8" si="3">SQRT(I8)</f>
         <v>0.32171467490279426</v>
       </c>
       <c r="K8" s="5">
@@ -4191,11 +4862,11 @@
         <v>1.7</v>
       </c>
       <c r="P8">
-        <f t="shared" ref="P8:P15" si="3">N8/O8</f>
+        <f t="shared" ref="P8:P15" si="4">N8/O8</f>
         <v>55.882352941176471</v>
       </c>
       <c r="Q8">
-        <f t="shared" ref="Q8:Q15" si="4">P8/M8</f>
+        <f t="shared" ref="Q8:Q15" si="5">P8/M8</f>
         <v>0.49673202614379086</v>
       </c>
     </row>
@@ -4217,7 +4888,7 @@
         <v>81</v>
       </c>
       <c r="F9">
-        <f t="shared" ref="F8:F14" si="5">B9*SQRT($E$7/$D$7)</f>
+        <f t="shared" ref="F9:F11" si="6">B9*SQRT($E$7/$D$7)</f>
         <v>8.4861593587589237</v>
       </c>
       <c r="G9">
@@ -4228,7 +4899,7 @@
         <v>382000000</v>
       </c>
       <c r="I9" s="9">
-        <f>E9/H9*1000000</f>
+        <f t="shared" si="2"/>
         <v>0.21204188481675393</v>
       </c>
       <c r="J9" s="4">
@@ -4252,11 +4923,11 @@
         <v>1.7</v>
       </c>
       <c r="P9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>55.882352941176471</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.49673202614379086</v>
       </c>
     </row>
@@ -4271,7 +4942,7 @@
         <v>593</v>
       </c>
       <c r="D10" s="5">
-        <f t="shared" ref="D10:D11" si="6">B10*C10</f>
+        <f t="shared" ref="D10:D11" si="7">B10*C10</f>
         <v>52777</v>
       </c>
       <c r="E10" s="5">
@@ -4279,7 +4950,7 @@
         <v>13.18009360316697</v>
       </c>
       <c r="F10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.4064584412095795</v>
       </c>
       <c r="G10">
@@ -4291,15 +4962,15 @@
         <v>62157972.30135534</v>
       </c>
       <c r="I10" s="6">
-        <f>E10/H10*1000000</f>
+        <f t="shared" si="2"/>
         <v>0.21204188481675393</v>
       </c>
       <c r="J10" s="5">
-        <f t="shared" ref="J10:J14" si="7">SQRT(I10)</f>
+        <f t="shared" ref="J10:J14" si="8">SQRT(I10)</f>
         <v>0.4604800590869858</v>
       </c>
       <c r="K10" s="5">
-        <f t="shared" ref="K10:K14" si="8">2*J10</f>
+        <f t="shared" ref="K10:K14" si="9">2*J10</f>
         <v>0.92096011817397161</v>
       </c>
       <c r="L10" s="5">
@@ -4315,11 +4986,11 @@
         <v>1.8</v>
       </c>
       <c r="P10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>83.888888888888886</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.49697209057398628</v>
       </c>
     </row>
@@ -4334,15 +5005,15 @@
         <v>593</v>
       </c>
       <c r="D11" s="5">
+        <f t="shared" si="7"/>
+        <v>36173</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" ref="E11:E12" si="10">D11/$D$9*$E$9</f>
+        <v>9.0335473010470242</v>
+      </c>
+      <c r="F11">
         <f t="shared" si="6"/>
-        <v>36173</v>
-      </c>
-      <c r="E11" s="5">
-        <f t="shared" ref="E11:E12" si="9">D11/$D$9*$E$9</f>
-        <v>9.0335473010470242</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="5"/>
         <v>0.96397713386274542</v>
       </c>
       <c r="G11">
@@ -4354,15 +5025,15 @@
         <v>42602655.172839053</v>
       </c>
       <c r="I11" s="6">
-        <f>E11/H11*1000000</f>
+        <f t="shared" si="2"/>
         <v>0.21204188481675393</v>
       </c>
       <c r="J11" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.4604800590869858</v>
       </c>
       <c r="K11" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.92096011817397161</v>
       </c>
       <c r="L11" s="5">
@@ -4378,11 +5049,11 @@
         <v>1.8</v>
       </c>
       <c r="P11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>113.33333333333333</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.50370370370370365</v>
       </c>
     </row>
@@ -4397,7 +5068,7 @@
         <v>88950</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>22.213640904213992</v>
       </c>
       <c r="H12" s="6">
@@ -4405,15 +5076,15 @@
         <v>104760627.47419438</v>
       </c>
       <c r="I12" s="6">
-        <f>E12/H12*1000000</f>
+        <f t="shared" si="2"/>
         <v>0.21204188481675396</v>
       </c>
       <c r="J12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.4604800590869858</v>
       </c>
       <c r="K12" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.92096011817397161</v>
       </c>
       <c r="L12" s="5">
@@ -4429,11 +5100,11 @@
         <v>1.8</v>
       </c>
       <c r="P12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>168.33333333333334</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.4986176935229068</v>
       </c>
     </row>
@@ -4448,7 +5119,7 @@
         <v>512</v>
       </c>
       <c r="D13" s="5">
-        <f t="shared" ref="D13" si="10">D11+D12</f>
+        <f t="shared" ref="D13" si="11">D11+D12</f>
         <v>125123</v>
       </c>
       <c r="E13">
@@ -4459,22 +5130,22 @@
         <v>11.439921946188761</v>
       </c>
       <c r="G13">
-        <f t="shared" ref="G13" si="11">C13*SQRT($E$13/$D$13)</f>
+        <f t="shared" ref="G13" si="12">C13*SQRT($E$13/$D$13)</f>
         <v>15.454459199072945</v>
       </c>
       <c r="H13" s="2">
         <v>177000000</v>
       </c>
       <c r="I13" s="6">
-        <f>E13/H13*1000000</f>
+        <f t="shared" si="2"/>
         <v>0.64406779661016944</v>
       </c>
       <c r="J13" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.8025383458814721</v>
       </c>
       <c r="K13" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.6050766917629442</v>
       </c>
       <c r="L13" s="5">
@@ -4490,11 +5161,11 @@
         <v>1.7</v>
       </c>
       <c r="P13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>228.23529411764707</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.50707685873727404</v>
       </c>
     </row>
@@ -4511,11 +5182,11 @@
         <v>73.279141324936262</v>
       </c>
       <c r="F14">
-        <f t="shared" ref="F14:F15" si="12">B14*SQRT($E$13/$D$13)</f>
+        <f t="shared" ref="F14:F15" si="13">B14*SQRT($E$13/$D$13)</f>
         <v>0</v>
       </c>
       <c r="G14">
-        <f t="shared" ref="G14:G15" si="13">C14*SQRT($E$13/$D$13)</f>
+        <f t="shared" ref="G14:G15" si="14">C14*SQRT($E$13/$D$13)</f>
         <v>0</v>
       </c>
       <c r="H14" s="2">
@@ -4523,15 +5194,15 @@
         <v>113775508.89924315</v>
       </c>
       <c r="I14" s="6">
-        <f>E14/H14*1000000</f>
+        <f t="shared" si="2"/>
         <v>0.64406779661016944</v>
       </c>
       <c r="J14" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.8025383458814721</v>
       </c>
       <c r="K14" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.6050766917629442</v>
       </c>
       <c r="L14" s="5">
@@ -4547,11 +5218,11 @@
         <v>1.8</v>
       </c>
       <c r="P14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>280</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.49426301853486321</v>
       </c>
     </row>
@@ -4574,27 +5245,27 @@
         <v>30.306945965170275</v>
       </c>
       <c r="F15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.7048687277827863</v>
       </c>
       <c r="G15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>5.312470349681325</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" ref="H15" si="14">E15/E14*H14</f>
+        <f t="shared" ref="H15" si="15">E15/E14*H14</f>
         <v>47055521.366974905</v>
       </c>
       <c r="I15" s="6">
-        <f t="shared" ref="I15" si="15">E15/H15*1000000</f>
+        <f t="shared" ref="I15" si="16">E15/H15*1000000</f>
         <v>0.64406779661016944</v>
       </c>
       <c r="J15" s="5">
-        <f t="shared" ref="J15" si="16">SQRT(I15)</f>
+        <f t="shared" ref="J15" si="17">SQRT(I15)</f>
         <v>0.8025383458814721</v>
       </c>
       <c r="K15" s="5">
-        <f t="shared" ref="K15" si="17">2*J15</f>
+        <f t="shared" ref="K15" si="18">2*J15</f>
         <v>1.6050766917629442</v>
       </c>
       <c r="L15" s="5">
@@ -4610,11 +5281,11 @@
         <v>1.5</v>
       </c>
       <c r="P15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5333.333333333333</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.274914089347079</v>
       </c>
     </row>
@@ -4778,7 +5449,7 @@
         <v>0.93571920931886965</v>
       </c>
       <c r="H25">
-        <f t="shared" ref="H25:H29" si="18">E25*SQRT($E$13/$D$13)</f>
+        <f t="shared" ref="H25:H29" si="19">E25*SQRT($E$13/$D$13)</f>
         <v>1.7808849467681713</v>
       </c>
     </row>
@@ -4793,15 +5464,15 @@
         <v>213</v>
       </c>
       <c r="F26">
-        <f t="shared" ref="F26:F29" si="19">D26*E26</f>
+        <f t="shared" ref="F26:F29" si="20">D26*E26</f>
         <v>57510</v>
       </c>
       <c r="G26">
-        <f t="shared" ref="G26:G29" si="20">D26*SQRT($E$13/$D$13)</f>
+        <f t="shared" ref="G26:G29" si="21">D26*SQRT($E$13/$D$13)</f>
         <v>8.149812468261123</v>
       </c>
       <c r="H26">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6.429296502739331</v>
       </c>
     </row>
@@ -4816,15 +5487,15 @@
         <v>44</v>
       </c>
       <c r="F27">
+        <f t="shared" si="20"/>
+        <v>1276</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="21"/>
+        <v>0.87535022807249097</v>
+      </c>
+      <c r="H27">
         <f t="shared" si="19"/>
-        <v>1276</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="20"/>
-        <v>0.87535022807249097</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="18"/>
         <v>1.3281175874203313</v>
       </c>
     </row>
@@ -4839,15 +5510,15 @@
         <v>179</v>
       </c>
       <c r="F28">
+        <f t="shared" si="20"/>
+        <v>18437</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="21"/>
+        <v>3.1090025341885026</v>
+      </c>
+      <c r="H28">
         <f t="shared" si="19"/>
-        <v>18437</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="20"/>
-        <v>3.1090025341885026</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="18"/>
         <v>5.4030238215508932</v>
       </c>
     </row>
@@ -4862,15 +5533,15 @@
         <v>27</v>
       </c>
       <c r="F29">
+        <f t="shared" si="20"/>
+        <v>1377</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="21"/>
+        <v>1.5394090217826566</v>
+      </c>
+      <c r="H29">
         <f t="shared" si="19"/>
-        <v>1377</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="20"/>
-        <v>1.5394090217826566</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="18"/>
         <v>0.81498124682611228</v>
       </c>
     </row>
@@ -4890,6 +5561,1658 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L3" s="7">
+        <v>73</v>
+      </c>
+      <c r="M3" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="N3" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="O3" s="5">
+        <v>3.6</v>
+      </c>
+      <c r="P3" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="5">
+        <v>120</v>
+      </c>
+      <c r="C7" s="5">
+        <v>228</v>
+      </c>
+      <c r="D7" s="5">
+        <f>B7*C7</f>
+        <v>27360</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" ref="E7" si="0">D7/$D$9*$E$9</f>
+        <v>18.07959013852404</v>
+      </c>
+      <c r="F7">
+        <f>B7*SQRT($E$7/$D$7)</f>
+        <v>3.0847323639366051</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7:G11" si="1">C7*SQRT($E$7/$D$7)</f>
+        <v>5.8609914914795489</v>
+      </c>
+      <c r="H7" s="6">
+        <f>B22</f>
+        <v>42169887.76870238</v>
+      </c>
+      <c r="I7" s="6">
+        <f t="shared" ref="I7:I15" si="2">E7/H7*1000000</f>
+        <v>0.42873223276497163</v>
+      </c>
+      <c r="J7" s="5">
+        <f>SQRT(I7)</f>
+        <v>0.65477647542117123</v>
+      </c>
+      <c r="K7" s="5">
+        <f>2*J7</f>
+        <v>1.3095529508423425</v>
+      </c>
+      <c r="L7" s="5">
+        <v>1</v>
+      </c>
+      <c r="M7" s="5">
+        <v>112.5</v>
+      </c>
+      <c r="N7" s="5">
+        <v>95</v>
+      </c>
+      <c r="O7" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="P7">
+        <f>N7/O7</f>
+        <v>55.882352941176471</v>
+      </c>
+      <c r="Q7">
+        <f>P7/M7</f>
+        <v>0.49673202614379086</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="5">
+        <v>240</v>
+      </c>
+      <c r="C8" s="5">
+        <v>132</v>
+      </c>
+      <c r="D8" s="5">
+        <f>B8*C8</f>
+        <v>31680</v>
+      </c>
+      <c r="E8" s="5">
+        <f>D8/$D$9*$E$9</f>
+        <v>20.93426226565942</v>
+      </c>
+      <c r="F8">
+        <f>B8*SQRT($E$7/$D$7)</f>
+        <v>6.1694647278732102</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>3.3932056003302655</v>
+      </c>
+      <c r="H8" s="6">
+        <f>H18</f>
+        <v>201326592</v>
+      </c>
+      <c r="I8" s="6">
+        <f t="shared" si="2"/>
+        <v>0.10398160549829116</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" ref="J8" si="3">SQRT(I8)</f>
+        <v>0.32246178920655261</v>
+      </c>
+      <c r="K8" s="5">
+        <f>SQRT(G18)*J8</f>
+        <v>0.78986684510096183</v>
+      </c>
+      <c r="L8" s="5">
+        <v>2</v>
+      </c>
+      <c r="M8" s="5">
+        <v>112.5</v>
+      </c>
+      <c r="N8" s="5">
+        <v>95</v>
+      </c>
+      <c r="O8" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="P8">
+        <f t="shared" ref="P8:P15" si="4">N8/O8</f>
+        <v>55.882352941176471</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" ref="Q8:Q15" si="5">P8/M8</f>
+        <v>0.49673202614379086</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="4">
+        <v>334</v>
+      </c>
+      <c r="C9" s="4">
+        <v>367</v>
+      </c>
+      <c r="D9" s="4">
+        <f>B9*C9</f>
+        <v>122578</v>
+      </c>
+      <c r="E9" s="4">
+        <v>81</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9:F11" si="6">B9*SQRT($E$7/$D$7)</f>
+        <v>8.5858384129568837</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>9.4341398130394492</v>
+      </c>
+      <c r="H9" s="9">
+        <v>382000000</v>
+      </c>
+      <c r="I9" s="9">
+        <f t="shared" si="2"/>
+        <v>0.21204188481675393</v>
+      </c>
+      <c r="J9" s="4">
+        <f>SQRT(I9)</f>
+        <v>0.4604800590869858</v>
+      </c>
+      <c r="K9" s="4">
+        <f>2*J9</f>
+        <v>0.92096011817397161</v>
+      </c>
+      <c r="L9" s="5">
+        <v>3</v>
+      </c>
+      <c r="M9" s="5">
+        <v>112.5</v>
+      </c>
+      <c r="N9" s="5">
+        <v>95</v>
+      </c>
+      <c r="O9" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="4"/>
+        <v>55.882352941176471</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="5"/>
+        <v>0.49673202614379086</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="5">
+        <v>52</v>
+      </c>
+      <c r="C10" s="5">
+        <v>368</v>
+      </c>
+      <c r="D10" s="5">
+        <f t="shared" ref="D10:D11" si="7">B10*C10</f>
+        <v>19136</v>
+      </c>
+      <c r="E10" s="5">
+        <f>D10/$D$9*$E$9</f>
+        <v>12.645140237236697</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="6"/>
+        <v>1.3367173577058622</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>9.4598459160722559</v>
+      </c>
+      <c r="H10" s="6">
+        <f>E10/$E$9*$H$9</f>
+        <v>59635105.810178012</v>
+      </c>
+      <c r="I10" s="6">
+        <f t="shared" si="2"/>
+        <v>0.2120418848167539</v>
+      </c>
+      <c r="J10" s="5">
+        <f t="shared" ref="J10:J15" si="8">SQRT(I10)</f>
+        <v>0.46048005908698575</v>
+      </c>
+      <c r="K10" s="5">
+        <f t="shared" ref="K10:K15" si="9">2*J10</f>
+        <v>0.9209601181739715</v>
+      </c>
+      <c r="L10" s="5">
+        <v>4</v>
+      </c>
+      <c r="M10" s="5">
+        <v>168.8</v>
+      </c>
+      <c r="N10" s="5">
+        <v>151</v>
+      </c>
+      <c r="O10" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="4"/>
+        <v>83.888888888888886</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="5"/>
+        <v>0.49697209057398628</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="5">
+        <v>32</v>
+      </c>
+      <c r="C11" s="5">
+        <v>368</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" si="7"/>
+        <v>11776</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" ref="E11:E12" si="10">D11/$D$9*$E$9</f>
+        <v>7.7816247613764302</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="6"/>
+        <v>0.82259529704976131</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>9.4598459160722559</v>
+      </c>
+      <c r="H11" s="6">
+        <f>E11/$E$9*$H$9</f>
+        <v>36698526.652417243</v>
+      </c>
+      <c r="I11" s="6">
+        <f t="shared" si="2"/>
+        <v>0.21204188481675393</v>
+      </c>
+      <c r="J11" s="5">
+        <f t="shared" si="8"/>
+        <v>0.4604800590869858</v>
+      </c>
+      <c r="K11" s="5">
+        <f t="shared" si="9"/>
+        <v>0.92096011817397161</v>
+      </c>
+      <c r="L11" s="5">
+        <v>5</v>
+      </c>
+      <c r="M11" s="5">
+        <v>225</v>
+      </c>
+      <c r="N11" s="5">
+        <v>204</v>
+      </c>
+      <c r="O11" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="4"/>
+        <v>113.33333333333333</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="5"/>
+        <v>0.50370370370370365</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5">
+        <f>D10+D11</f>
+        <v>30912</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="10"/>
+        <v>20.426764998613127</v>
+      </c>
+      <c r="H12" s="6">
+        <f>E12/$E$9*$H$9</f>
+        <v>96333632.462595239</v>
+      </c>
+      <c r="I12" s="6">
+        <f t="shared" si="2"/>
+        <v>0.21204188481675393</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" si="8"/>
+        <v>0.4604800590869858</v>
+      </c>
+      <c r="K12" s="5">
+        <f t="shared" si="9"/>
+        <v>0.92096011817397161</v>
+      </c>
+      <c r="L12" s="5">
+        <v>6</v>
+      </c>
+      <c r="M12" s="5">
+        <v>337.6</v>
+      </c>
+      <c r="N12" s="5">
+        <v>303</v>
+      </c>
+      <c r="O12" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="4"/>
+        <v>168.33333333333334</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="5"/>
+        <v>0.4986176935229068</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="5">
+        <v>379</v>
+      </c>
+      <c r="C13" s="5">
+        <v>512</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" ref="D13" si="11">D11+D12</f>
+        <v>42688</v>
+      </c>
+      <c r="E13">
+        <v>114</v>
+      </c>
+      <c r="F13">
+        <f>B13*SQRT($E$13/$D$13)</f>
+        <v>19.585683479937884</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ref="G13:G15" si="12">C13*SQRT($E$13/$D$13)</f>
+        <v>26.458759740707645</v>
+      </c>
+      <c r="H13" s="2">
+        <v>177000000</v>
+      </c>
+      <c r="I13" s="6">
+        <f t="shared" si="2"/>
+        <v>0.64406779661016944</v>
+      </c>
+      <c r="J13" s="5">
+        <f t="shared" si="8"/>
+        <v>0.8025383458814721</v>
+      </c>
+      <c r="K13" s="5">
+        <f t="shared" si="9"/>
+        <v>1.6050766917629442</v>
+      </c>
+      <c r="L13" s="5">
+        <v>7</v>
+      </c>
+      <c r="M13" s="5">
+        <v>450.1</v>
+      </c>
+      <c r="N13" s="5">
+        <v>388</v>
+      </c>
+      <c r="O13" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="4"/>
+        <v>228.23529411764707</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="5"/>
+        <v>0.50707685873727404</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14">
+        <f>F30</f>
+        <v>80429</v>
+      </c>
+      <c r="E14">
+        <f>D14/D13*E13</f>
+        <v>214.7888399550225</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14:F15" si="13">B14*SQRT($E$13/$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <f>E14/E13*H13</f>
+        <v>333487935.7196402</v>
+      </c>
+      <c r="I14" s="6">
+        <f t="shared" si="2"/>
+        <v>0.64406779661016944</v>
+      </c>
+      <c r="J14" s="5">
+        <f t="shared" si="8"/>
+        <v>0.8025383458814721</v>
+      </c>
+      <c r="K14" s="5">
+        <f t="shared" si="9"/>
+        <v>1.6050766917629442</v>
+      </c>
+      <c r="L14" s="5">
+        <v>8</v>
+      </c>
+      <c r="M14" s="5">
+        <v>566.5</v>
+      </c>
+      <c r="N14" s="5">
+        <v>504</v>
+      </c>
+      <c r="O14" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="4"/>
+        <v>280</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="5"/>
+        <v>0.49426301853486321</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="5">
+        <v>189</v>
+      </c>
+      <c r="C15" s="5">
+        <v>176</v>
+      </c>
+      <c r="D15">
+        <f>C15*B15</f>
+        <v>33264</v>
+      </c>
+      <c r="E15">
+        <f>E13/D13*D15</f>
+        <v>88.832833583208398</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="13"/>
+        <v>9.7670031074096588</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="12"/>
+        <v>9.0951986608682525</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" ref="H15" si="14">E15/E14*H14</f>
+        <v>137924662.66866568</v>
+      </c>
+      <c r="I15" s="6">
+        <f t="shared" si="2"/>
+        <v>0.64406779661016944</v>
+      </c>
+      <c r="J15" s="5">
+        <f t="shared" si="8"/>
+        <v>0.8025383458814721</v>
+      </c>
+      <c r="K15" s="5">
+        <f t="shared" si="9"/>
+        <v>1.6050766917629442</v>
+      </c>
+      <c r="L15" s="5">
+        <v>9</v>
+      </c>
+      <c r="M15" s="5">
+        <v>19400</v>
+      </c>
+      <c r="N15" s="5">
+        <v>8000</v>
+      </c>
+      <c r="O15" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="4"/>
+        <v>5333.333333333333</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="5"/>
+        <v>0.274914089347079</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D16" s="1"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="L16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M16" s="6">
+        <v>145900</v>
+      </c>
+      <c r="N16" s="6">
+        <v>25500</v>
+      </c>
+      <c r="O16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2">
+        <f>H9</f>
+        <v>382000000</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18">
+        <f>P3</f>
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <f>E18*POWER(2,20)*8</f>
+        <v>33554432</v>
+      </c>
+      <c r="G18">
+        <v>6</v>
+      </c>
+      <c r="H18">
+        <f>G18*F18</f>
+        <v>201326592</v>
+      </c>
+      <c r="I18">
+        <f>E8/F18*1000000</f>
+        <v>0.62388963298974698</v>
+      </c>
+      <c r="J18">
+        <f>SQRT(I18)</f>
+        <v>0.78986684510096195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <f>H18</f>
+        <v>201326592</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="G19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="2">
+        <f>B18-B19</f>
+        <v>180673408</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="2">
+        <f>H12</f>
+        <v>96333632.462595239</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <f>(B20-B21)/Q3</f>
+        <v>42169887.76870238</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>59</v>
+      </c>
+      <c r="F25">
+        <f>D25*E25</f>
+        <v>1829</v>
+      </c>
+      <c r="G25">
+        <f>D25*SQRT($E$13/$D$13)</f>
+        <v>1.6019952186756583</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ref="H25:H29" si="15">E25*SQRT($E$13/$D$13)</f>
+        <v>3.0489586419956076</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26">
+        <v>270</v>
+      </c>
+      <c r="E26">
+        <v>213</v>
+      </c>
+      <c r="F26">
+        <f t="shared" ref="F26:F29" si="16">D26*E26</f>
+        <v>57510</v>
+      </c>
+      <c r="G26">
+        <f t="shared" ref="G26:G29" si="17">D26*SQRT($E$13/$D$13)</f>
+        <v>13.952861582013798</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="15"/>
+        <v>11.007257470255329</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27">
+        <v>29</v>
+      </c>
+      <c r="E27">
+        <v>44</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="16"/>
+        <v>1276</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="17"/>
+        <v>1.4986406884385191</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="15"/>
+        <v>2.2737996652170631</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28">
+        <v>103</v>
+      </c>
+      <c r="E28">
+        <v>179</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="16"/>
+        <v>18437</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="17"/>
+        <v>5.3227583072126707</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="15"/>
+        <v>9.2502304562239619</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29">
+        <v>51</v>
+      </c>
+      <c r="E29">
+        <v>27</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="16"/>
+        <v>1377</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="17"/>
+        <v>2.6355405210470506</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="15"/>
+        <v>1.3952861582013798</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F30" s="1">
+        <f>SUM(F25:F29)</f>
+        <v>80429</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L3" s="7">
+        <v>130</v>
+      </c>
+      <c r="M3" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="N3" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="O3" s="5">
+        <v>3.33</v>
+      </c>
+      <c r="P3" s="5">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="5">
+        <v>86</v>
+      </c>
+      <c r="C7" s="5">
+        <v>168</v>
+      </c>
+      <c r="D7" s="5">
+        <f>B7*C7</f>
+        <v>14448</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" ref="E7" si="0">D7/$D$9*$E$9</f>
+        <v>19.54819863680623</v>
+      </c>
+      <c r="F7">
+        <f>B7*SQRT($E$7/$D$7)</f>
+        <v>3.1633551758917751</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7:G13" si="1">C7*SQRT($E$7/$D$7)</f>
+        <v>6.1795775529048633</v>
+      </c>
+      <c r="H7" s="6">
+        <f>B21</f>
+        <v>77719013.428379491</v>
+      </c>
+      <c r="I7" s="6">
+        <f t="shared" ref="I7:I13" si="2">E7/H7*1000000</f>
+        <v>0.25152401934206886</v>
+      </c>
+      <c r="J7" s="5">
+        <f>SQRT(I7)</f>
+        <v>0.50152170375973648</v>
+      </c>
+      <c r="K7" s="5">
+        <f>2*J7</f>
+        <v>1.003043407519473</v>
+      </c>
+      <c r="L7" s="5">
+        <v>1</v>
+      </c>
+      <c r="M7" s="5">
+        <v>112.5</v>
+      </c>
+      <c r="N7" s="5">
+        <v>95</v>
+      </c>
+      <c r="O7" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="P7">
+        <f>N7/O7</f>
+        <v>55.882352941176471</v>
+      </c>
+      <c r="Q7">
+        <f>P7/M7</f>
+        <v>0.49673202614379086</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="5">
+        <v>256</v>
+      </c>
+      <c r="C8" s="5">
+        <v>94</v>
+      </c>
+      <c r="D8" s="5">
+        <f>B8*C8</f>
+        <v>24064</v>
+      </c>
+      <c r="E8" s="5">
+        <f>D8/$D$9*$E$9</f>
+        <v>32.558683000837846</v>
+      </c>
+      <c r="F8">
+        <f>B8*SQRT($E$7/$D$7)</f>
+        <v>9.4164991282359818</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>3.4576207736491495</v>
+      </c>
+      <c r="H8" s="6">
+        <f>H17/2</f>
+        <v>301989888</v>
+      </c>
+      <c r="I8" s="6">
+        <f t="shared" si="2"/>
+        <v>0.10781381858997162</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" ref="J8" si="3">SQRT(I8)</f>
+        <v>0.32835014632244586</v>
+      </c>
+      <c r="K8" s="5">
+        <f>SQRT(G17)*J8</f>
+        <v>0.80429031545818674</v>
+      </c>
+      <c r="L8" s="5">
+        <v>2</v>
+      </c>
+      <c r="M8" s="5">
+        <v>112.5</v>
+      </c>
+      <c r="N8" s="5">
+        <v>95</v>
+      </c>
+      <c r="O8" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="P8">
+        <f t="shared" ref="P8:P14" si="4">N8/O8</f>
+        <v>55.882352941176471</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" ref="Q8:Q14" si="5">P8/M8</f>
+        <v>0.49673202614379086</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="4">
+        <v>559</v>
+      </c>
+      <c r="C9" s="4">
+        <v>316</v>
+      </c>
+      <c r="D9" s="4">
+        <f>B9*C9</f>
+        <v>176644</v>
+      </c>
+      <c r="E9" s="4">
+        <v>239</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9:F13" si="6">B9*SQRT($E$7/$D$7)</f>
+        <v>20.561808643296537</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>11.623491111416291</v>
+      </c>
+      <c r="H9" s="9">
+        <v>382000000</v>
+      </c>
+      <c r="I9" s="9">
+        <f t="shared" si="2"/>
+        <v>0.62565445026178013</v>
+      </c>
+      <c r="J9" s="4">
+        <f>SQRT(I9)</f>
+        <v>0.7909832174337077</v>
+      </c>
+      <c r="K9" s="4">
+        <f>2*J9</f>
+        <v>1.5819664348674154</v>
+      </c>
+      <c r="L9" s="5">
+        <v>3</v>
+      </c>
+      <c r="M9" s="5">
+        <v>112.5</v>
+      </c>
+      <c r="N9" s="5">
+        <v>95</v>
+      </c>
+      <c r="O9" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="4"/>
+        <v>55.882352941176471</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="5"/>
+        <v>0.49673202614379086</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="5">
+        <v>27</v>
+      </c>
+      <c r="C10" s="5">
+        <v>198</v>
+      </c>
+      <c r="D10" s="5">
+        <f t="shared" ref="D10:D13" si="7">B10*C10</f>
+        <v>5346</v>
+      </c>
+      <c r="E10" s="5">
+        <f>D10/$D$9*$E$9</f>
+        <v>7.2331582165258936</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="6"/>
+        <v>0.99314639243113867</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>7.283073544495017</v>
+      </c>
+      <c r="H10" s="6">
+        <f>E10/$E$9*$H$9</f>
+        <v>11560947.442313353</v>
+      </c>
+      <c r="I10" s="6">
+        <f t="shared" si="2"/>
+        <v>0.62565445026178013</v>
+      </c>
+      <c r="J10" s="5">
+        <f t="shared" ref="J10:J13" si="8">SQRT(I10)</f>
+        <v>0.7909832174337077</v>
+      </c>
+      <c r="K10" s="5">
+        <f t="shared" ref="K10:K13" si="9">2*J10</f>
+        <v>1.5819664348674154</v>
+      </c>
+      <c r="L10" s="5">
+        <v>4</v>
+      </c>
+      <c r="M10" s="5">
+        <v>168.8</v>
+      </c>
+      <c r="N10" s="5">
+        <v>151</v>
+      </c>
+      <c r="O10" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="4"/>
+        <v>83.888888888888886</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="5"/>
+        <v>0.49697209057398628</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" s="5">
+        <v>27</v>
+      </c>
+      <c r="C11" s="5">
+        <v>166</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" si="7"/>
+        <v>4482</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" ref="E11:E13" si="10">D11/$D$9*$E$9</f>
+        <v>6.0641629492085771</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="6"/>
+        <v>0.99314639243113867</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>6.106011153465519</v>
+      </c>
+      <c r="H11" s="6">
+        <f>E11/$E$9*$H$9</f>
+        <v>9692511.492040487</v>
+      </c>
+      <c r="I11" s="6">
+        <f t="shared" si="2"/>
+        <v>0.62565445026178013</v>
+      </c>
+      <c r="J11" s="5">
+        <f t="shared" si="8"/>
+        <v>0.7909832174337077</v>
+      </c>
+      <c r="K11" s="5">
+        <f t="shared" si="9"/>
+        <v>1.5819664348674154</v>
+      </c>
+      <c r="L11" s="5">
+        <v>5</v>
+      </c>
+      <c r="M11" s="5">
+        <v>225</v>
+      </c>
+      <c r="N11" s="5">
+        <v>204</v>
+      </c>
+      <c r="O11" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="4"/>
+        <v>113.33333333333333</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="5"/>
+        <v>0.50370370370370365</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="5">
+        <v>448</v>
+      </c>
+      <c r="C12" s="5">
+        <v>57</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" si="7"/>
+        <v>25536</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="10"/>
+        <v>34.550304567378454</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="6"/>
+        <v>16.478873474412968</v>
+      </c>
+      <c r="G12">
+        <f>C12*SQRT($E$12/$D$12)</f>
+        <v>2.0966423840212927</v>
+      </c>
+      <c r="H12" s="6">
+        <f t="shared" ref="H12:H13" si="11">E12/$E$9*$H$9</f>
+        <v>55222662.530286901</v>
+      </c>
+      <c r="I12" s="6">
+        <f t="shared" si="2"/>
+        <v>0.62565445026178013</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" si="8"/>
+        <v>0.7909832174337077</v>
+      </c>
+      <c r="K12" s="5">
+        <f t="shared" si="9"/>
+        <v>1.5819664348674154</v>
+      </c>
+      <c r="L12" s="5">
+        <v>7</v>
+      </c>
+      <c r="M12" s="5">
+        <v>450.1</v>
+      </c>
+      <c r="N12" s="5">
+        <v>388</v>
+      </c>
+      <c r="O12" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="4"/>
+        <v>228.23529411764707</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="5"/>
+        <v>0.50707685873727404</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="5">
+        <v>41</v>
+      </c>
+      <c r="C13" s="5">
+        <v>262</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" si="7"/>
+        <v>10742</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="10"/>
+        <v>14.533966622132651</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="6"/>
+        <v>1.5081111885065439</v>
+      </c>
+      <c r="G13">
+        <f>C13*SQRT($E$12/$D$12)</f>
+        <v>9.637198326554012</v>
+      </c>
+      <c r="H13" s="6">
+        <f t="shared" si="11"/>
+        <v>23230021.965082314</v>
+      </c>
+      <c r="I13" s="6">
+        <f t="shared" si="2"/>
+        <v>0.62565445026178002</v>
+      </c>
+      <c r="J13" s="5">
+        <f t="shared" si="8"/>
+        <v>0.79098321743370759</v>
+      </c>
+      <c r="K13" s="5">
+        <f t="shared" si="9"/>
+        <v>1.5819664348674152</v>
+      </c>
+      <c r="L13" s="5">
+        <v>8</v>
+      </c>
+      <c r="M13" s="5">
+        <v>566.5</v>
+      </c>
+      <c r="N13" s="5">
+        <v>504</v>
+      </c>
+      <c r="O13" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="4"/>
+        <v>280</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="5"/>
+        <v>0.49426301853486321</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5">
+        <v>9</v>
+      </c>
+      <c r="M14" s="5">
+        <v>19400</v>
+      </c>
+      <c r="N14" s="5">
+        <v>8000</v>
+      </c>
+      <c r="O14" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="4"/>
+        <v>5333.333333333333</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="5"/>
+        <v>0.274914089347079</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="L15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M15" s="6">
+        <v>145900</v>
+      </c>
+      <c r="N15" s="6">
+        <v>25500</v>
+      </c>
+      <c r="O15" s="5"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1170000000</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17">
+        <f>P3</f>
+        <v>12</v>
+      </c>
+      <c r="F17">
+        <f>E17*POWER(2,20)*8</f>
+        <v>100663296</v>
+      </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <f>G17*F17</f>
+        <v>603979776</v>
+      </c>
+      <c r="I17">
+        <f>E8/F17*1000000</f>
+        <v>0.32344145576991484</v>
+      </c>
+      <c r="J17">
+        <f>SQRT(I17)</f>
+        <v>0.56871913610315139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <f>H17</f>
+        <v>603979776</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="G18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2">
+        <f>B17-B18</f>
+        <v>566020224</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="2">
+        <f>SUM(H10:H13)</f>
+        <v>99706143.429723054</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <f>(B19-B20)/Q3</f>
+        <v>77719013.428379491</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q24"/>
   <sheetViews>
@@ -5508,7 +7831,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R29"/>
   <sheetViews>
@@ -6102,646 +8425,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>169</v>
-      </c>
-      <c r="C2">
-        <v>287</v>
-      </c>
-      <c r="D2">
-        <f>B2*C2</f>
-        <v>48503</v>
-      </c>
-      <c r="E2">
-        <f>D2/$D$4*$E$4</f>
-        <v>18.546941608010311</v>
-      </c>
-      <c r="F2" s="2">
-        <f>E2/$E$4*$F$4</f>
-        <v>85436143.055417866</v>
-      </c>
-      <c r="G2" s="2">
-        <f>E2/F2*1000000</f>
-        <v>0.21708542713567841</v>
-      </c>
-      <c r="H2">
-        <f>SQRT(G2)</f>
-        <v>0.46592427188941166</v>
-      </c>
-      <c r="I2">
-        <f>2*H2</f>
-        <v>0.93184854377882331</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>228</v>
-      </c>
-      <c r="C3">
-        <v>325</v>
-      </c>
-      <c r="D3">
-        <f>B3*C3</f>
-        <v>74100</v>
-      </c>
-      <c r="F3">
-        <f>B8</f>
-        <v>1006632960</v>
-      </c>
-      <c r="G3" s="2">
-        <f>E3/F3*1000000</f>
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <f>SQRT(G3)</f>
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <f>2*H3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1078</v>
-      </c>
-      <c r="C4" s="1">
-        <v>524</v>
-      </c>
-      <c r="D4">
-        <f>B4*C4</f>
-        <v>564872</v>
-      </c>
-      <c r="E4">
-        <v>216</v>
-      </c>
-      <c r="F4" s="2">
-        <v>995000000</v>
-      </c>
-      <c r="G4" s="2">
-        <f>E4/F4*1000000</f>
-        <v>0.21708542713567841</v>
-      </c>
-      <c r="H4">
-        <f>SQRT(G4)</f>
-        <v>0.46592427188941166</v>
-      </c>
-      <c r="I4">
-        <f>2*H4</f>
-        <v>0.93184854377882331</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="E6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2">
-        <v>2270000000</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7">
-        <v>20</v>
-      </c>
-      <c r="F7">
-        <f>E7*POWER(2,20)*8</f>
-        <v>167772160</v>
-      </c>
-      <c r="G7">
-        <v>6</v>
-      </c>
-      <c r="H7">
-        <f>G7*F7</f>
-        <v>1006632960</v>
-      </c>
-      <c r="I7">
-        <f>E3/H7*1000000</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <f>H7</f>
-        <v>1006632960</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8">
-        <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2">
-        <f>B7-B8</f>
-        <v>1263367040</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L13" s="5">
-        <v>112.5</v>
-      </c>
-      <c r="M13" s="5">
-        <v>112.5</v>
-      </c>
-      <c r="N13" s="5">
-        <v>112.5</v>
-      </c>
-      <c r="O13" s="5">
-        <v>168.8</v>
-      </c>
-      <c r="P13" s="5">
-        <v>225</v>
-      </c>
-      <c r="Q13" s="5">
-        <v>337.6</v>
-      </c>
-      <c r="R13" s="5">
-        <v>450.1</v>
-      </c>
-      <c r="S13" s="5">
-        <v>566.5</v>
-      </c>
-      <c r="T13" s="5">
-        <v>19400</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="D14">
-        <v>0.1125</v>
-      </c>
-      <c r="F14" s="5">
-        <v>1</v>
-      </c>
-      <c r="G14" s="5">
-        <v>112.5</v>
-      </c>
-      <c r="H14">
-        <v>112.5</v>
-      </c>
-      <c r="I14">
-        <v>112.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="3">
-        <v>0.1993</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="5">
-        <v>2</v>
-      </c>
-      <c r="G15" s="5">
-        <v>112.5</v>
-      </c>
-      <c r="H15">
-        <v>112.5</v>
-      </c>
-      <c r="I15">
-        <v>112.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="D16">
-        <v>0.42</v>
-      </c>
-      <c r="F16" s="5">
-        <v>3</v>
-      </c>
-      <c r="G16" s="5">
-        <v>112.5</v>
-      </c>
-      <c r="H16">
-        <v>199.3</v>
-      </c>
-      <c r="I16">
-        <v>131.49469999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D17">
-        <v>0.71819999999999995</v>
-      </c>
-      <c r="F17" s="5">
-        <v>4</v>
-      </c>
-      <c r="G17" s="5">
-        <v>168.8</v>
-      </c>
-      <c r="H17">
-        <v>199.3</v>
-      </c>
-      <c r="I17">
-        <v>247.32849999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F18" s="5">
-        <v>5</v>
-      </c>
-      <c r="G18" s="5">
-        <v>225</v>
-      </c>
-      <c r="H18">
-        <v>420</v>
-      </c>
-      <c r="I18">
-        <v>374.14409999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F19" s="5">
-        <v>6</v>
-      </c>
-      <c r="G19" s="5">
-        <v>337.6</v>
-      </c>
-      <c r="H19">
-        <v>420</v>
-      </c>
-      <c r="I19">
-        <v>540.39850000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F20" s="5">
-        <v>7</v>
-      </c>
-      <c r="G20" s="5">
-        <v>450.1</v>
-      </c>
-      <c r="H20">
-        <v>718.2</v>
-      </c>
-      <c r="I20">
-        <v>718.20759999999996</v>
-      </c>
-    </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F21" s="5">
-        <v>8</v>
-      </c>
-      <c r="G21" s="5">
-        <v>566.5</v>
-      </c>
-      <c r="H21">
-        <v>718.2</v>
-      </c>
-    </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F22" s="5">
-        <v>9</v>
-      </c>
-      <c r="G22" s="5">
-        <v>19400</v>
-      </c>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="F23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G23" s="6">
-        <v>145900</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>79</v>
-      </c>
-      <c r="C3">
-        <v>144</v>
-      </c>
-      <c r="D3">
-        <f>B3*C3</f>
-        <v>11376</v>
-      </c>
-      <c r="E3">
-        <f>D3*E5/D5</f>
-        <v>11.516760404949382</v>
-      </c>
-      <c r="F3" s="2">
-        <f>F5*E3/E5</f>
-        <v>95058974.771010771</v>
-      </c>
-      <c r="G3" s="2">
-        <f>E3/F3</f>
-        <v>1.2115384615384617E-7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3">
-        <v>635</v>
-      </c>
-      <c r="C5" s="3">
-        <v>539</v>
-      </c>
-      <c r="D5" s="3">
-        <f>B5*C5</f>
-        <v>342265</v>
-      </c>
-      <c r="E5">
-        <v>346.5</v>
-      </c>
-      <c r="F5" s="2">
-        <v>2860000000</v>
-      </c>
-      <c r="G5" s="2">
-        <f>E5/F5*1000000</f>
-        <v>0.12115384615384614</v>
-      </c>
-      <c r="H5">
-        <f>SQRT(G5)</f>
-        <v>0.34807161066919279</v>
-      </c>
-      <c r="I5">
-        <f>2*H5</f>
-        <v>0.69614322133838558</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <v>90</v>
-      </c>
-      <c r="C9" s="5">
-        <v>90</v>
-      </c>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>80</v>
-      </c>
-      <c r="C10" s="5">
-        <v>90</v>
-      </c>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>3</v>
-      </c>
-      <c r="B11">
-        <v>80</v>
-      </c>
-      <c r="C11" s="5">
-        <v>90</v>
-      </c>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>4</v>
-      </c>
-      <c r="B12">
-        <v>112</v>
-      </c>
-      <c r="C12" s="5">
-        <v>115.836</v>
-      </c>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>5</v>
-      </c>
-      <c r="B13">
-        <v>160</v>
-      </c>
-      <c r="C13" s="5">
-        <v>210.5411</v>
-      </c>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>6</v>
-      </c>
-      <c r="B14">
-        <v>240</v>
-      </c>
-      <c r="C14" s="5">
-        <v>322.54140000000001</v>
-      </c>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>7</v>
-      </c>
-      <c r="B15">
-        <v>320</v>
-      </c>
-      <c r="C15" s="5">
-        <v>493.471</v>
-      </c>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>8</v>
-      </c>
-      <c r="B16">
-        <v>360</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>9</v>
-      </c>
-      <c r="B17">
-        <v>14000</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>